<commit_message>
fjern cph link der er dødt
</commit_message>
<xml_diff>
--- a/Danske aktiekurser.xlsx
+++ b/Danske aktiekurser.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1021" uniqueCount="1021">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1022" uniqueCount="1022">
   <si>
     <t xml:space="preserve"/>
   </si>
@@ -3075,6 +3075,9 @@
   </si>
   <si>
     <t xml:space="preserve">2022-01-31</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2022-02-01</t>
   </si>
 </sst>
 </file>
@@ -3447,10 +3450,10 @@
         <v>5</v>
       </c>
       <c r="B4" t="n">
-        <v>190.51384</v>
+        <v>190.513824</v>
       </c>
       <c r="C4" t="n">
-        <v>192.351486</v>
+        <v>192.351501</v>
       </c>
     </row>
     <row r="5">
@@ -3458,10 +3461,10 @@
         <v>6</v>
       </c>
       <c r="B5" t="n">
-        <v>190.748581</v>
+        <v>190.74855</v>
       </c>
       <c r="C5" t="n">
-        <v>192.046173</v>
+        <v>192.046188</v>
       </c>
     </row>
     <row r="6">
@@ -3472,7 +3475,7 @@
         <v>191.843918</v>
       </c>
       <c r="C6" t="n">
-        <v>191.74086</v>
+        <v>191.740845</v>
       </c>
     </row>
     <row r="7">
@@ -3483,7 +3486,7 @@
         <v>190.357361</v>
       </c>
       <c r="C7" t="n">
-        <v>191.588181</v>
+        <v>191.588196</v>
       </c>
     </row>
     <row r="8">
@@ -3491,10 +3494,10 @@
         <v>9</v>
       </c>
       <c r="B8" t="n">
-        <v>194.34758</v>
+        <v>194.347595</v>
       </c>
       <c r="C8" t="n">
-        <v>195.404694</v>
+        <v>195.404709</v>
       </c>
     </row>
     <row r="9">
@@ -3524,7 +3527,7 @@
         <v>12</v>
       </c>
       <c r="B11" t="n">
-        <v>196.303589</v>
+        <v>196.303574</v>
       </c>
       <c r="C11" t="n">
         <v>193.572784</v>
@@ -3535,10 +3538,10 @@
         <v>13</v>
       </c>
       <c r="B12" t="n">
-        <v>195.521179</v>
+        <v>195.521194</v>
       </c>
       <c r="C12" t="n">
-        <v>192.504166</v>
+        <v>192.50415</v>
       </c>
     </row>
     <row r="13">
@@ -3546,10 +3549,10 @@
         <v>14</v>
       </c>
       <c r="B13" t="n">
-        <v>195.990631</v>
+        <v>195.990616</v>
       </c>
       <c r="C13" t="n">
-        <v>191.435562</v>
+        <v>191.435547</v>
       </c>
     </row>
     <row r="14">
@@ -3557,10 +3560,10 @@
         <v>15</v>
       </c>
       <c r="B14" t="n">
-        <v>191.452713</v>
+        <v>191.452728</v>
       </c>
       <c r="C14" t="n">
-        <v>191.588181</v>
+        <v>191.588196</v>
       </c>
     </row>
     <row r="15">
@@ -3582,7 +3585,7 @@
         <v>193.330475</v>
       </c>
       <c r="C16" t="n">
-        <v>193.114807</v>
+        <v>193.114792</v>
       </c>
     </row>
     <row r="17">
@@ -3590,10 +3593,10 @@
         <v>18</v>
       </c>
       <c r="B17" t="n">
-        <v>192.078659</v>
+        <v>192.078644</v>
       </c>
       <c r="C17" t="n">
-        <v>191.435562</v>
+        <v>191.435547</v>
       </c>
     </row>
     <row r="18">
@@ -3601,7 +3604,7 @@
         <v>19</v>
       </c>
       <c r="B18" t="n">
-        <v>192.078659</v>
+        <v>192.078644</v>
       </c>
       <c r="C18" t="n">
         <v>190.214249</v>
@@ -3612,10 +3615,10 @@
         <v>20</v>
       </c>
       <c r="B19" t="n">
-        <v>186.680084</v>
+        <v>186.680099</v>
       </c>
       <c r="C19" t="n">
-        <v>185.634445</v>
+        <v>185.63446</v>
       </c>
     </row>
     <row r="20">
@@ -3623,7 +3626,7 @@
         <v>21</v>
       </c>
       <c r="B20" t="n">
-        <v>189.966171</v>
+        <v>189.966156</v>
       </c>
       <c r="C20" t="n">
         <v>187.466385</v>
@@ -3645,10 +3648,10 @@
         <v>23</v>
       </c>
       <c r="B22" t="n">
-        <v>189.966171</v>
+        <v>189.966156</v>
       </c>
       <c r="C22" t="n">
-        <v>185.787109</v>
+        <v>185.787094</v>
       </c>
     </row>
     <row r="23">
@@ -3656,7 +3659,7 @@
         <v>24</v>
       </c>
       <c r="B23" t="n">
-        <v>190.51384</v>
+        <v>190.513824</v>
       </c>
       <c r="C23" t="n">
         <v>187.008408</v>
@@ -3711,10 +3714,10 @@
         <v>29</v>
       </c>
       <c r="B28" t="n">
-        <v>189.261993</v>
+        <v>189.262009</v>
       </c>
       <c r="C28" t="n">
-        <v>188.687653</v>
+        <v>188.687683</v>
       </c>
     </row>
     <row r="29">
@@ -3722,7 +3725,7 @@
         <v>30</v>
       </c>
       <c r="B29" t="n">
-        <v>188.557846</v>
+        <v>188.557861</v>
       </c>
       <c r="C29" t="n">
         <v>187.161057</v>
@@ -3736,7 +3739,7 @@
         <v>188.244904</v>
       </c>
       <c r="C30" t="n">
-        <v>185.787109</v>
+        <v>185.787094</v>
       </c>
     </row>
     <row r="31">
@@ -3744,10 +3747,10 @@
         <v>32</v>
       </c>
       <c r="B31" t="n">
-        <v>189.966171</v>
+        <v>189.966156</v>
       </c>
       <c r="C31" t="n">
-        <v>188.687653</v>
+        <v>188.687683</v>
       </c>
     </row>
     <row r="32">
@@ -3777,10 +3780,10 @@
         <v>35</v>
       </c>
       <c r="B34" t="n">
-        <v>192.31337</v>
+        <v>192.313354</v>
       </c>
       <c r="C34" t="n">
-        <v>193.420105</v>
+        <v>193.42012</v>
       </c>
     </row>
     <row r="35">
@@ -3788,10 +3791,10 @@
         <v>36</v>
       </c>
       <c r="B35" t="n">
-        <v>194.660553</v>
+        <v>194.660568</v>
       </c>
       <c r="C35" t="n">
-        <v>196.625992</v>
+        <v>196.625977</v>
       </c>
     </row>
     <row r="36">
@@ -3802,7 +3805,7 @@
         <v>194.895279</v>
       </c>
       <c r="C36" t="n">
-        <v>196.167984</v>
+        <v>196.168015</v>
       </c>
     </row>
     <row r="37">
@@ -3810,7 +3813,7 @@
         <v>38</v>
       </c>
       <c r="B37" t="n">
-        <v>191.687424</v>
+        <v>191.687439</v>
       </c>
       <c r="C37" t="n">
         <v>185.481796</v>
@@ -3821,7 +3824,7 @@
         <v>39</v>
       </c>
       <c r="B38" t="n">
-        <v>192.861038</v>
+        <v>192.861023</v>
       </c>
       <c r="C38" t="n">
         <v>182.428604</v>
@@ -3832,10 +3835,10 @@
         <v>40</v>
       </c>
       <c r="B39" t="n">
-        <v>193.252243</v>
+        <v>193.252228</v>
       </c>
       <c r="C39" t="n">
-        <v>180.444016</v>
+        <v>180.444031</v>
       </c>
     </row>
     <row r="40">
@@ -3843,7 +3846,7 @@
         <v>41</v>
       </c>
       <c r="B40" t="n">
-        <v>194.504089</v>
+        <v>194.504074</v>
       </c>
       <c r="C40" t="n">
         <v>186.245102</v>
@@ -3868,7 +3871,7 @@
         <v>189.731445</v>
       </c>
       <c r="C42" t="n">
-        <v>183.19191</v>
+        <v>183.191895</v>
       </c>
     </row>
     <row r="43">
@@ -3876,10 +3879,10 @@
         <v>44</v>
       </c>
       <c r="B43" t="n">
-        <v>192.626328</v>
+        <v>192.626312</v>
       </c>
       <c r="C43" t="n">
-        <v>182.733917</v>
+        <v>182.733932</v>
       </c>
     </row>
     <row r="44">
@@ -3887,7 +3890,7 @@
         <v>45</v>
       </c>
       <c r="B44" t="n">
-        <v>190.748581</v>
+        <v>190.74855</v>
       </c>
       <c r="C44" t="n">
         <v>181.665298</v>
@@ -3901,7 +3904,7 @@
         <v>189.731445</v>
       </c>
       <c r="C45" t="n">
-        <v>177.696136</v>
+        <v>177.696152</v>
       </c>
     </row>
     <row r="46">
@@ -3923,7 +3926,7 @@
         <v>189.34024</v>
       </c>
       <c r="C47" t="n">
-        <v>180.749344</v>
+        <v>180.749359</v>
       </c>
     </row>
     <row r="48">
@@ -3934,7 +3937,7 @@
         <v>191.53096</v>
       </c>
       <c r="C48" t="n">
-        <v>180.749344</v>
+        <v>180.749359</v>
       </c>
     </row>
     <row r="49">
@@ -3953,7 +3956,7 @@
         <v>51</v>
       </c>
       <c r="B50" t="n">
-        <v>192.626328</v>
+        <v>192.626312</v>
       </c>
       <c r="C50" t="n">
         <v>180.902008</v>
@@ -3964,7 +3967,7 @@
         <v>52</v>
       </c>
       <c r="B51" t="n">
-        <v>193.095764</v>
+        <v>193.095749</v>
       </c>
       <c r="C51" t="n">
         <v>180.291351</v>
@@ -3975,7 +3978,7 @@
         <v>53</v>
       </c>
       <c r="B52" t="n">
-        <v>193.799911</v>
+        <v>193.799927</v>
       </c>
       <c r="C52" t="n">
         <v>183.344559</v>
@@ -4000,7 +4003,7 @@
         <v>191.061523</v>
       </c>
       <c r="C54" t="n">
-        <v>183.113083</v>
+        <v>183.113098</v>
       </c>
     </row>
     <row r="55">
@@ -4099,7 +4102,7 @@
         <v>183.882431</v>
       </c>
       <c r="C63" t="n">
-        <v>178.14241</v>
+        <v>178.142426</v>
       </c>
     </row>
     <row r="64">
@@ -4110,7 +4113,7 @@
         <v>183.148224</v>
       </c>
       <c r="C64" t="n">
-        <v>178.463104</v>
+        <v>178.46312</v>
       </c>
     </row>
     <row r="65">
@@ -4143,7 +4146,7 @@
         <v>182.495575</v>
       </c>
       <c r="C67" t="n">
-        <v>178.14241</v>
+        <v>178.142426</v>
       </c>
     </row>
     <row r="68">
@@ -4151,10 +4154,10 @@
         <v>69</v>
       </c>
       <c r="B68" t="n">
-        <v>182.985062</v>
+        <v>182.985046</v>
       </c>
       <c r="C68" t="n">
-        <v>180.868301</v>
+        <v>180.868286</v>
       </c>
     </row>
     <row r="69">
@@ -4165,7 +4168,7 @@
         <v>183.39296</v>
       </c>
       <c r="C69" t="n">
-        <v>180.547592</v>
+        <v>180.547577</v>
       </c>
     </row>
     <row r="70">
@@ -4176,7 +4179,7 @@
         <v>179.477097</v>
       </c>
       <c r="C70" t="n">
-        <v>180.868301</v>
+        <v>180.868286</v>
       </c>
     </row>
     <row r="71">
@@ -4187,7 +4190,7 @@
         <v>180.619217</v>
       </c>
       <c r="C71" t="n">
-        <v>184.395844</v>
+        <v>184.395859</v>
       </c>
     </row>
     <row r="72">
@@ -4195,7 +4198,7 @@
         <v>73</v>
       </c>
       <c r="B72" t="n">
-        <v>180.211319</v>
+        <v>180.211304</v>
       </c>
       <c r="C72" t="n">
         <v>182.311371</v>
@@ -4217,7 +4220,7 @@
         <v>75</v>
       </c>
       <c r="B74" t="n">
-        <v>181.924515</v>
+        <v>181.9245</v>
       </c>
       <c r="C74" t="n">
         <v>184.075165</v>
@@ -4231,7 +4234,7 @@
         <v>183.637711</v>
       </c>
       <c r="C75" t="n">
-        <v>188.083771</v>
+        <v>188.083755</v>
       </c>
     </row>
     <row r="76">
@@ -4242,7 +4245,7 @@
         <v>182.577164</v>
       </c>
       <c r="C76" t="n">
-        <v>188.885483</v>
+        <v>188.885498</v>
       </c>
     </row>
     <row r="77">
@@ -4264,7 +4267,7 @@
         <v>183.229797</v>
       </c>
       <c r="C78" t="n">
-        <v>192.894073</v>
+        <v>192.894089</v>
       </c>
     </row>
     <row r="79">
@@ -4275,7 +4278,7 @@
         <v>184.127182</v>
       </c>
       <c r="C79" t="n">
-        <v>194.657867</v>
+        <v>194.657883</v>
       </c>
     </row>
     <row r="80">
@@ -4286,7 +4289,7 @@
         <v>178.498123</v>
       </c>
       <c r="C80" t="n">
-        <v>187.602722</v>
+        <v>187.602737</v>
       </c>
     </row>
     <row r="81">
@@ -4294,10 +4297,10 @@
         <v>82</v>
       </c>
       <c r="B81" t="n">
-        <v>179.069199</v>
+        <v>179.069183</v>
       </c>
       <c r="C81" t="n">
-        <v>186.319962</v>
+        <v>186.319977</v>
       </c>
     </row>
     <row r="82">
@@ -4305,7 +4308,7 @@
         <v>83</v>
       </c>
       <c r="B82" t="n">
-        <v>175.72438</v>
+        <v>175.724396</v>
       </c>
       <c r="C82" t="n">
         <v>183.433777</v>
@@ -4316,7 +4319,7 @@
         <v>84</v>
       </c>
       <c r="B83" t="n">
-        <v>177.763901</v>
+        <v>177.763885</v>
       </c>
       <c r="C83" t="n">
         <v>181.669998</v>
@@ -4330,7 +4333,7 @@
         <v>177.84549</v>
       </c>
       <c r="C84" t="n">
-        <v>184.716507</v>
+        <v>184.716522</v>
       </c>
     </row>
     <row r="85">
@@ -4349,7 +4352,7 @@
         <v>87</v>
       </c>
       <c r="B86" t="n">
-        <v>176.132294</v>
+        <v>176.132278</v>
       </c>
       <c r="C86" t="n">
         <v>183.433777</v>
@@ -4371,7 +4374,7 @@
         <v>89</v>
       </c>
       <c r="B88" t="n">
-        <v>176.784943</v>
+        <v>176.784927</v>
       </c>
       <c r="C88" t="n">
         <v>187.121704</v>
@@ -4393,7 +4396,7 @@
         <v>91</v>
       </c>
       <c r="B90" t="n">
-        <v>174.990173</v>
+        <v>174.990158</v>
       </c>
       <c r="C90" t="n">
         <v>186.640656</v>
@@ -4407,7 +4410,7 @@
         <v>175.561234</v>
       </c>
       <c r="C91" t="n">
-        <v>185.999283</v>
+        <v>185.999298</v>
       </c>
     </row>
     <row r="92">
@@ -4448,7 +4451,7 @@
         <v>96</v>
       </c>
       <c r="B95" t="n">
-        <v>176.132294</v>
+        <v>176.132278</v>
       </c>
       <c r="C95" t="n">
         <v>185.35791</v>
@@ -4459,10 +4462,10 @@
         <v>97</v>
       </c>
       <c r="B96" t="n">
-        <v>176.94809</v>
+        <v>176.948105</v>
       </c>
       <c r="C96" t="n">
-        <v>185.037216</v>
+        <v>185.037231</v>
       </c>
     </row>
     <row r="97">
@@ -4470,7 +4473,7 @@
         <v>98</v>
       </c>
       <c r="B97" t="n">
-        <v>173.603317</v>
+        <v>173.603302</v>
       </c>
       <c r="C97" t="n">
         <v>182.632065</v>
@@ -4495,7 +4498,7 @@
         <v>173.113815</v>
       </c>
       <c r="C99" t="n">
-        <v>181.028625</v>
+        <v>181.02861</v>
       </c>
     </row>
     <row r="100">
@@ -4514,7 +4517,7 @@
         <v>102</v>
       </c>
       <c r="B101" t="n">
-        <v>168.871628</v>
+        <v>168.871643</v>
       </c>
       <c r="C101" t="n">
         <v>175.737259</v>
@@ -4536,10 +4539,10 @@
         <v>104</v>
       </c>
       <c r="B103" t="n">
-        <v>176.295456</v>
+        <v>176.295471</v>
       </c>
       <c r="C103" t="n">
-        <v>178.30275</v>
+        <v>178.302765</v>
       </c>
     </row>
     <row r="104">
@@ -4558,10 +4561,10 @@
         <v>106</v>
       </c>
       <c r="B105" t="n">
-        <v>175.72438</v>
+        <v>175.724396</v>
       </c>
       <c r="C105" t="n">
-        <v>177.982086</v>
+        <v>177.982071</v>
       </c>
     </row>
     <row r="106">
@@ -4572,7 +4575,7 @@
         <v>175.561234</v>
       </c>
       <c r="C106" t="n">
-        <v>177.501038</v>
+        <v>177.501053</v>
       </c>
     </row>
     <row r="107">
@@ -4594,7 +4597,7 @@
         <v>177.84549</v>
       </c>
       <c r="C108" t="n">
-        <v>177.02002</v>
+        <v>177.020004</v>
       </c>
     </row>
     <row r="109">
@@ -4627,7 +4630,7 @@
         <v>178.742874</v>
       </c>
       <c r="C111" t="n">
-        <v>178.623459</v>
+        <v>178.623444</v>
       </c>
     </row>
     <row r="112">
@@ -4646,7 +4649,7 @@
         <v>114</v>
       </c>
       <c r="B113" t="n">
-        <v>173.929626</v>
+        <v>173.929611</v>
       </c>
       <c r="C113" t="n">
         <v>175.897598</v>
@@ -4668,7 +4671,7 @@
         <v>116</v>
       </c>
       <c r="B115" t="n">
-        <v>170.258499</v>
+        <v>170.258484</v>
       </c>
       <c r="C115" t="n">
         <v>175.416565</v>
@@ -4679,7 +4682,7 @@
         <v>117</v>
       </c>
       <c r="B116" t="n">
-        <v>167.811096</v>
+        <v>167.811081</v>
       </c>
       <c r="C116" t="n">
         <v>173.171753</v>
@@ -4690,7 +4693,7 @@
         <v>118</v>
       </c>
       <c r="B117" t="n">
-        <v>168.626892</v>
+        <v>168.626877</v>
       </c>
       <c r="C117" t="n">
         <v>174.294144</v>
@@ -4701,7 +4704,7 @@
         <v>119</v>
       </c>
       <c r="B118" t="n">
-        <v>166.0979</v>
+        <v>166.097916</v>
       </c>
       <c r="C118" t="n">
         <v>174.294144</v>
@@ -4715,7 +4718,7 @@
         <v>161.243851</v>
       </c>
       <c r="C119" t="n">
-        <v>173.813126</v>
+        <v>173.813141</v>
       </c>
     </row>
     <row r="120">
@@ -4726,7 +4729,7 @@
         <v>162.018875</v>
       </c>
       <c r="C120" t="n">
-        <v>173.652771</v>
+        <v>173.652786</v>
       </c>
     </row>
     <row r="121">
@@ -4770,7 +4773,7 @@
         <v>164.303116</v>
       </c>
       <c r="C124" t="n">
-        <v>177.501038</v>
+        <v>177.501053</v>
       </c>
     </row>
     <row r="125">
@@ -4792,7 +4795,7 @@
         <v>156.797714</v>
       </c>
       <c r="C126" t="n">
-        <v>177.501038</v>
+        <v>177.501053</v>
       </c>
     </row>
     <row r="127">
@@ -4822,7 +4825,7 @@
         <v>130</v>
       </c>
       <c r="B129" t="n">
-        <v>158.102997</v>
+        <v>158.103012</v>
       </c>
       <c r="C129" t="n">
         <v>182.151031</v>
@@ -4844,7 +4847,7 @@
         <v>132</v>
       </c>
       <c r="B131" t="n">
-        <v>159.122757</v>
+        <v>159.122772</v>
       </c>
       <c r="C131" t="n">
         <v>183.754471</v>
@@ -4877,7 +4880,7 @@
         <v>135</v>
       </c>
       <c r="B134" t="n">
-        <v>159.163544</v>
+        <v>159.163559</v>
       </c>
       <c r="C134" t="n">
         <v>180.707932</v>
@@ -4888,7 +4891,7 @@
         <v>136</v>
       </c>
       <c r="B135" t="n">
-        <v>144.642212</v>
+        <v>144.642227</v>
       </c>
       <c r="C135" t="n">
         <v>177.661407</v>
@@ -4902,7 +4905,7 @@
         <v>148.394928</v>
       </c>
       <c r="C136" t="n">
-        <v>179.74585</v>
+        <v>179.745865</v>
       </c>
     </row>
     <row r="137">
@@ -4910,10 +4913,10 @@
         <v>138</v>
       </c>
       <c r="B137" t="n">
-        <v>147.456757</v>
+        <v>147.456741</v>
       </c>
       <c r="C137" t="n">
-        <v>180.387222</v>
+        <v>180.387238</v>
       </c>
     </row>
     <row r="138">
@@ -4921,7 +4924,7 @@
         <v>139</v>
       </c>
       <c r="B138" t="n">
-        <v>149.985748</v>
+        <v>149.985764</v>
       </c>
       <c r="C138" t="n">
         <v>181.669998</v>
@@ -4935,7 +4938,7 @@
         <v>151.94368</v>
       </c>
       <c r="C139" t="n">
-        <v>185.037216</v>
+        <v>185.037231</v>
       </c>
     </row>
     <row r="140">
@@ -4946,7 +4949,7 @@
         <v>150.92392</v>
       </c>
       <c r="C140" t="n">
-        <v>185.518265</v>
+        <v>185.51825</v>
       </c>
     </row>
     <row r="141">
@@ -4957,7 +4960,7 @@
         <v>152.800278</v>
       </c>
       <c r="C141" t="n">
-        <v>186.319962</v>
+        <v>186.319977</v>
       </c>
     </row>
     <row r="142">
@@ -4987,7 +4990,7 @@
         <v>145</v>
       </c>
       <c r="B144" t="n">
-        <v>151.127884</v>
+        <v>151.127869</v>
       </c>
       <c r="C144" t="n">
         <v>189.526855</v>
@@ -5001,7 +5004,7 @@
         <v>149.12915</v>
       </c>
       <c r="C145" t="n">
-        <v>188.083771</v>
+        <v>188.083755</v>
       </c>
     </row>
     <row r="146">
@@ -5012,7 +5015,7 @@
         <v>146.029083</v>
       </c>
       <c r="C146" t="n">
-        <v>184.395844</v>
+        <v>184.395859</v>
       </c>
     </row>
     <row r="147">
@@ -5023,7 +5026,7 @@
         <v>149.12915</v>
       </c>
       <c r="C147" t="n">
-        <v>185.037216</v>
+        <v>185.037231</v>
       </c>
     </row>
     <row r="148">
@@ -5031,7 +5034,7 @@
         <v>149</v>
       </c>
       <c r="B148" t="n">
-        <v>147.53833</v>
+        <v>147.538345</v>
       </c>
       <c r="C148" t="n">
         <v>177.180344</v>
@@ -5042,10 +5045,10 @@
         <v>150</v>
       </c>
       <c r="B149" t="n">
-        <v>147.905441</v>
+        <v>147.905457</v>
       </c>
       <c r="C149" t="n">
-        <v>180.387222</v>
+        <v>180.387238</v>
       </c>
     </row>
     <row r="150">
@@ -5056,7 +5059,7 @@
         <v>147.415955</v>
       </c>
       <c r="C150" t="n">
-        <v>178.14241</v>
+        <v>178.142426</v>
       </c>
     </row>
     <row r="151">
@@ -5078,7 +5081,7 @@
         <v>149.700211</v>
       </c>
       <c r="C152" t="n">
-        <v>177.501038</v>
+        <v>177.501053</v>
       </c>
     </row>
     <row r="153">
@@ -5086,10 +5089,10 @@
         <v>154</v>
       </c>
       <c r="B153" t="n">
-        <v>150.026535</v>
+        <v>150.02652</v>
       </c>
       <c r="C153" t="n">
-        <v>178.30275</v>
+        <v>178.302765</v>
       </c>
     </row>
     <row r="154">
@@ -5100,7 +5103,7 @@
         <v>147.008057</v>
       </c>
       <c r="C154" t="n">
-        <v>176.538971</v>
+        <v>176.538986</v>
       </c>
     </row>
     <row r="155">
@@ -5119,10 +5122,10 @@
         <v>157</v>
       </c>
       <c r="B156" t="n">
-        <v>148.313354</v>
+        <v>148.313339</v>
       </c>
       <c r="C156" t="n">
-        <v>176.218292</v>
+        <v>176.218277</v>
       </c>
     </row>
     <row r="157">
@@ -5141,7 +5144,7 @@
         <v>159</v>
       </c>
       <c r="B158" t="n">
-        <v>150.230484</v>
+        <v>150.230469</v>
       </c>
       <c r="C158" t="n">
         <v>175.737259</v>
@@ -5152,7 +5155,7 @@
         <v>160</v>
       </c>
       <c r="B159" t="n">
-        <v>150.719955</v>
+        <v>150.719971</v>
       </c>
       <c r="C159" t="n">
         <v>177.661407</v>
@@ -5196,7 +5199,7 @@
         <v>164</v>
       </c>
       <c r="B163" t="n">
-        <v>157.817459</v>
+        <v>157.817474</v>
       </c>
       <c r="C163" t="n">
         <v>175.256226</v>
@@ -5221,7 +5224,7 @@
         <v>157.001663</v>
       </c>
       <c r="C165" t="n">
-        <v>153.770096</v>
+        <v>153.770111</v>
       </c>
     </row>
     <row r="166">
@@ -5229,7 +5232,7 @@
         <v>167</v>
       </c>
       <c r="B166" t="n">
-        <v>156.634552</v>
+        <v>156.634567</v>
       </c>
       <c r="C166" t="n">
         <v>151.926132</v>
@@ -5243,7 +5246,7 @@
         <v>154.146347</v>
       </c>
       <c r="C167" t="n">
-        <v>150.723557</v>
+        <v>150.723541</v>
       </c>
     </row>
     <row r="168">
@@ -5254,7 +5257,7 @@
         <v>154.309509</v>
       </c>
       <c r="C168" t="n">
-        <v>149.120102</v>
+        <v>149.120117</v>
       </c>
     </row>
     <row r="169">
@@ -5284,7 +5287,7 @@
         <v>172</v>
       </c>
       <c r="B171" t="n">
-        <v>150.719955</v>
+        <v>150.719971</v>
       </c>
       <c r="C171" t="n">
         <v>148.158051</v>
@@ -5295,10 +5298,10 @@
         <v>173</v>
       </c>
       <c r="B172" t="n">
-        <v>144.397476</v>
+        <v>144.397491</v>
       </c>
       <c r="C172" t="n">
-        <v>148.799438</v>
+        <v>148.799423</v>
       </c>
     </row>
     <row r="173">
@@ -5309,7 +5312,7 @@
         <v>140.155304</v>
       </c>
       <c r="C173" t="n">
-        <v>148.799438</v>
+        <v>148.799423</v>
       </c>
     </row>
     <row r="174">
@@ -5328,7 +5331,7 @@
         <v>176</v>
       </c>
       <c r="B175" t="n">
-        <v>137.096039</v>
+        <v>137.096024</v>
       </c>
       <c r="C175" t="n">
         <v>148.39856</v>
@@ -5364,7 +5367,7 @@
         <v>137.748672</v>
       </c>
       <c r="C178" t="n">
-        <v>149.200302</v>
+        <v>149.200287</v>
       </c>
     </row>
     <row r="179">
@@ -5386,7 +5389,7 @@
         <v>137.871048</v>
       </c>
       <c r="C180" t="n">
-        <v>149.92186</v>
+        <v>149.921844</v>
       </c>
     </row>
     <row r="181">
@@ -5394,10 +5397,10 @@
         <v>182</v>
       </c>
       <c r="B181" t="n">
-        <v>144.397476</v>
+        <v>144.397491</v>
       </c>
       <c r="C181" t="n">
-        <v>151.284775</v>
+        <v>151.28476</v>
       </c>
     </row>
     <row r="182">
@@ -5408,7 +5411,7 @@
         <v>138.727646</v>
       </c>
       <c r="C182" t="n">
-        <v>152.888214</v>
+        <v>152.888199</v>
       </c>
     </row>
     <row r="183">
@@ -5427,7 +5430,7 @@
         <v>185</v>
       </c>
       <c r="B184" t="n">
-        <v>138.686859</v>
+        <v>138.686844</v>
       </c>
       <c r="C184" t="n">
         <v>152.968384</v>
@@ -5441,7 +5444,7 @@
         <v>140.563202</v>
       </c>
       <c r="C185" t="n">
-        <v>155.934753</v>
+        <v>155.934738</v>
       </c>
     </row>
     <row r="186">
@@ -5449,7 +5452,7 @@
         <v>187</v>
       </c>
       <c r="B186" t="n">
-        <v>138.768433</v>
+        <v>138.768448</v>
       </c>
       <c r="C186" t="n">
         <v>151.364929</v>
@@ -5460,7 +5463,7 @@
         <v>188</v>
       </c>
       <c r="B187" t="n">
-        <v>137.626312</v>
+        <v>137.626297</v>
       </c>
       <c r="C187" t="n">
         <v>151.525284</v>
@@ -5474,7 +5477,7 @@
         <v>138.238144</v>
       </c>
       <c r="C188" t="n">
-        <v>152.647675</v>
+        <v>152.64769</v>
       </c>
     </row>
     <row r="189">
@@ -5482,7 +5485,7 @@
         <v>190</v>
       </c>
       <c r="B189" t="n">
-        <v>137.667099</v>
+        <v>137.667084</v>
       </c>
       <c r="C189" t="n">
         <v>150.402878</v>
@@ -5496,7 +5499,7 @@
         <v>135.627579</v>
       </c>
       <c r="C190" t="n">
-        <v>149.440781</v>
+        <v>149.440796</v>
       </c>
     </row>
     <row r="191">
@@ -5504,7 +5507,7 @@
         <v>192</v>
       </c>
       <c r="B191" t="n">
-        <v>129.386688</v>
+        <v>129.386673</v>
       </c>
       <c r="C191" t="n">
         <v>148.158051</v>
@@ -5515,10 +5518,10 @@
         <v>193</v>
       </c>
       <c r="B192" t="n">
-        <v>121.310188</v>
+        <v>121.310196</v>
       </c>
       <c r="C192" t="n">
-        <v>150.483032</v>
+        <v>150.483047</v>
       </c>
     </row>
     <row r="193">
@@ -5526,7 +5529,7 @@
         <v>194</v>
       </c>
       <c r="B193" t="n">
-        <v>116.945656</v>
+        <v>116.945648</v>
       </c>
       <c r="C193" t="n">
         <v>146.795135</v>
@@ -5581,7 +5584,7 @@
         <v>199</v>
       </c>
       <c r="B198" t="n">
-        <v>113.886375</v>
+        <v>113.886383</v>
       </c>
       <c r="C198" t="n">
         <v>142.546005</v>
@@ -5592,7 +5595,7 @@
         <v>200</v>
       </c>
       <c r="B199" t="n">
-        <v>115.436417</v>
+        <v>115.436401</v>
       </c>
       <c r="C199" t="n">
         <v>143.588242</v>
@@ -5603,7 +5606,7 @@
         <v>201</v>
       </c>
       <c r="B200" t="n">
-        <v>112.254776</v>
+        <v>112.254768</v>
       </c>
       <c r="C200" t="n">
         <v>143.748581</v>
@@ -5625,10 +5628,10 @@
         <v>203</v>
       </c>
       <c r="B202" t="n">
-        <v>107.033615</v>
+        <v>107.033607</v>
       </c>
       <c r="C202" t="n">
-        <v>142.706345</v>
+        <v>142.70636</v>
       </c>
     </row>
     <row r="203">
@@ -5672,7 +5675,7 @@
         <v>103.076958</v>
       </c>
       <c r="C206" t="n">
-        <v>142.064987</v>
+        <v>142.064972</v>
       </c>
     </row>
     <row r="207">
@@ -5683,7 +5686,7 @@
         <v>102.791428</v>
       </c>
       <c r="C207" t="n">
-        <v>140.862396</v>
+        <v>140.862381</v>
       </c>
     </row>
     <row r="208">
@@ -5691,7 +5694,7 @@
         <v>209</v>
       </c>
       <c r="B208" t="n">
-        <v>104.586189</v>
+        <v>104.586197</v>
       </c>
       <c r="C208" t="n">
         <v>144.069275</v>
@@ -5735,10 +5738,10 @@
         <v>213</v>
       </c>
       <c r="B212" t="n">
-        <v>111.765274</v>
+        <v>111.765282</v>
       </c>
       <c r="C212" t="n">
-        <v>127.874504</v>
+        <v>127.874519</v>
       </c>
     </row>
     <row r="213">
@@ -5760,7 +5763,7 @@
         <v>110.174461</v>
       </c>
       <c r="C214" t="n">
-        <v>130.680542</v>
+        <v>130.680527</v>
       </c>
     </row>
     <row r="215">
@@ -5768,10 +5771,10 @@
         <v>216</v>
       </c>
       <c r="B215" t="n">
-        <v>117.516716</v>
+        <v>117.516708</v>
       </c>
       <c r="C215" t="n">
-        <v>132.52449</v>
+        <v>132.524506</v>
       </c>
     </row>
     <row r="216">
@@ -5779,7 +5782,7 @@
         <v>217</v>
       </c>
       <c r="B216" t="n">
-        <v>117.027229</v>
+        <v>117.027222</v>
       </c>
       <c r="C216" t="n">
         <v>133.326218</v>
@@ -5793,7 +5796,7 @@
         <v>117.598282</v>
       </c>
       <c r="C217" t="n">
-        <v>131.32193</v>
+        <v>131.321915</v>
       </c>
     </row>
     <row r="218">
@@ -5801,10 +5804,10 @@
         <v>219</v>
       </c>
       <c r="B218" t="n">
-        <v>116.619316</v>
+        <v>116.619324</v>
       </c>
       <c r="C218" t="n">
-        <v>130.440018</v>
+        <v>130.440002</v>
       </c>
     </row>
     <row r="219">
@@ -5812,10 +5815,10 @@
         <v>220</v>
       </c>
       <c r="B219" t="n">
-        <v>115.028496</v>
+        <v>115.028503</v>
       </c>
       <c r="C219" t="n">
-        <v>129.79863</v>
+        <v>129.798645</v>
       </c>
     </row>
     <row r="220">
@@ -5837,7 +5840,7 @@
         <v>113.519257</v>
       </c>
       <c r="C221" t="n">
-        <v>127.874504</v>
+        <v>127.874519</v>
       </c>
     </row>
     <row r="222">
@@ -5856,7 +5859,7 @@
         <v>224</v>
       </c>
       <c r="B223" t="n">
-        <v>110.500786</v>
+        <v>110.500778</v>
       </c>
       <c r="C223" t="n">
         <v>128.756409</v>
@@ -5881,7 +5884,7 @@
         <v>107.441513</v>
       </c>
       <c r="C225" t="n">
-        <v>127.874504</v>
+        <v>127.874519</v>
       </c>
     </row>
     <row r="226">
@@ -5889,10 +5892,10 @@
         <v>227</v>
       </c>
       <c r="B226" t="n">
-        <v>108.461266</v>
+        <v>108.461273</v>
       </c>
       <c r="C226" t="n">
-        <v>127.874504</v>
+        <v>127.874519</v>
       </c>
     </row>
     <row r="227">
@@ -5903,7 +5906,7 @@
         <v>108.869164</v>
       </c>
       <c r="C227" t="n">
-        <v>128.27536</v>
+        <v>128.275375</v>
       </c>
     </row>
     <row r="228">
@@ -5911,7 +5914,7 @@
         <v>229</v>
       </c>
       <c r="B228" t="n">
-        <v>111.071838</v>
+        <v>111.071846</v>
       </c>
       <c r="C228" t="n">
         <v>131.08139</v>
@@ -5922,7 +5925,7 @@
         <v>230</v>
       </c>
       <c r="B229" t="n">
-        <v>110.133667</v>
+        <v>110.133675</v>
       </c>
       <c r="C229" t="n">
         <v>131.08139</v>
@@ -5955,7 +5958,7 @@
         <v>233</v>
       </c>
       <c r="B232" t="n">
-        <v>107.196777</v>
+        <v>107.19677</v>
       </c>
       <c r="C232" t="n">
         <v>130.359848</v>
@@ -5969,7 +5972,7 @@
         <v>108.706017</v>
       </c>
       <c r="C233" t="n">
-        <v>126.671928</v>
+        <v>126.671936</v>
       </c>
     </row>
     <row r="234">
@@ -5980,7 +5983,7 @@
         <v>108.583641</v>
       </c>
       <c r="C234" t="n">
-        <v>127.152977</v>
+        <v>127.152962</v>
       </c>
     </row>
     <row r="235">
@@ -5991,7 +5994,7 @@
         <v>114.620605</v>
       </c>
       <c r="C235" t="n">
-        <v>129.79863</v>
+        <v>129.798645</v>
       </c>
     </row>
     <row r="236">
@@ -5999,7 +6002,7 @@
         <v>237</v>
       </c>
       <c r="B236" t="n">
-        <v>111.316589</v>
+        <v>111.316582</v>
       </c>
       <c r="C236" t="n">
         <v>126.992607</v>
@@ -6013,7 +6016,7 @@
         <v>116.007462</v>
       </c>
       <c r="C237" t="n">
-        <v>129.558136</v>
+        <v>129.558121</v>
       </c>
     </row>
     <row r="238">
@@ -6021,10 +6024,10 @@
         <v>239</v>
       </c>
       <c r="B238" t="n">
-        <v>112.050812</v>
+        <v>112.050827</v>
       </c>
       <c r="C238" t="n">
-        <v>127.152977</v>
+        <v>127.152962</v>
       </c>
     </row>
     <row r="239">
@@ -6032,10 +6035,10 @@
         <v>240</v>
       </c>
       <c r="B239" t="n">
-        <v>114.2127</v>
+        <v>114.212692</v>
       </c>
       <c r="C239" t="n">
-        <v>129.558136</v>
+        <v>129.558121</v>
       </c>
     </row>
     <row r="240">
@@ -6046,7 +6049,7 @@
         <v>113.519257</v>
       </c>
       <c r="C240" t="n">
-        <v>129.077103</v>
+        <v>129.077087</v>
       </c>
     </row>
     <row r="241">
@@ -6057,7 +6060,7 @@
         <v>113.396889</v>
       </c>
       <c r="C241" t="n">
-        <v>128.676239</v>
+        <v>128.676224</v>
       </c>
     </row>
     <row r="242">
@@ -6068,7 +6071,7 @@
         <v>112.62188</v>
       </c>
       <c r="C242" t="n">
-        <v>128.034866</v>
+        <v>128.034851</v>
       </c>
     </row>
     <row r="243">
@@ -6076,7 +6079,7 @@
         <v>244</v>
       </c>
       <c r="B243" t="n">
-        <v>110.459984</v>
+        <v>110.459991</v>
       </c>
       <c r="C243" t="n">
         <v>127.633987</v>
@@ -6090,7 +6093,7 @@
         <v>112.213982</v>
       </c>
       <c r="C244" t="n">
-        <v>122.663315</v>
+        <v>122.663322</v>
       </c>
     </row>
     <row r="245">
@@ -6109,10 +6112,10 @@
         <v>247</v>
       </c>
       <c r="B246" t="n">
-        <v>105.442795</v>
+        <v>105.442787</v>
       </c>
       <c r="C246" t="n">
-        <v>117.772827</v>
+        <v>117.77282</v>
       </c>
     </row>
     <row r="247">
@@ -6123,7 +6126,7 @@
         <v>104.626984</v>
       </c>
       <c r="C247" t="n">
-        <v>120.258163</v>
+        <v>120.258156</v>
       </c>
     </row>
     <row r="248">
@@ -6134,7 +6137,7 @@
         <v>102.95459</v>
       </c>
       <c r="C248" t="n">
-        <v>120.819351</v>
+        <v>120.819366</v>
       </c>
     </row>
     <row r="249">
@@ -6153,10 +6156,10 @@
         <v>251</v>
       </c>
       <c r="B250" t="n">
-        <v>104.994095</v>
+        <v>104.994102</v>
       </c>
       <c r="C250" t="n">
-        <v>126.271065</v>
+        <v>126.27108</v>
       </c>
     </row>
     <row r="251">
@@ -6178,7 +6181,7 @@
         <v>109.195503</v>
       </c>
       <c r="C252" t="n">
-        <v>127.313301</v>
+        <v>127.313316</v>
       </c>
     </row>
     <row r="253">
@@ -6186,7 +6189,7 @@
         <v>254</v>
       </c>
       <c r="B253" t="n">
-        <v>108.909966</v>
+        <v>108.909973</v>
       </c>
       <c r="C253" t="n">
         <v>126.591751</v>
@@ -6211,7 +6214,7 @@
         <v>107.074402</v>
       </c>
       <c r="C255" t="n">
-        <v>126.431419</v>
+        <v>126.431404</v>
       </c>
     </row>
     <row r="256">
@@ -6263,10 +6266,10 @@
         <v>261</v>
       </c>
       <c r="B260" t="n">
-        <v>105.034889</v>
+        <v>105.034897</v>
       </c>
       <c r="C260" t="n">
-        <v>126.271065</v>
+        <v>126.27108</v>
       </c>
     </row>
     <row r="261">
@@ -6285,7 +6288,7 @@
         <v>263</v>
       </c>
       <c r="B262" t="n">
-        <v>103.199333</v>
+        <v>103.199326</v>
       </c>
       <c r="C262" t="n">
         <v>125.870209</v>
@@ -6296,7 +6299,7 @@
         <v>264</v>
       </c>
       <c r="B263" t="n">
-        <v>105.238838</v>
+        <v>105.238846</v>
       </c>
       <c r="C263" t="n">
         <v>124.507286</v>
@@ -6329,10 +6332,10 @@
         <v>267</v>
       </c>
       <c r="B266" t="n">
-        <v>99.976898</v>
+        <v>99.976906</v>
       </c>
       <c r="C266" t="n">
-        <v>126.110741</v>
+        <v>126.110725</v>
       </c>
     </row>
     <row r="267">
@@ -6340,7 +6343,7 @@
         <v>268</v>
       </c>
       <c r="B267" t="n">
-        <v>102.138779</v>
+        <v>102.138786</v>
       </c>
       <c r="C267" t="n">
         <v>126.832268</v>
@@ -6365,7 +6368,7 @@
         <v>99.85453</v>
       </c>
       <c r="C269" t="n">
-        <v>123.465042</v>
+        <v>123.465057</v>
       </c>
     </row>
     <row r="270">
@@ -6376,7 +6379,7 @@
         <v>100.140068</v>
       </c>
       <c r="C270" t="n">
-        <v>123.144379</v>
+        <v>123.144363</v>
       </c>
     </row>
     <row r="271">
@@ -6387,7 +6390,7 @@
         <v>98.304497</v>
       </c>
       <c r="C271" t="n">
-        <v>120.739189</v>
+        <v>120.739204</v>
       </c>
     </row>
     <row r="272">
@@ -6395,7 +6398,7 @@
         <v>273</v>
       </c>
       <c r="B272" t="n">
-        <v>103.444077</v>
+        <v>103.444069</v>
       </c>
       <c r="C272" t="n">
         <v>121.781418</v>
@@ -6406,7 +6409,7 @@
         <v>274</v>
       </c>
       <c r="B273" t="n">
-        <v>101.078239</v>
+        <v>101.078232</v>
       </c>
       <c r="C273" t="n">
         <v>122.262466</v>
@@ -6417,7 +6420,7 @@
         <v>275</v>
       </c>
       <c r="B274" t="n">
-        <v>103.199333</v>
+        <v>103.199326</v>
       </c>
       <c r="C274" t="n">
         <v>122.102127</v>
@@ -6464,7 +6467,7 @@
         <v>98.712402</v>
       </c>
       <c r="C278" t="n">
-        <v>119.13575</v>
+        <v>119.135765</v>
       </c>
     </row>
     <row r="279">
@@ -6475,7 +6478,7 @@
         <v>101.119026</v>
       </c>
       <c r="C279" t="n">
-        <v>121.22023</v>
+        <v>121.220215</v>
       </c>
     </row>
     <row r="280">
@@ -6497,7 +6500,7 @@
         <v>99.936104</v>
       </c>
       <c r="C281" t="n">
-        <v>121.22023</v>
+        <v>121.220215</v>
       </c>
     </row>
     <row r="282">
@@ -6527,10 +6530,10 @@
         <v>285</v>
       </c>
       <c r="B284" t="n">
-        <v>102.873009</v>
+        <v>102.873001</v>
       </c>
       <c r="C284" t="n">
-        <v>121.540924</v>
+        <v>121.540909</v>
       </c>
     </row>
     <row r="285">
@@ -6538,7 +6541,7 @@
         <v>286</v>
       </c>
       <c r="B285" t="n">
-        <v>103.117744</v>
+        <v>103.117752</v>
       </c>
       <c r="C285" t="n">
         <v>121.781418</v>
@@ -6560,7 +6563,7 @@
         <v>288</v>
       </c>
       <c r="B287" t="n">
-        <v>98.467667</v>
+        <v>98.467659</v>
       </c>
       <c r="C287" t="n">
         <v>120.578835</v>
@@ -6571,7 +6574,7 @@
         <v>289</v>
       </c>
       <c r="B288" t="n">
-        <v>102.301949</v>
+        <v>102.301941</v>
       </c>
       <c r="C288" t="n">
         <v>121.781418</v>
@@ -6582,10 +6585,10 @@
         <v>290</v>
       </c>
       <c r="B289" t="n">
-        <v>102.220367</v>
+        <v>102.22036</v>
       </c>
       <c r="C289" t="n">
-        <v>119.777115</v>
+        <v>119.77713</v>
       </c>
     </row>
     <row r="290">
@@ -6596,7 +6599,7 @@
         <v>106.054649</v>
       </c>
       <c r="C290" t="n">
-        <v>127.393478</v>
+        <v>127.393471</v>
       </c>
     </row>
     <row r="291">
@@ -6607,7 +6610,7 @@
         <v>106.462555</v>
       </c>
       <c r="C291" t="n">
-        <v>125.228828</v>
+        <v>125.228813</v>
       </c>
     </row>
     <row r="292">
@@ -6629,7 +6632,7 @@
         <v>105.687538</v>
       </c>
       <c r="C293" t="n">
-        <v>122.422806</v>
+        <v>122.422791</v>
       </c>
     </row>
     <row r="294">
@@ -6648,10 +6651,10 @@
         <v>296</v>
       </c>
       <c r="B295" t="n">
-        <v>105.442795</v>
+        <v>105.442787</v>
       </c>
       <c r="C295" t="n">
-        <v>119.616791</v>
+        <v>119.616776</v>
       </c>
     </row>
     <row r="296">
@@ -6659,10 +6662,10 @@
         <v>297</v>
       </c>
       <c r="B296" t="n">
-        <v>104.137512</v>
+        <v>104.137505</v>
       </c>
       <c r="C296" t="n">
-        <v>117.69265</v>
+        <v>117.692642</v>
       </c>
     </row>
     <row r="297">
@@ -6673,7 +6676,7 @@
         <v>103.036171</v>
       </c>
       <c r="C297" t="n">
-        <v>116.570221</v>
+        <v>116.570236</v>
       </c>
     </row>
     <row r="298">
@@ -6684,7 +6687,7 @@
         <v>103.892769</v>
       </c>
       <c r="C298" t="n">
-        <v>115.768517</v>
+        <v>115.768501</v>
       </c>
     </row>
     <row r="299">
@@ -6695,7 +6698,7 @@
         <v>104.463829</v>
       </c>
       <c r="C299" t="n">
-        <v>117.933182</v>
+        <v>117.933174</v>
       </c>
     </row>
     <row r="300">
@@ -6706,7 +6709,7 @@
         <v>105.361206</v>
       </c>
       <c r="C300" t="n">
-        <v>118.013336</v>
+        <v>118.013351</v>
       </c>
     </row>
     <row r="301">
@@ -6714,7 +6717,7 @@
         <v>302</v>
       </c>
       <c r="B301" t="n">
-        <v>107.971802</v>
+        <v>107.971794</v>
       </c>
       <c r="C301" t="n">
         <v>118.654716</v>
@@ -6728,7 +6731,7 @@
         <v>108.706017</v>
       </c>
       <c r="C302" t="n">
-        <v>120.258163</v>
+        <v>120.258156</v>
       </c>
     </row>
     <row r="303">
@@ -6750,7 +6753,7 @@
         <v>110.308449</v>
       </c>
       <c r="C304" t="n">
-        <v>123.304703</v>
+        <v>123.304688</v>
       </c>
     </row>
     <row r="305">
@@ -6772,7 +6775,7 @@
         <v>108.000374</v>
       </c>
       <c r="C306" t="n">
-        <v>120.899544</v>
+        <v>120.899529</v>
       </c>
     </row>
     <row r="307">
@@ -6802,7 +6805,7 @@
         <v>310</v>
       </c>
       <c r="B309" t="n">
-        <v>105.03907</v>
+        <v>105.039078</v>
       </c>
       <c r="C309" t="n">
         <v>114.540001</v>
@@ -6813,7 +6816,7 @@
         <v>311</v>
       </c>
       <c r="B310" t="n">
-        <v>105.474564</v>
+        <v>105.474556</v>
       </c>
       <c r="C310" t="n">
         <v>116.762421</v>
@@ -6824,7 +6827,7 @@
         <v>312</v>
       </c>
       <c r="B311" t="n">
-        <v>101.685837</v>
+        <v>101.685844</v>
       </c>
       <c r="C311" t="n">
         <v>117.104317</v>
@@ -6849,7 +6852,7 @@
         <v>106.066818</v>
       </c>
       <c r="C313" t="n">
-        <v>121.121765</v>
+        <v>121.12178</v>
       </c>
     </row>
     <row r="314">
@@ -6923,7 +6926,7 @@
         <v>321</v>
       </c>
       <c r="B320" t="n">
-        <v>105.95359</v>
+        <v>105.953598</v>
       </c>
       <c r="C320" t="n">
         <v>120.352478</v>
@@ -6934,10 +6937,10 @@
         <v>322</v>
       </c>
       <c r="B321" t="n">
-        <v>108.13102</v>
+        <v>108.131027</v>
       </c>
       <c r="C321" t="n">
-        <v>122.232994</v>
+        <v>122.232979</v>
       </c>
     </row>
     <row r="322">
@@ -6948,7 +6951,7 @@
         <v>110.613289</v>
       </c>
       <c r="C322" t="n">
-        <v>123.51516</v>
+        <v>123.515144</v>
       </c>
     </row>
     <row r="323">
@@ -6981,7 +6984,7 @@
         <v>112.268127</v>
       </c>
       <c r="C325" t="n">
-        <v>124.968254</v>
+        <v>124.968269</v>
       </c>
     </row>
     <row r="326">
@@ -6992,7 +6995,7 @@
         <v>110.87458</v>
       </c>
       <c r="C326" t="n">
-        <v>123.429672</v>
+        <v>123.429657</v>
       </c>
     </row>
     <row r="327">
@@ -7033,7 +7036,7 @@
         <v>331</v>
       </c>
       <c r="B330" t="n">
-        <v>113.705231</v>
+        <v>113.705238</v>
       </c>
       <c r="C330" t="n">
         <v>123.942535</v>
@@ -7044,7 +7047,7 @@
         <v>332</v>
       </c>
       <c r="B331" t="n">
-        <v>102.818108</v>
+        <v>102.8181</v>
       </c>
       <c r="C331" t="n">
         <v>122.831322</v>
@@ -7066,7 +7069,7 @@
         <v>334</v>
       </c>
       <c r="B333" t="n">
-        <v>102.382614</v>
+        <v>102.382622</v>
       </c>
       <c r="C333" t="n">
         <v>109.325867</v>
@@ -7088,7 +7091,7 @@
         <v>336</v>
       </c>
       <c r="B335" t="n">
-        <v>100.510025</v>
+        <v>100.510033</v>
       </c>
       <c r="C335" t="n">
         <v>107.787262</v>
@@ -7143,7 +7146,7 @@
         <v>341</v>
       </c>
       <c r="B340" t="n">
-        <v>96.068085</v>
+        <v>96.068077</v>
       </c>
       <c r="C340" t="n">
         <v>106.590576</v>
@@ -7154,7 +7157,7 @@
         <v>342</v>
       </c>
       <c r="B341" t="n">
-        <v>93.890648</v>
+        <v>93.890656</v>
       </c>
       <c r="C341" t="n">
         <v>106.847015</v>
@@ -7187,7 +7190,7 @@
         <v>345</v>
       </c>
       <c r="B344" t="n">
-        <v>96.416466</v>
+        <v>96.416458</v>
       </c>
       <c r="C344" t="n">
         <v>106.676064</v>
@@ -7209,10 +7212,10 @@
         <v>347</v>
       </c>
       <c r="B346" t="n">
-        <v>96.764854</v>
+        <v>96.764847</v>
       </c>
       <c r="C346" t="n">
-        <v>105.906769</v>
+        <v>105.906761</v>
       </c>
     </row>
     <row r="347">
@@ -7223,7 +7226,7 @@
         <v>96.28582</v>
       </c>
       <c r="C347" t="n">
-        <v>106.334152</v>
+        <v>106.334145</v>
       </c>
     </row>
     <row r="348">
@@ -7253,7 +7256,7 @@
         <v>351</v>
       </c>
       <c r="B350" t="n">
-        <v>97.984215</v>
+        <v>97.984207</v>
       </c>
       <c r="C350" t="n">
         <v>107.359879</v>
@@ -7275,7 +7278,7 @@
         <v>353</v>
       </c>
       <c r="B352" t="n">
-        <v>95.458389</v>
+        <v>95.458397</v>
       </c>
       <c r="C352" t="n">
         <v>107.359879</v>
@@ -7297,10 +7300,10 @@
         <v>355</v>
       </c>
       <c r="B354" t="n">
-        <v>94.674522</v>
+        <v>94.674515</v>
       </c>
       <c r="C354" t="n">
-        <v>107.616318</v>
+        <v>107.61631</v>
       </c>
     </row>
     <row r="355">
@@ -7308,7 +7311,7 @@
         <v>356</v>
       </c>
       <c r="B355" t="n">
-        <v>95.589043</v>
+        <v>95.589035</v>
       </c>
       <c r="C355" t="n">
         <v>108.813004</v>
@@ -7319,7 +7322,7 @@
         <v>357</v>
       </c>
       <c r="B356" t="n">
-        <v>96.851944</v>
+        <v>96.851952</v>
       </c>
       <c r="C356" t="n">
         <v>110.266121</v>
@@ -7333,7 +7336,7 @@
         <v>96.939049</v>
       </c>
       <c r="C357" t="n">
-        <v>111.120895</v>
+        <v>111.120888</v>
       </c>
     </row>
     <row r="358">
@@ -7344,7 +7347,7 @@
         <v>97.374535</v>
       </c>
       <c r="C358" t="n">
-        <v>111.975677</v>
+        <v>111.97567</v>
       </c>
     </row>
     <row r="359">
@@ -7352,7 +7355,7 @@
         <v>360</v>
       </c>
       <c r="B359" t="n">
-        <v>95.458389</v>
+        <v>95.458397</v>
       </c>
       <c r="C359" t="n">
         <v>111.377327</v>
@@ -7377,7 +7380,7 @@
         <v>90.929352</v>
       </c>
       <c r="C361" t="n">
-        <v>110.864456</v>
+        <v>110.864464</v>
       </c>
     </row>
     <row r="362">
@@ -7385,7 +7388,7 @@
         <v>363</v>
       </c>
       <c r="B362" t="n">
-        <v>91.800316</v>
+        <v>91.800323</v>
       </c>
       <c r="C362" t="n">
         <v>113.172348</v>
@@ -7399,7 +7402,7 @@
         <v>90.189026</v>
       </c>
       <c r="C363" t="n">
-        <v>109.667778</v>
+        <v>109.66777</v>
       </c>
     </row>
     <row r="364">
@@ -7410,7 +7413,7 @@
         <v>90.493866</v>
       </c>
       <c r="C364" t="n">
-        <v>108.727516</v>
+        <v>108.727524</v>
       </c>
     </row>
     <row r="365">
@@ -7418,7 +7421,7 @@
         <v>366</v>
       </c>
       <c r="B365" t="n">
-        <v>87.706749</v>
+        <v>87.706757</v>
       </c>
       <c r="C365" t="n">
         <v>107.274406</v>
@@ -7443,7 +7446,7 @@
         <v>87.750305</v>
       </c>
       <c r="C367" t="n">
-        <v>105.222939</v>
+        <v>105.222946</v>
       </c>
     </row>
     <row r="368">
@@ -7451,7 +7454,7 @@
         <v>369</v>
       </c>
       <c r="B368" t="n">
-        <v>89.535797</v>
+        <v>89.535805</v>
       </c>
       <c r="C368" t="n">
         <v>106.676064</v>
@@ -7462,7 +7465,7 @@
         <v>370</v>
       </c>
       <c r="B369" t="n">
-        <v>90.36322</v>
+        <v>90.363213</v>
       </c>
       <c r="C369" t="n">
         <v>106.932487</v>
@@ -7473,7 +7476,7 @@
         <v>371</v>
       </c>
       <c r="B370" t="n">
-        <v>91.234192</v>
+        <v>91.234184</v>
       </c>
       <c r="C370" t="n">
         <v>108.813004</v>
@@ -7506,7 +7509,7 @@
         <v>374</v>
       </c>
       <c r="B373" t="n">
-        <v>91.234192</v>
+        <v>91.234184</v>
       </c>
       <c r="C373" t="n">
         <v>110.180641</v>
@@ -7528,7 +7531,7 @@
         <v>376</v>
       </c>
       <c r="B375" t="n">
-        <v>90.75515</v>
+        <v>90.755157</v>
       </c>
       <c r="C375" t="n">
         <v>109.411346</v>
@@ -7561,7 +7564,7 @@
         <v>379</v>
       </c>
       <c r="B378" t="n">
-        <v>89.492249</v>
+        <v>89.492241</v>
       </c>
       <c r="C378" t="n">
         <v>105.393898</v>
@@ -7575,7 +7578,7 @@
         <v>90.232574</v>
       </c>
       <c r="C379" t="n">
-        <v>106.505096</v>
+        <v>106.505104</v>
       </c>
     </row>
     <row r="380">
@@ -7583,7 +7586,7 @@
         <v>381</v>
       </c>
       <c r="B380" t="n">
-        <v>90.66806</v>
+        <v>90.668053</v>
       </c>
       <c r="C380" t="n">
         <v>104.624596</v>
@@ -7597,7 +7600,7 @@
         <v>91.495483</v>
       </c>
       <c r="C381" t="n">
-        <v>105.222939</v>
+        <v>105.222946</v>
       </c>
     </row>
     <row r="382">
@@ -7616,7 +7619,7 @@
         <v>384</v>
       </c>
       <c r="B383" t="n">
-        <v>89.361595</v>
+        <v>89.361603</v>
       </c>
       <c r="C383" t="n">
         <v>102.145744</v>
@@ -7630,7 +7633,7 @@
         <v>89.274506</v>
       </c>
       <c r="C384" t="n">
-        <v>101.20549</v>
+        <v>101.205498</v>
       </c>
     </row>
     <row r="385">
@@ -7641,7 +7644,7 @@
         <v>88.53418</v>
       </c>
       <c r="C385" t="n">
-        <v>101.632881</v>
+        <v>101.632889</v>
       </c>
     </row>
     <row r="386">
@@ -7660,7 +7663,7 @@
         <v>388</v>
       </c>
       <c r="B387" t="n">
-        <v>89.709984</v>
+        <v>89.709991</v>
       </c>
       <c r="C387" t="n">
         <v>103.684349</v>
@@ -7671,7 +7674,7 @@
         <v>389</v>
       </c>
       <c r="B388" t="n">
-        <v>90.66806</v>
+        <v>90.668053</v>
       </c>
       <c r="C388" t="n">
         <v>104.197212</v>
@@ -7693,7 +7696,7 @@
         <v>391</v>
       </c>
       <c r="B390" t="n">
-        <v>89.14386</v>
+        <v>89.143852</v>
       </c>
       <c r="C390" t="n">
         <v>103.684349</v>
@@ -7704,10 +7707,10 @@
         <v>392</v>
       </c>
       <c r="B391" t="n">
-        <v>87.044823</v>
+        <v>87.044815</v>
       </c>
       <c r="C391" t="n">
-        <v>101.632881</v>
+        <v>101.632889</v>
       </c>
     </row>
     <row r="392">
@@ -7718,7 +7721,7 @@
         <v>87.314819</v>
       </c>
       <c r="C392" t="n">
-        <v>100.350708</v>
+        <v>100.350716</v>
       </c>
     </row>
     <row r="393">
@@ -7737,10 +7740,10 @@
         <v>395</v>
       </c>
       <c r="B394" t="n">
-        <v>85.564163</v>
+        <v>85.564171</v>
       </c>
       <c r="C394" t="n">
-        <v>99.15403</v>
+        <v>99.154037</v>
       </c>
     </row>
     <row r="395">
@@ -7748,10 +7751,10 @@
         <v>396</v>
       </c>
       <c r="B395" t="n">
-        <v>84.066093</v>
+        <v>84.066101</v>
       </c>
       <c r="C395" t="n">
-        <v>98.042824</v>
+        <v>98.042816</v>
       </c>
     </row>
     <row r="396">
@@ -7759,7 +7762,7 @@
         <v>397</v>
       </c>
       <c r="B396" t="n">
-        <v>83.839645</v>
+        <v>83.839653</v>
       </c>
       <c r="C396" t="n">
         <v>99.923325</v>
@@ -7773,7 +7776,7 @@
         <v>83.508675</v>
       </c>
       <c r="C397" t="n">
-        <v>98.726639</v>
+        <v>98.726646</v>
       </c>
     </row>
     <row r="398">
@@ -7781,10 +7784,10 @@
         <v>399</v>
       </c>
       <c r="B398" t="n">
-        <v>83.857071</v>
+        <v>83.857063</v>
       </c>
       <c r="C398" t="n">
-        <v>98.641159</v>
+        <v>98.641167</v>
       </c>
     </row>
     <row r="399">
@@ -7792,7 +7795,7 @@
         <v>400</v>
       </c>
       <c r="B399" t="n">
-        <v>82.672539</v>
+        <v>82.672546</v>
       </c>
       <c r="C399" t="n">
         <v>98.128304</v>
@@ -7817,7 +7820,7 @@
         <v>81.505447</v>
       </c>
       <c r="C401" t="n">
-        <v>95.563972</v>
+        <v>95.56398</v>
       </c>
     </row>
     <row r="402">
@@ -7825,10 +7828,10 @@
         <v>403</v>
       </c>
       <c r="B402" t="n">
-        <v>77.516403</v>
+        <v>77.516396</v>
       </c>
       <c r="C402" t="n">
-        <v>92.230339</v>
+        <v>92.230347</v>
       </c>
     </row>
     <row r="403">
@@ -7839,7 +7842,7 @@
         <v>76.749947</v>
       </c>
       <c r="C403" t="n">
-        <v>91.461044</v>
+        <v>91.461037</v>
       </c>
     </row>
     <row r="404">
@@ -7847,10 +7850,10 @@
         <v>405</v>
       </c>
       <c r="B404" t="n">
-        <v>79.362854</v>
+        <v>79.362862</v>
       </c>
       <c r="C404" t="n">
-        <v>94.70919</v>
+        <v>94.709198</v>
       </c>
     </row>
     <row r="405">
@@ -7869,7 +7872,7 @@
         <v>407</v>
       </c>
       <c r="B406" t="n">
-        <v>77.88221</v>
+        <v>77.882202</v>
       </c>
       <c r="C406" t="n">
         <v>93.597984</v>
@@ -7880,10 +7883,10 @@
         <v>408</v>
       </c>
       <c r="B407" t="n">
-        <v>77.516403</v>
+        <v>77.516396</v>
       </c>
       <c r="C407" t="n">
-        <v>92.65773</v>
+        <v>92.657738</v>
       </c>
     </row>
     <row r="408">
@@ -7891,7 +7894,7 @@
         <v>409</v>
       </c>
       <c r="B408" t="n">
-        <v>78.561562</v>
+        <v>78.561554</v>
       </c>
       <c r="C408" t="n">
         <v>94.88015</v>
@@ -7902,7 +7905,7 @@
         <v>410</v>
       </c>
       <c r="B409" t="n">
-        <v>77.673172</v>
+        <v>77.67318</v>
       </c>
       <c r="C409" t="n">
         <v>94.88015</v>
@@ -7913,7 +7916,7 @@
         <v>411</v>
       </c>
       <c r="B410" t="n">
-        <v>76.418976</v>
+        <v>76.418968</v>
       </c>
       <c r="C410" t="n">
         <v>93.256073</v>
@@ -7946,7 +7949,7 @@
         <v>414</v>
       </c>
       <c r="B413" t="n">
-        <v>76.593178</v>
+        <v>76.59317</v>
       </c>
       <c r="C413" t="n">
         <v>80.348953</v>
@@ -8004,7 +8007,7 @@
         <v>78.875107</v>
       </c>
       <c r="C418" t="n">
-        <v>82.998756</v>
+        <v>82.998764</v>
       </c>
     </row>
     <row r="419">
@@ -8034,7 +8037,7 @@
         <v>422</v>
       </c>
       <c r="B421" t="n">
-        <v>88.055138</v>
+        <v>88.055145</v>
       </c>
       <c r="C421" t="n">
         <v>88.554802</v>
@@ -8056,10 +8059,10 @@
         <v>424</v>
       </c>
       <c r="B423" t="n">
-        <v>88.011597</v>
+        <v>88.011604</v>
       </c>
       <c r="C423" t="n">
-        <v>87.870987</v>
+        <v>87.870979</v>
       </c>
     </row>
     <row r="424">
@@ -8081,7 +8084,7 @@
         <v>88.22934</v>
       </c>
       <c r="C425" t="n">
-        <v>88.640274</v>
+        <v>88.640282</v>
       </c>
     </row>
     <row r="426">
@@ -8100,7 +8103,7 @@
         <v>428</v>
       </c>
       <c r="B427" t="n">
-        <v>83.247383</v>
+        <v>83.247391</v>
       </c>
       <c r="C427" t="n">
         <v>87.529076</v>
@@ -8111,10 +8114,10 @@
         <v>429</v>
       </c>
       <c r="B428" t="n">
-        <v>84.414482</v>
+        <v>84.41449</v>
       </c>
       <c r="C428" t="n">
-        <v>89.495056</v>
+        <v>89.495064</v>
       </c>
     </row>
     <row r="429">
@@ -8122,7 +8125,7 @@
         <v>430</v>
       </c>
       <c r="B429" t="n">
-        <v>85.355133</v>
+        <v>85.355141</v>
       </c>
       <c r="C429" t="n">
         <v>99.495941</v>
@@ -8133,7 +8136,7 @@
         <v>431</v>
       </c>
       <c r="B430" t="n">
-        <v>83.61319</v>
+        <v>83.613197</v>
       </c>
       <c r="C430" t="n">
         <v>101.461922</v>
@@ -8169,7 +8172,7 @@
         <v>82.289322</v>
       </c>
       <c r="C433" t="n">
-        <v>108.385612</v>
+        <v>108.38562</v>
       </c>
     </row>
     <row r="434">
@@ -8177,7 +8180,7 @@
         <v>435</v>
       </c>
       <c r="B434" t="n">
-        <v>83.386742</v>
+        <v>83.386734</v>
       </c>
       <c r="C434" t="n">
         <v>104.881027</v>
@@ -8199,7 +8202,7 @@
         <v>437</v>
       </c>
       <c r="B436" t="n">
-        <v>82.742226</v>
+        <v>82.742218</v>
       </c>
       <c r="C436" t="n">
         <v>102.402184</v>
@@ -8235,7 +8238,7 @@
         <v>79.989952</v>
       </c>
       <c r="C439" t="n">
-        <v>99.15403</v>
+        <v>99.154037</v>
       </c>
     </row>
     <row r="440">
@@ -8257,7 +8260,7 @@
         <v>80.059631</v>
       </c>
       <c r="C441" t="n">
-        <v>102.658607</v>
+        <v>102.658615</v>
       </c>
     </row>
     <row r="442">
@@ -8276,7 +8279,7 @@
         <v>444</v>
       </c>
       <c r="B443" t="n">
-        <v>80.164146</v>
+        <v>80.164154</v>
       </c>
       <c r="C443" t="n">
         <v>100.521667</v>
@@ -8287,7 +8290,7 @@
         <v>445</v>
       </c>
       <c r="B444" t="n">
-        <v>82.881577</v>
+        <v>82.881584</v>
       </c>
       <c r="C444" t="n">
         <v>102.145744</v>
@@ -8298,10 +8301,10 @@
         <v>446</v>
       </c>
       <c r="B445" t="n">
-        <v>83.595772</v>
+        <v>83.595779</v>
       </c>
       <c r="C445" t="n">
-        <v>104.795547</v>
+        <v>104.795555</v>
       </c>
     </row>
     <row r="446">
@@ -8342,7 +8345,7 @@
         <v>450</v>
       </c>
       <c r="B449" t="n">
-        <v>83.82222</v>
+        <v>83.822227</v>
       </c>
       <c r="C449" t="n">
         <v>110.266121</v>
@@ -8353,10 +8356,10 @@
         <v>451</v>
       </c>
       <c r="B450" t="n">
-        <v>85.877716</v>
+        <v>85.877724</v>
       </c>
       <c r="C450" t="n">
-        <v>112.659492</v>
+        <v>112.6595</v>
       </c>
     </row>
     <row r="451">
@@ -8364,7 +8367,7 @@
         <v>452</v>
       </c>
       <c r="B451" t="n">
-        <v>85.877716</v>
+        <v>85.877724</v>
       </c>
       <c r="C451" t="n">
         <v>113.257835</v>
@@ -8397,7 +8400,7 @@
         <v>455</v>
       </c>
       <c r="B454" t="n">
-        <v>85.877716</v>
+        <v>85.877724</v>
       </c>
       <c r="C454" t="n">
         <v>116.078598</v>
@@ -8422,7 +8425,7 @@
         <v>84.867393</v>
       </c>
       <c r="C456" t="n">
-        <v>115.736671</v>
+        <v>115.736687</v>
       </c>
     </row>
     <row r="457">
@@ -8441,7 +8444,7 @@
         <v>459</v>
       </c>
       <c r="B458" t="n">
-        <v>83.247383</v>
+        <v>83.247391</v>
       </c>
       <c r="C458" t="n">
         <v>112.317574</v>
@@ -8485,7 +8488,7 @@
         <v>463</v>
       </c>
       <c r="B462" t="n">
-        <v>81.766739</v>
+        <v>81.766731</v>
       </c>
       <c r="C462" t="n">
         <v>115.651207</v>
@@ -8496,7 +8499,7 @@
         <v>464</v>
       </c>
       <c r="B463" t="n">
-        <v>83.630615</v>
+        <v>83.630608</v>
       </c>
       <c r="C463" t="n">
         <v>116.33503</v>
@@ -8510,7 +8513,7 @@
         <v>83.369324</v>
       </c>
       <c r="C464" t="n">
-        <v>115.993111</v>
+        <v>115.993118</v>
       </c>
     </row>
     <row r="465">
@@ -8529,7 +8532,7 @@
         <v>467</v>
       </c>
       <c r="B466" t="n">
-        <v>82.306732</v>
+        <v>82.30674</v>
       </c>
       <c r="C466" t="n">
         <v>116.93338</v>
@@ -8540,10 +8543,10 @@
         <v>468</v>
       </c>
       <c r="B467" t="n">
-        <v>80.442856</v>
+        <v>80.442863</v>
       </c>
       <c r="C467" t="n">
-        <v>113.514267</v>
+        <v>113.514275</v>
       </c>
     </row>
     <row r="468">
@@ -8573,7 +8576,7 @@
         <v>471</v>
       </c>
       <c r="B470" t="n">
-        <v>79.240921</v>
+        <v>79.240929</v>
       </c>
       <c r="C470" t="n">
         <v>110.949944</v>
@@ -8584,10 +8587,10 @@
         <v>472</v>
       </c>
       <c r="B471" t="n">
-        <v>79.362854</v>
+        <v>79.362862</v>
       </c>
       <c r="C471" t="n">
-        <v>110.864456</v>
+        <v>110.864464</v>
       </c>
     </row>
     <row r="472">
@@ -8609,7 +8612,7 @@
         <v>78.735756</v>
       </c>
       <c r="C473" t="n">
-        <v>108.727516</v>
+        <v>108.727524</v>
       </c>
     </row>
     <row r="474">
@@ -8642,7 +8645,7 @@
         <v>79.275757</v>
       </c>
       <c r="C476" t="n">
-        <v>108.727516</v>
+        <v>108.727524</v>
       </c>
     </row>
     <row r="477">
@@ -8672,10 +8675,10 @@
         <v>480</v>
       </c>
       <c r="B479" t="n">
-        <v>79.746086</v>
+        <v>79.746078</v>
       </c>
       <c r="C479" t="n">
-        <v>109.154907</v>
+        <v>109.154915</v>
       </c>
     </row>
     <row r="480">
@@ -8697,7 +8700,7 @@
         <v>79.223503</v>
       </c>
       <c r="C481" t="n">
-        <v>105.479378</v>
+        <v>105.47937</v>
       </c>
     </row>
     <row r="482">
@@ -8705,7 +8708,7 @@
         <v>483</v>
       </c>
       <c r="B482" t="n">
-        <v>79.780922</v>
+        <v>79.780914</v>
       </c>
       <c r="C482" t="n">
         <v>108.983955</v>
@@ -8716,7 +8719,7 @@
         <v>484</v>
       </c>
       <c r="B483" t="n">
-        <v>82.463516</v>
+        <v>82.463509</v>
       </c>
       <c r="C483" t="n">
         <v>110.949944</v>
@@ -8752,7 +8755,7 @@
         <v>84.170616</v>
       </c>
       <c r="C486" t="n">
-        <v>113.343323</v>
+        <v>113.343315</v>
       </c>
     </row>
     <row r="487">
@@ -8774,7 +8777,7 @@
         <v>87.271271</v>
       </c>
       <c r="C488" t="n">
-        <v>113.941658</v>
+        <v>113.94165</v>
       </c>
     </row>
     <row r="489">
@@ -8796,7 +8799,7 @@
         <v>92.671295</v>
       </c>
       <c r="C490" t="n">
-        <v>112.488541</v>
+        <v>112.488548</v>
       </c>
     </row>
     <row r="491">
@@ -8804,7 +8807,7 @@
         <v>492</v>
       </c>
       <c r="B491" t="n">
-        <v>94.108391</v>
+        <v>94.108398</v>
       </c>
       <c r="C491" t="n">
         <v>117.104317</v>
@@ -8815,7 +8818,7 @@
         <v>493</v>
       </c>
       <c r="B492" t="n">
-        <v>93.193871</v>
+        <v>93.193878</v>
       </c>
       <c r="C492" t="n">
         <v>118.215546</v>
@@ -8848,10 +8851,10 @@
         <v>496</v>
       </c>
       <c r="B495" t="n">
-        <v>93.193871</v>
+        <v>93.193878</v>
       </c>
       <c r="C495" t="n">
-        <v>118.899368</v>
+        <v>118.899353</v>
       </c>
     </row>
     <row r="496">
@@ -8870,10 +8873,10 @@
         <v>498</v>
       </c>
       <c r="B497" t="n">
-        <v>93.890648</v>
+        <v>93.890656</v>
       </c>
       <c r="C497" t="n">
-        <v>119.497711</v>
+        <v>119.497704</v>
       </c>
     </row>
     <row r="498">
@@ -8881,7 +8884,7 @@
         <v>499</v>
       </c>
       <c r="B498" t="n">
-        <v>96.111626</v>
+        <v>96.111618</v>
       </c>
       <c r="C498" t="n">
         <v>121.976547</v>
@@ -8892,7 +8895,7 @@
         <v>500</v>
       </c>
       <c r="B499" t="n">
-        <v>93.977753</v>
+        <v>93.977745</v>
       </c>
       <c r="C499" t="n">
         <v>121.463692</v>
@@ -8917,7 +8920,7 @@
         <v>93.847099</v>
       </c>
       <c r="C501" t="n">
-        <v>120.694374</v>
+        <v>120.694389</v>
       </c>
     </row>
     <row r="502">
@@ -8936,7 +8939,7 @@
         <v>504</v>
       </c>
       <c r="B503" t="n">
-        <v>96.068085</v>
+        <v>96.068077</v>
       </c>
       <c r="C503" t="n">
         <v>124.369926</v>
@@ -8947,7 +8950,7 @@
         <v>505</v>
       </c>
       <c r="B504" t="n">
-        <v>94.97937</v>
+        <v>94.979362</v>
       </c>
       <c r="C504" t="n">
         <v>121.976547</v>
@@ -8969,10 +8972,10 @@
         <v>507</v>
       </c>
       <c r="B506" t="n">
-        <v>94.06485</v>
+        <v>94.064842</v>
       </c>
       <c r="C506" t="n">
-        <v>123.686089</v>
+        <v>123.686104</v>
       </c>
     </row>
     <row r="507">
@@ -8991,10 +8994,10 @@
         <v>509</v>
       </c>
       <c r="B508" t="n">
-        <v>94.674522</v>
+        <v>94.674515</v>
       </c>
       <c r="C508" t="n">
-        <v>123.600624</v>
+        <v>123.600639</v>
       </c>
     </row>
     <row r="509">
@@ -9013,10 +9016,10 @@
         <v>511</v>
       </c>
       <c r="B510" t="n">
-        <v>95.632591</v>
+        <v>95.632599</v>
       </c>
       <c r="C510" t="n">
-        <v>127.361649</v>
+        <v>127.361641</v>
       </c>
     </row>
     <row r="511">
@@ -9038,7 +9041,7 @@
         <v>96.721306</v>
       </c>
       <c r="C512" t="n">
-        <v>127.703537</v>
+        <v>127.703552</v>
       </c>
     </row>
     <row r="513">
@@ -9049,7 +9052,7 @@
         <v>94.848717</v>
       </c>
       <c r="C513" t="n">
-        <v>126.934265</v>
+        <v>126.93425</v>
       </c>
     </row>
     <row r="514">
@@ -9057,7 +9060,7 @@
         <v>515</v>
       </c>
       <c r="B514" t="n">
-        <v>95.458389</v>
+        <v>95.458397</v>
       </c>
       <c r="C514" t="n">
         <v>125.993988</v>
@@ -9071,7 +9074,7 @@
         <v>92.453545</v>
       </c>
       <c r="C515" t="n">
-        <v>123.087769</v>
+        <v>123.087761</v>
       </c>
     </row>
     <row r="516">
@@ -9090,7 +9093,7 @@
         <v>518</v>
       </c>
       <c r="B517" t="n">
-        <v>95.893883</v>
+        <v>95.893875</v>
       </c>
       <c r="C517" t="n">
         <v>125.993988</v>
@@ -9101,10 +9104,10 @@
         <v>519</v>
       </c>
       <c r="B518" t="n">
-        <v>94.674522</v>
+        <v>94.674515</v>
       </c>
       <c r="C518" t="n">
-        <v>124.198967</v>
+        <v>124.198982</v>
       </c>
     </row>
     <row r="519">
@@ -9115,7 +9118,7 @@
         <v>98.332603</v>
       </c>
       <c r="C519" t="n">
-        <v>125.48114</v>
+        <v>125.481125</v>
       </c>
     </row>
     <row r="520">
@@ -9123,7 +9126,7 @@
         <v>521</v>
       </c>
       <c r="B520" t="n">
-        <v>97.200333</v>
+        <v>97.20034</v>
       </c>
       <c r="C520" t="n">
         <v>125.652092</v>
@@ -9134,7 +9137,7 @@
         <v>522</v>
       </c>
       <c r="B521" t="n">
-        <v>99.943893</v>
+        <v>99.943901</v>
       </c>
       <c r="C521" t="n">
         <v>127.276161</v>
@@ -9145,7 +9148,7 @@
         <v>523</v>
       </c>
       <c r="B522" t="n">
-        <v>100.422935</v>
+        <v>100.422928</v>
       </c>
       <c r="C522" t="n">
         <v>128.472855</v>
@@ -9156,7 +9159,7 @@
         <v>524</v>
       </c>
       <c r="B523" t="n">
-        <v>102.164879</v>
+        <v>102.164871</v>
       </c>
       <c r="C523" t="n">
         <v>131.293625</v>
@@ -9167,7 +9170,7 @@
         <v>525</v>
       </c>
       <c r="B524" t="n">
-        <v>102.51326</v>
+        <v>102.513252</v>
       </c>
       <c r="C524" t="n">
         <v>130.438843</v>
@@ -9189,10 +9192,10 @@
         <v>527</v>
       </c>
       <c r="B526" t="n">
-        <v>105.822952</v>
+        <v>105.822945</v>
       </c>
       <c r="C526" t="n">
-        <v>133.516037</v>
+        <v>133.516022</v>
       </c>
     </row>
     <row r="527">
@@ -9200,7 +9203,7 @@
         <v>528</v>
       </c>
       <c r="B527" t="n">
-        <v>107.608437</v>
+        <v>107.608444</v>
       </c>
       <c r="C527" t="n">
         <v>134.285324</v>
@@ -9211,7 +9214,7 @@
         <v>529</v>
       </c>
       <c r="B528" t="n">
-        <v>106.51973</v>
+        <v>106.519722</v>
       </c>
       <c r="C528" t="n">
         <v>134.19986</v>
@@ -9236,7 +9239,7 @@
         <v>104.951973</v>
       </c>
       <c r="C530" t="n">
-        <v>135.909393</v>
+        <v>135.909409</v>
       </c>
     </row>
     <row r="531">
@@ -9266,10 +9269,10 @@
         <v>534</v>
       </c>
       <c r="B533" t="n">
-        <v>106.476181</v>
+        <v>106.476173</v>
       </c>
       <c r="C533" t="n">
-        <v>138.47374</v>
+        <v>138.473724</v>
       </c>
     </row>
     <row r="534">
@@ -9302,7 +9305,7 @@
         <v>99.116478</v>
       </c>
       <c r="C536" t="n">
-        <v>130.951706</v>
+        <v>130.951691</v>
       </c>
     </row>
     <row r="537">
@@ -9343,7 +9346,7 @@
         <v>541</v>
       </c>
       <c r="B540" t="n">
-        <v>91.582581</v>
+        <v>91.582573</v>
       </c>
       <c r="C540" t="n">
         <v>107.872742</v>
@@ -9354,7 +9357,7 @@
         <v>542</v>
       </c>
       <c r="B541" t="n">
-        <v>93.063232</v>
+        <v>93.063225</v>
       </c>
       <c r="C541" t="n">
         <v>109.838737</v>
@@ -9368,7 +9371,7 @@
         <v>93.237427</v>
       </c>
       <c r="C542" t="n">
-        <v>106.505096</v>
+        <v>106.505104</v>
       </c>
     </row>
     <row r="543">
@@ -9379,7 +9382,7 @@
         <v>91.147095</v>
       </c>
       <c r="C543" t="n">
-        <v>104.795547</v>
+        <v>104.795555</v>
       </c>
     </row>
     <row r="544">
@@ -9409,7 +9412,7 @@
         <v>547</v>
       </c>
       <c r="B546" t="n">
-        <v>77.289948</v>
+        <v>77.28994</v>
       </c>
       <c r="C546" t="n">
         <v>93.854416</v>
@@ -9423,7 +9426,7 @@
         <v>74.48542</v>
       </c>
       <c r="C547" t="n">
-        <v>92.486771</v>
+        <v>92.486763</v>
       </c>
     </row>
     <row r="548">
@@ -9431,10 +9434,10 @@
         <v>549</v>
       </c>
       <c r="B548" t="n">
-        <v>67.726685</v>
+        <v>67.726692</v>
       </c>
       <c r="C548" t="n">
-        <v>82.272194</v>
+        <v>82.272202</v>
       </c>
     </row>
     <row r="549">
@@ -9445,7 +9448,7 @@
         <v>67.761528</v>
       </c>
       <c r="C549" t="n">
-        <v>83.682587</v>
+        <v>83.682579</v>
       </c>
     </row>
     <row r="550">
@@ -9467,7 +9470,7 @@
         <v>64.62603</v>
       </c>
       <c r="C551" t="n">
-        <v>80.220734</v>
+        <v>80.220741</v>
       </c>
     </row>
     <row r="552">
@@ -9478,7 +9481,7 @@
         <v>71.60997</v>
       </c>
       <c r="C552" t="n">
-        <v>77.399986</v>
+        <v>77.399979</v>
       </c>
     </row>
     <row r="553">
@@ -9577,7 +9580,7 @@
         <v>75.642952</v>
       </c>
       <c r="C561" t="n">
-        <v>91.515839</v>
+        <v>91.515846</v>
       </c>
     </row>
     <row r="562">
@@ -9610,7 +9613,7 @@
         <v>71.078796</v>
       </c>
       <c r="C564" t="n">
-        <v>88.706573</v>
+        <v>88.706566</v>
       </c>
     </row>
     <row r="565">
@@ -9621,7 +9624,7 @@
         <v>72.141136</v>
       </c>
       <c r="C565" t="n">
-        <v>88.373268</v>
+        <v>88.37326</v>
       </c>
     </row>
     <row r="566">
@@ -9687,7 +9690,7 @@
         <v>72.318199</v>
       </c>
       <c r="C571" t="n">
-        <v>89.373169</v>
+        <v>89.373177</v>
       </c>
     </row>
     <row r="572">
@@ -9698,7 +9701,7 @@
         <v>71.82637</v>
       </c>
       <c r="C572" t="n">
-        <v>90.992088</v>
+        <v>90.992081</v>
       </c>
     </row>
     <row r="573">
@@ -9731,7 +9734,7 @@
         <v>72.455917</v>
       </c>
       <c r="C575" t="n">
-        <v>91.230164</v>
+        <v>91.230156</v>
       </c>
     </row>
     <row r="576">
@@ -9742,7 +9745,7 @@
         <v>70.134491</v>
       </c>
       <c r="C576" t="n">
-        <v>89.706474</v>
+        <v>89.706482</v>
       </c>
     </row>
     <row r="577">
@@ -9786,7 +9789,7 @@
         <v>79.479202</v>
       </c>
       <c r="C580" t="n">
-        <v>107.89537</v>
+        <v>107.895378</v>
       </c>
     </row>
     <row r="581">
@@ -9830,7 +9833,7 @@
         <v>74.226486</v>
       </c>
       <c r="C584" t="n">
-        <v>95.08696</v>
+        <v>95.086967</v>
       </c>
     </row>
     <row r="585">
@@ -9852,7 +9855,7 @@
         <v>74.619949</v>
       </c>
       <c r="C586" t="n">
-        <v>100.086533</v>
+        <v>100.086525</v>
       </c>
     </row>
     <row r="587">
@@ -9863,7 +9866,7 @@
         <v>74.167473</v>
       </c>
       <c r="C587" t="n">
-        <v>101.134048</v>
+        <v>101.134056</v>
       </c>
     </row>
     <row r="588">
@@ -9896,7 +9899,7 @@
         <v>70.803375</v>
       </c>
       <c r="C590" t="n">
-        <v>99.991302</v>
+        <v>99.991295</v>
       </c>
     </row>
     <row r="591">
@@ -9918,7 +9921,7 @@
         <v>73.400223</v>
       </c>
       <c r="C592" t="n">
-        <v>100.657898</v>
+        <v>100.657906</v>
       </c>
     </row>
     <row r="593">
@@ -9929,7 +9932,7 @@
         <v>75.564255</v>
       </c>
       <c r="C593" t="n">
-        <v>102.467278</v>
+        <v>102.46727</v>
       </c>
     </row>
     <row r="594">
@@ -9973,7 +9976,7 @@
         <v>83.748253</v>
       </c>
       <c r="C597" t="n">
-        <v>111.799789</v>
+        <v>111.799797</v>
       </c>
     </row>
     <row r="598">
@@ -9995,7 +9998,7 @@
         <v>86.128693</v>
       </c>
       <c r="C599" t="n">
-        <v>116.656509</v>
+        <v>116.656517</v>
       </c>
     </row>
     <row r="600">
@@ -10017,7 +10020,7 @@
         <v>89.256706</v>
       </c>
       <c r="C601" t="n">
-        <v>123.893982</v>
+        <v>123.89399</v>
       </c>
     </row>
     <row r="602">
@@ -10072,7 +10075,7 @@
         <v>86.42379</v>
       </c>
       <c r="C606" t="n">
-        <v>117.704041</v>
+        <v>117.704048</v>
       </c>
     </row>
     <row r="607">
@@ -10094,7 +10097,7 @@
         <v>87.663193</v>
       </c>
       <c r="C608" t="n">
-        <v>120.751396</v>
+        <v>120.751404</v>
       </c>
     </row>
     <row r="609">
@@ -10160,7 +10163,7 @@
         <v>87.466461</v>
       </c>
       <c r="C614" t="n">
-        <v>117.704041</v>
+        <v>117.704048</v>
       </c>
     </row>
     <row r="615">
@@ -10204,7 +10207,7 @@
         <v>86.836922</v>
       </c>
       <c r="C618" t="n">
-        <v>117.13266</v>
+        <v>117.132668</v>
       </c>
     </row>
     <row r="619">
@@ -10325,7 +10328,7 @@
         <v>100.185097</v>
       </c>
       <c r="C629" t="n">
-        <v>124.465355</v>
+        <v>124.465363</v>
       </c>
     </row>
     <row r="630">
@@ -10336,7 +10339,7 @@
         <v>100.185097</v>
       </c>
       <c r="C630" t="n">
-        <v>125.512886</v>
+        <v>125.512894</v>
       </c>
     </row>
     <row r="631">
@@ -10358,7 +10361,7 @@
         <v>104.267265</v>
       </c>
       <c r="C632" t="n">
-        <v>125.036736</v>
+        <v>125.036743</v>
       </c>
     </row>
     <row r="633">
@@ -10391,7 +10394,7 @@
         <v>103.72625</v>
       </c>
       <c r="C635" t="n">
-        <v>125.322433</v>
+        <v>125.322441</v>
       </c>
     </row>
     <row r="636">
@@ -10402,7 +10405,7 @@
         <v>104.218079</v>
       </c>
       <c r="C636" t="n">
-        <v>124.941498</v>
+        <v>124.941505</v>
       </c>
     </row>
     <row r="637">
@@ -10413,7 +10416,7 @@
         <v>102.250771</v>
       </c>
       <c r="C637" t="n">
-        <v>122.655998</v>
+        <v>122.655991</v>
       </c>
     </row>
     <row r="638">
@@ -10468,7 +10471,7 @@
         <v>101.168755</v>
       </c>
       <c r="C642" t="n">
-        <v>115.894676</v>
+        <v>115.894669</v>
       </c>
     </row>
     <row r="643">
@@ -10479,7 +10482,7 @@
         <v>100.480202</v>
       </c>
       <c r="C643" t="n">
-        <v>116.75174</v>
+        <v>116.751747</v>
       </c>
     </row>
     <row r="644">
@@ -10490,7 +10493,7 @@
         <v>100.922836</v>
       </c>
       <c r="C644" t="n">
-        <v>115.989914</v>
+        <v>115.989906</v>
       </c>
     </row>
     <row r="645">
@@ -10501,7 +10504,7 @@
         <v>100.332649</v>
       </c>
       <c r="C645" t="n">
-        <v>115.418526</v>
+        <v>115.418518</v>
       </c>
     </row>
     <row r="646">
@@ -10567,7 +10570,7 @@
         <v>102.349144</v>
       </c>
       <c r="C651" t="n">
-        <v>113.609169</v>
+        <v>113.609161</v>
       </c>
     </row>
     <row r="652">
@@ -10611,7 +10614,7 @@
         <v>96.496399</v>
       </c>
       <c r="C655" t="n">
-        <v>110.466576</v>
+        <v>110.466583</v>
       </c>
     </row>
     <row r="656">
@@ -10622,7 +10625,7 @@
         <v>97.047249</v>
       </c>
       <c r="C656" t="n">
-        <v>109.799973</v>
+        <v>109.799965</v>
       </c>
     </row>
     <row r="657">
@@ -10655,7 +10658,7 @@
         <v>97.971878</v>
       </c>
       <c r="C659" t="n">
-        <v>107.228767</v>
+        <v>107.22876</v>
       </c>
     </row>
     <row r="660">
@@ -10666,7 +10669,7 @@
         <v>96.594765</v>
       </c>
       <c r="C660" t="n">
-        <v>106.847847</v>
+        <v>106.847839</v>
       </c>
     </row>
     <row r="661">
@@ -10699,7 +10702,7 @@
         <v>92.463425</v>
       </c>
       <c r="C663" t="n">
-        <v>95.705963</v>
+        <v>95.705956</v>
       </c>
     </row>
     <row r="664">
@@ -10754,7 +10757,7 @@
         <v>87.859924</v>
       </c>
       <c r="C668" t="n">
-        <v>96.467796</v>
+        <v>96.467804</v>
       </c>
     </row>
     <row r="669">
@@ -10765,7 +10768,7 @@
         <v>88.627174</v>
       </c>
       <c r="C669" t="n">
-        <v>98.181938</v>
+        <v>98.181931</v>
       </c>
     </row>
     <row r="670">
@@ -10776,7 +10779,7 @@
         <v>88.587822</v>
       </c>
       <c r="C670" t="n">
-        <v>99.705605</v>
+        <v>99.705612</v>
       </c>
     </row>
     <row r="671">
@@ -10787,7 +10790,7 @@
         <v>86.502487</v>
       </c>
       <c r="C671" t="n">
-        <v>99.610382</v>
+        <v>99.610374</v>
       </c>
     </row>
     <row r="672">
@@ -10809,7 +10812,7 @@
         <v>86.187714</v>
       </c>
       <c r="C673" t="n">
-        <v>99.134232</v>
+        <v>99.134224</v>
       </c>
     </row>
     <row r="674">
@@ -10820,7 +10823,7 @@
         <v>86.384445</v>
       </c>
       <c r="C674" t="n">
-        <v>97.896248</v>
+        <v>97.89624</v>
       </c>
     </row>
     <row r="675">
@@ -10842,7 +10845,7 @@
         <v>83.0597</v>
       </c>
       <c r="C676" t="n">
-        <v>96.372559</v>
+        <v>96.372566</v>
       </c>
     </row>
     <row r="677">
@@ -10853,7 +10856,7 @@
         <v>80.659584</v>
       </c>
       <c r="C677" t="n">
-        <v>94.372734</v>
+        <v>94.372742</v>
       </c>
     </row>
     <row r="678">
@@ -10875,7 +10878,7 @@
         <v>81.938332</v>
       </c>
       <c r="C679" t="n">
-        <v>93.563293</v>
+        <v>93.563286</v>
       </c>
     </row>
     <row r="680">
@@ -10930,7 +10933,7 @@
         <v>84.692558</v>
       </c>
       <c r="C684" t="n">
-        <v>94.848885</v>
+        <v>94.848892</v>
       </c>
     </row>
     <row r="685">
@@ -10952,7 +10955,7 @@
         <v>83.453156</v>
       </c>
       <c r="C686" t="n">
-        <v>103.133881</v>
+        <v>103.133888</v>
       </c>
     </row>
     <row r="687">
@@ -10963,7 +10966,7 @@
         <v>85.57785</v>
       </c>
       <c r="C687" t="n">
-        <v>103.133881</v>
+        <v>103.133888</v>
       </c>
     </row>
     <row r="688">
@@ -10996,7 +10999,7 @@
         <v>89.453445</v>
       </c>
       <c r="C690" t="n">
-        <v>103.990952</v>
+        <v>103.990944</v>
       </c>
     </row>
     <row r="691">
@@ -11073,7 +11076,7 @@
         <v>91.401077</v>
       </c>
       <c r="C697" t="n">
-        <v>103.990952</v>
+        <v>103.990944</v>
       </c>
     </row>
     <row r="698">
@@ -11161,7 +11164,7 @@
         <v>84.161385</v>
       </c>
       <c r="C705" t="n">
-        <v>102.372047</v>
+        <v>102.37204</v>
       </c>
     </row>
     <row r="706">
@@ -11205,7 +11208,7 @@
         <v>86.974632</v>
       </c>
       <c r="C709" t="n">
-        <v>111.799789</v>
+        <v>111.799797</v>
       </c>
     </row>
     <row r="710">
@@ -11227,7 +11230,7 @@
         <v>88.627174</v>
       </c>
       <c r="C711" t="n">
-        <v>109.514275</v>
+        <v>109.514282</v>
       </c>
     </row>
     <row r="712">
@@ -11293,7 +11296,7 @@
         <v>102.447502</v>
       </c>
       <c r="C717" t="n">
-        <v>124.274902</v>
+        <v>124.274895</v>
       </c>
     </row>
     <row r="718">
@@ -11304,7 +11307,7 @@
         <v>102.890144</v>
       </c>
       <c r="C718" t="n">
-        <v>126.274734</v>
+        <v>126.274727</v>
       </c>
     </row>
     <row r="719">
@@ -11359,7 +11362,7 @@
         <v>103.234421</v>
       </c>
       <c r="C723" t="n">
-        <v>124.751053</v>
+        <v>124.751045</v>
       </c>
     </row>
     <row r="724">
@@ -11381,7 +11384,7 @@
         <v>102.98851</v>
       </c>
       <c r="C725" t="n">
-        <v>124.751053</v>
+        <v>124.751045</v>
       </c>
     </row>
     <row r="726">
@@ -11425,7 +11428,7 @@
         <v>102.250771</v>
       </c>
       <c r="C729" t="n">
-        <v>124.751053</v>
+        <v>124.751045</v>
       </c>
     </row>
     <row r="730">
@@ -11447,7 +11450,7 @@
         <v>101.513031</v>
       </c>
       <c r="C731" t="n">
-        <v>124.274902</v>
+        <v>124.274895</v>
       </c>
     </row>
     <row r="732">
@@ -11546,7 +11549,7 @@
         <v>94.529091</v>
       </c>
       <c r="C740" t="n">
-        <v>121.608459</v>
+        <v>121.608467</v>
       </c>
     </row>
     <row r="741">
@@ -11579,7 +11582,7 @@
         <v>96.870193</v>
       </c>
       <c r="C743" t="n">
-        <v>124.941498</v>
+        <v>124.941505</v>
       </c>
     </row>
     <row r="744">
@@ -11590,7 +11593,7 @@
         <v>99.742462</v>
       </c>
       <c r="C744" t="n">
-        <v>125.989037</v>
+        <v>125.989044</v>
       </c>
     </row>
     <row r="745">
@@ -11623,7 +11626,7 @@
         <v>99.004723</v>
       </c>
       <c r="C747" t="n">
-        <v>128.084091</v>
+        <v>128.084106</v>
       </c>
     </row>
     <row r="748">
@@ -11656,7 +11659,7 @@
         <v>103.627884</v>
       </c>
       <c r="C750" t="n">
-        <v>128.941147</v>
+        <v>128.941162</v>
       </c>
     </row>
     <row r="751">
@@ -11667,7 +11670,7 @@
         <v>108.054329</v>
       </c>
       <c r="C751" t="n">
-        <v>132.369446</v>
+        <v>132.369431</v>
       </c>
     </row>
     <row r="752">
@@ -11854,7 +11857,7 @@
         <v>103.480339</v>
       </c>
       <c r="C768" t="n">
-        <v>121.608459</v>
+        <v>121.608467</v>
       </c>
     </row>
     <row r="769">
@@ -11865,7 +11868,7 @@
         <v>104.070534</v>
       </c>
       <c r="C769" t="n">
-        <v>123.893982</v>
+        <v>123.89399</v>
       </c>
     </row>
     <row r="770">
@@ -11942,7 +11945,7 @@
         <v>107.955963</v>
       </c>
       <c r="C776" t="n">
-        <v>126.750885</v>
+        <v>126.750877</v>
       </c>
     </row>
     <row r="777">
@@ -11986,7 +11989,7 @@
         <v>110.857735</v>
       </c>
       <c r="C780" t="n">
-        <v>132.369446</v>
+        <v>132.369431</v>
       </c>
     </row>
     <row r="781">
@@ -12019,7 +12022,7 @@
         <v>111.644661</v>
       </c>
       <c r="C783" t="n">
-        <v>132.940826</v>
+        <v>132.940811</v>
       </c>
     </row>
     <row r="784">
@@ -12030,7 +12033,7 @@
         <v>111.447937</v>
       </c>
       <c r="C784" t="n">
-        <v>134.178787</v>
+        <v>134.178802</v>
       </c>
     </row>
     <row r="785">
@@ -12041,7 +12044,7 @@
         <v>112.333221</v>
       </c>
       <c r="C785" t="n">
-        <v>134.940628</v>
+        <v>134.940643</v>
       </c>
     </row>
     <row r="786">
@@ -12052,7 +12055,7 @@
         <v>115.087448</v>
       </c>
       <c r="C786" t="n">
-        <v>135.226334</v>
+        <v>135.226318</v>
       </c>
     </row>
     <row r="787">
@@ -12074,7 +12077,7 @@
         <v>114.595627</v>
       </c>
       <c r="C788" t="n">
-        <v>136.654785</v>
+        <v>136.65477</v>
       </c>
     </row>
     <row r="789">
@@ -12096,7 +12099,7 @@
         <v>116.366203</v>
       </c>
       <c r="C790" t="n">
-        <v>153.319992</v>
+        <v>153.319977</v>
       </c>
     </row>
     <row r="791">
@@ -12107,7 +12110,7 @@
         <v>116.218651</v>
       </c>
       <c r="C791" t="n">
-        <v>152.367691</v>
+        <v>152.367706</v>
       </c>
     </row>
     <row r="792">
@@ -12118,7 +12121,7 @@
         <v>118.82534</v>
       </c>
       <c r="C792" t="n">
-        <v>151.129715</v>
+        <v>151.1297</v>
       </c>
     </row>
     <row r="793">
@@ -12173,7 +12176,7 @@
         <v>120.54673</v>
       </c>
       <c r="C797" t="n">
-        <v>154.938904</v>
+        <v>154.938889</v>
       </c>
     </row>
     <row r="798">
@@ -12184,7 +12187,7 @@
         <v>120.497543</v>
       </c>
       <c r="C798" t="n">
-        <v>154.272293</v>
+        <v>154.272278</v>
       </c>
     </row>
     <row r="799">
@@ -12195,7 +12198,7 @@
         <v>120.349998</v>
       </c>
       <c r="C799" t="n">
-        <v>155.415054</v>
+        <v>155.415039</v>
       </c>
     </row>
     <row r="800">
@@ -12250,7 +12253,7 @@
         <v>118.25</v>
       </c>
       <c r="C804" t="n">
-        <v>155.224594</v>
+        <v>155.224579</v>
       </c>
     </row>
     <row r="805">
@@ -12261,7 +12264,7 @@
         <v>119.300003</v>
       </c>
       <c r="C805" t="n">
-        <v>159.986084</v>
+        <v>159.986069</v>
       </c>
     </row>
     <row r="806">
@@ -14616,6 +14619,17 @@
       </c>
       <c r="C1019" t="n">
         <v>233</v>
+      </c>
+    </row>
+    <row r="1020">
+      <c r="A1020" t="s">
+        <v>1021</v>
+      </c>
+      <c r="B1020" t="n">
+        <v>128.75</v>
+      </c>
+      <c r="C1020" t="n">
+        <v>236.399994</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
kapitel 3 not showing
</commit_message>
<xml_diff>
--- a/Danske aktiekurser.xlsx
+++ b/Danske aktiekurser.xlsx
@@ -3428,10 +3428,10 @@
         <v>3</v>
       </c>
       <c r="B2" t="n">
-        <v>189.887939</v>
+        <v>189.887924</v>
       </c>
       <c r="C2" t="n">
-        <v>191.282898</v>
+        <v>191.282867</v>
       </c>
     </row>
     <row r="3">
@@ -3439,7 +3439,7 @@
         <v>4</v>
       </c>
       <c r="B3" t="n">
-        <v>188.870804</v>
+        <v>188.870819</v>
       </c>
       <c r="C3" t="n">
         <v>190.82489</v>
@@ -3461,7 +3461,7 @@
         <v>6</v>
       </c>
       <c r="B5" t="n">
-        <v>190.74855</v>
+        <v>190.748581</v>
       </c>
       <c r="C5" t="n">
         <v>192.046173</v>
@@ -3472,7 +3472,7 @@
         <v>7</v>
       </c>
       <c r="B6" t="n">
-        <v>191.843903</v>
+        <v>191.843918</v>
       </c>
       <c r="C6" t="n">
         <v>191.74086</v>
@@ -3494,10 +3494,10 @@
         <v>9</v>
       </c>
       <c r="B8" t="n">
-        <v>194.347595</v>
+        <v>194.34758</v>
       </c>
       <c r="C8" t="n">
-        <v>195.404694</v>
+        <v>195.404678</v>
       </c>
     </row>
     <row r="9">
@@ -3519,7 +3519,7 @@
         <v>194.817032</v>
       </c>
       <c r="C10" t="n">
-        <v>195.099365</v>
+        <v>195.09938</v>
       </c>
     </row>
     <row r="11">
@@ -3527,7 +3527,7 @@
         <v>12</v>
       </c>
       <c r="B11" t="n">
-        <v>196.303574</v>
+        <v>196.303589</v>
       </c>
       <c r="C11" t="n">
         <v>193.572784</v>
@@ -3541,7 +3541,7 @@
         <v>195.521179</v>
       </c>
       <c r="C12" t="n">
-        <v>192.504166</v>
+        <v>192.50415</v>
       </c>
     </row>
     <row r="13">
@@ -3549,10 +3549,10 @@
         <v>14</v>
       </c>
       <c r="B13" t="n">
-        <v>195.990616</v>
+        <v>195.990631</v>
       </c>
       <c r="C13" t="n">
-        <v>191.435532</v>
+        <v>191.435547</v>
       </c>
     </row>
     <row r="14">
@@ -3585,7 +3585,7 @@
         <v>193.330475</v>
       </c>
       <c r="C16" t="n">
-        <v>193.114807</v>
+        <v>193.114792</v>
       </c>
     </row>
     <row r="17">
@@ -3593,10 +3593,10 @@
         <v>18</v>
       </c>
       <c r="B17" t="n">
-        <v>192.078644</v>
+        <v>192.078659</v>
       </c>
       <c r="C17" t="n">
-        <v>191.435532</v>
+        <v>191.435547</v>
       </c>
     </row>
     <row r="18">
@@ -3604,7 +3604,7 @@
         <v>19</v>
       </c>
       <c r="B18" t="n">
-        <v>192.078644</v>
+        <v>192.078659</v>
       </c>
       <c r="C18" t="n">
         <v>190.214249</v>
@@ -3615,7 +3615,7 @@
         <v>20</v>
       </c>
       <c r="B19" t="n">
-        <v>186.680099</v>
+        <v>186.680084</v>
       </c>
       <c r="C19" t="n">
         <v>185.63446</v>
@@ -3626,7 +3626,7 @@
         <v>21</v>
       </c>
       <c r="B20" t="n">
-        <v>189.966156</v>
+        <v>189.966171</v>
       </c>
       <c r="C20" t="n">
         <v>187.466385</v>
@@ -3637,7 +3637,7 @@
         <v>22</v>
       </c>
       <c r="B21" t="n">
-        <v>191.843903</v>
+        <v>191.843918</v>
       </c>
       <c r="C21" t="n">
         <v>187.771698</v>
@@ -3648,10 +3648,10 @@
         <v>23</v>
       </c>
       <c r="B22" t="n">
-        <v>189.966156</v>
+        <v>189.966171</v>
       </c>
       <c r="C22" t="n">
-        <v>185.787125</v>
+        <v>185.787109</v>
       </c>
     </row>
     <row r="23">
@@ -3662,7 +3662,7 @@
         <v>190.51384</v>
       </c>
       <c r="C23" t="n">
-        <v>187.008377</v>
+        <v>187.008408</v>
       </c>
     </row>
     <row r="24">
@@ -3684,7 +3684,7 @@
         <v>191.609192</v>
       </c>
       <c r="C25" t="n">
-        <v>187.619034</v>
+        <v>187.619049</v>
       </c>
     </row>
     <row r="26">
@@ -3695,7 +3695,7 @@
         <v>191.609192</v>
       </c>
       <c r="C26" t="n">
-        <v>186.397751</v>
+        <v>186.397766</v>
       </c>
     </row>
     <row r="27">
@@ -3714,10 +3714,10 @@
         <v>29</v>
       </c>
       <c r="B28" t="n">
-        <v>189.262009</v>
+        <v>189.261993</v>
       </c>
       <c r="C28" t="n">
-        <v>188.687653</v>
+        <v>188.687668</v>
       </c>
     </row>
     <row r="29">
@@ -3725,10 +3725,10 @@
         <v>30</v>
       </c>
       <c r="B29" t="n">
-        <v>188.557861</v>
+        <v>188.557846</v>
       </c>
       <c r="C29" t="n">
-        <v>187.161057</v>
+        <v>187.161041</v>
       </c>
     </row>
     <row r="30">
@@ -3739,7 +3739,7 @@
         <v>188.244904</v>
       </c>
       <c r="C30" t="n">
-        <v>185.787125</v>
+        <v>185.787109</v>
       </c>
     </row>
     <row r="31">
@@ -3747,10 +3747,10 @@
         <v>32</v>
       </c>
       <c r="B31" t="n">
-        <v>189.966156</v>
+        <v>189.966171</v>
       </c>
       <c r="C31" t="n">
-        <v>188.687653</v>
+        <v>188.687668</v>
       </c>
     </row>
     <row r="32">
@@ -3761,7 +3761,7 @@
         <v>188.949051</v>
       </c>
       <c r="C32" t="n">
-        <v>188.535004</v>
+        <v>188.534988</v>
       </c>
     </row>
     <row r="33">
@@ -3769,7 +3769,7 @@
         <v>34</v>
       </c>
       <c r="B33" t="n">
-        <v>191.061508</v>
+        <v>191.061523</v>
       </c>
       <c r="C33" t="n">
         <v>193.267456</v>
@@ -3780,7 +3780,7 @@
         <v>35</v>
       </c>
       <c r="B34" t="n">
-        <v>192.313354</v>
+        <v>192.31337</v>
       </c>
       <c r="C34" t="n">
         <v>193.420105</v>
@@ -3791,7 +3791,7 @@
         <v>36</v>
       </c>
       <c r="B35" t="n">
-        <v>194.660568</v>
+        <v>194.660553</v>
       </c>
       <c r="C35" t="n">
         <v>196.625992</v>
@@ -3805,7 +3805,7 @@
         <v>194.895279</v>
       </c>
       <c r="C36" t="n">
-        <v>196.167999</v>
+        <v>196.167984</v>
       </c>
     </row>
     <row r="37">
@@ -3813,10 +3813,10 @@
         <v>38</v>
       </c>
       <c r="B37" t="n">
-        <v>191.687439</v>
+        <v>191.687424</v>
       </c>
       <c r="C37" t="n">
-        <v>185.481812</v>
+        <v>185.481796</v>
       </c>
     </row>
     <row r="38">
@@ -3827,7 +3827,7 @@
         <v>192.861038</v>
       </c>
       <c r="C38" t="n">
-        <v>182.428619</v>
+        <v>182.428604</v>
       </c>
     </row>
     <row r="39">
@@ -3846,10 +3846,10 @@
         <v>41</v>
       </c>
       <c r="B40" t="n">
-        <v>194.504074</v>
+        <v>194.504089</v>
       </c>
       <c r="C40" t="n">
-        <v>186.245117</v>
+        <v>186.245102</v>
       </c>
     </row>
     <row r="41">
@@ -3860,7 +3860,7 @@
         <v>195.677673</v>
       </c>
       <c r="C41" t="n">
-        <v>183.802536</v>
+        <v>183.802551</v>
       </c>
     </row>
     <row r="42">
@@ -3871,7 +3871,7 @@
         <v>189.731445</v>
       </c>
       <c r="C42" t="n">
-        <v>183.191895</v>
+        <v>183.19191</v>
       </c>
     </row>
     <row r="43">
@@ -3879,7 +3879,7 @@
         <v>44</v>
       </c>
       <c r="B43" t="n">
-        <v>192.626297</v>
+        <v>192.626328</v>
       </c>
       <c r="C43" t="n">
         <v>182.733917</v>
@@ -3890,7 +3890,7 @@
         <v>45</v>
       </c>
       <c r="B44" t="n">
-        <v>190.74855</v>
+        <v>190.748581</v>
       </c>
       <c r="C44" t="n">
         <v>181.665298</v>
@@ -3904,7 +3904,7 @@
         <v>189.731445</v>
       </c>
       <c r="C45" t="n">
-        <v>177.696136</v>
+        <v>177.696167</v>
       </c>
     </row>
     <row r="46">
@@ -3934,7 +3934,7 @@
         <v>49</v>
       </c>
       <c r="B48" t="n">
-        <v>191.530945</v>
+        <v>191.53096</v>
       </c>
       <c r="C48" t="n">
         <v>180.749344</v>
@@ -3945,10 +3945,10 @@
         <v>50</v>
       </c>
       <c r="B49" t="n">
-        <v>191.217987</v>
+        <v>191.218002</v>
       </c>
       <c r="C49" t="n">
-        <v>182.428619</v>
+        <v>182.428604</v>
       </c>
     </row>
     <row r="50">
@@ -3956,10 +3956,10 @@
         <v>51</v>
       </c>
       <c r="B50" t="n">
-        <v>192.626297</v>
+        <v>192.626328</v>
       </c>
       <c r="C50" t="n">
-        <v>180.901993</v>
+        <v>180.902008</v>
       </c>
     </row>
     <row r="51">
@@ -3970,7 +3970,7 @@
         <v>193.095764</v>
       </c>
       <c r="C51" t="n">
-        <v>180.291351</v>
+        <v>180.291336</v>
       </c>
     </row>
     <row r="52">
@@ -3992,7 +3992,7 @@
         <v>190.983292</v>
       </c>
       <c r="C53" t="n">
-        <v>180.138687</v>
+        <v>180.138702</v>
       </c>
     </row>
     <row r="54">
@@ -4000,10 +4000,10 @@
         <v>55</v>
       </c>
       <c r="B54" t="n">
-        <v>191.061508</v>
+        <v>191.061523</v>
       </c>
       <c r="C54" t="n">
-        <v>183.113098</v>
+        <v>183.113083</v>
       </c>
     </row>
     <row r="55">
@@ -4014,7 +4014,7 @@
         <v>191.306274</v>
       </c>
       <c r="C55" t="n">
-        <v>182.792419</v>
+        <v>182.792404</v>
       </c>
     </row>
     <row r="56">
@@ -4025,7 +4025,7 @@
         <v>191.795761</v>
       </c>
       <c r="C56" t="n">
-        <v>183.594131</v>
+        <v>183.594116</v>
       </c>
     </row>
     <row r="57">
@@ -4091,7 +4091,7 @@
         <v>183.474533</v>
       </c>
       <c r="C62" t="n">
-        <v>179.585526</v>
+        <v>179.58551</v>
       </c>
     </row>
     <row r="63">
@@ -4124,7 +4124,7 @@
         <v>181.761353</v>
       </c>
       <c r="C65" t="n">
-        <v>176.378632</v>
+        <v>176.378647</v>
       </c>
     </row>
     <row r="66">
@@ -4135,7 +4135,7 @@
         <v>183.882431</v>
       </c>
       <c r="C66" t="n">
-        <v>178.944138</v>
+        <v>178.944153</v>
       </c>
     </row>
     <row r="67">
@@ -4154,10 +4154,10 @@
         <v>69</v>
       </c>
       <c r="B68" t="n">
-        <v>182.985046</v>
+        <v>182.985062</v>
       </c>
       <c r="C68" t="n">
-        <v>180.868271</v>
+        <v>180.868286</v>
       </c>
     </row>
     <row r="69">
@@ -4179,7 +4179,7 @@
         <v>179.477097</v>
       </c>
       <c r="C70" t="n">
-        <v>180.868271</v>
+        <v>180.868286</v>
       </c>
     </row>
     <row r="71">
@@ -4190,7 +4190,7 @@
         <v>180.619217</v>
       </c>
       <c r="C71" t="n">
-        <v>184.395828</v>
+        <v>184.395859</v>
       </c>
     </row>
     <row r="72">
@@ -4198,10 +4198,10 @@
         <v>73</v>
       </c>
       <c r="B72" t="n">
-        <v>180.211304</v>
+        <v>180.211319</v>
       </c>
       <c r="C72" t="n">
-        <v>182.311371</v>
+        <v>182.311386</v>
       </c>
     </row>
     <row r="73">
@@ -4220,7 +4220,7 @@
         <v>75</v>
       </c>
       <c r="B74" t="n">
-        <v>181.9245</v>
+        <v>181.924515</v>
       </c>
       <c r="C74" t="n">
         <v>184.075165</v>
@@ -4234,7 +4234,7 @@
         <v>183.637711</v>
       </c>
       <c r="C75" t="n">
-        <v>188.083755</v>
+        <v>188.083771</v>
       </c>
     </row>
     <row r="76">
@@ -4278,7 +4278,7 @@
         <v>184.127182</v>
       </c>
       <c r="C79" t="n">
-        <v>194.657883</v>
+        <v>194.657867</v>
       </c>
     </row>
     <row r="80">
@@ -4286,10 +4286,10 @@
         <v>81</v>
       </c>
       <c r="B80" t="n">
-        <v>178.498138</v>
+        <v>178.498123</v>
       </c>
       <c r="C80" t="n">
-        <v>187.602753</v>
+        <v>187.602722</v>
       </c>
     </row>
     <row r="81">
@@ -4297,10 +4297,10 @@
         <v>82</v>
       </c>
       <c r="B81" t="n">
-        <v>179.069183</v>
+        <v>179.069199</v>
       </c>
       <c r="C81" t="n">
-        <v>186.319977</v>
+        <v>186.319962</v>
       </c>
     </row>
     <row r="82">
@@ -4311,7 +4311,7 @@
         <v>175.72438</v>
       </c>
       <c r="C82" t="n">
-        <v>183.433792</v>
+        <v>183.433777</v>
       </c>
     </row>
     <row r="83">
@@ -4355,7 +4355,7 @@
         <v>176.132294</v>
       </c>
       <c r="C86" t="n">
-        <v>183.433792</v>
+        <v>183.433777</v>
       </c>
     </row>
     <row r="87">
@@ -4374,7 +4374,7 @@
         <v>89</v>
       </c>
       <c r="B88" t="n">
-        <v>176.784927</v>
+        <v>176.784943</v>
       </c>
       <c r="C88" t="n">
         <v>187.121704</v>
@@ -4421,7 +4421,7 @@
         <v>174.255951</v>
       </c>
       <c r="C92" t="n">
-        <v>183.594131</v>
+        <v>183.594116</v>
       </c>
     </row>
     <row r="93">
@@ -4432,7 +4432,7 @@
         <v>176.540192</v>
       </c>
       <c r="C93" t="n">
-        <v>185.197556</v>
+        <v>185.197571</v>
       </c>
     </row>
     <row r="94">
@@ -4440,7 +4440,7 @@
         <v>95</v>
       </c>
       <c r="B94" t="n">
-        <v>176.458603</v>
+        <v>176.458618</v>
       </c>
       <c r="C94" t="n">
         <v>184.075165</v>
@@ -4473,7 +4473,7 @@
         <v>98</v>
       </c>
       <c r="B97" t="n">
-        <v>173.603302</v>
+        <v>173.603317</v>
       </c>
       <c r="C97" t="n">
         <v>182.632065</v>
@@ -4498,7 +4498,7 @@
         <v>173.113815</v>
       </c>
       <c r="C99" t="n">
-        <v>181.02861</v>
+        <v>181.028625</v>
       </c>
     </row>
     <row r="100">
@@ -4506,7 +4506,7 @@
         <v>101</v>
       </c>
       <c r="B100" t="n">
-        <v>168.953201</v>
+        <v>168.953217</v>
       </c>
       <c r="C100" t="n">
         <v>174.935547</v>
@@ -4520,7 +4520,7 @@
         <v>168.871628</v>
       </c>
       <c r="C101" t="n">
-        <v>175.737274</v>
+        <v>175.737259</v>
       </c>
     </row>
     <row r="102">
@@ -4531,7 +4531,7 @@
         <v>172.461166</v>
       </c>
       <c r="C102" t="n">
-        <v>173.171738</v>
+        <v>173.171753</v>
       </c>
     </row>
     <row r="103">
@@ -4553,7 +4553,7 @@
         <v>178.253387</v>
       </c>
       <c r="C104" t="n">
-        <v>178.944138</v>
+        <v>178.944153</v>
       </c>
     </row>
     <row r="105">
@@ -4586,7 +4586,7 @@
         <v>174.092773</v>
       </c>
       <c r="C107" t="n">
-        <v>175.737274</v>
+        <v>175.737259</v>
       </c>
     </row>
     <row r="108">
@@ -4597,7 +4597,7 @@
         <v>177.84549</v>
       </c>
       <c r="C108" t="n">
-        <v>177.020004</v>
+        <v>177.02002</v>
       </c>
     </row>
     <row r="109">
@@ -4605,7 +4605,7 @@
         <v>110</v>
       </c>
       <c r="B109" t="n">
-        <v>178.498138</v>
+        <v>178.498123</v>
       </c>
       <c r="C109" t="n">
         <v>177.180344</v>
@@ -4619,7 +4619,7 @@
         <v>178.253387</v>
       </c>
       <c r="C110" t="n">
-        <v>177.340683</v>
+        <v>177.340698</v>
       </c>
     </row>
     <row r="111">
@@ -4630,7 +4630,7 @@
         <v>178.742874</v>
       </c>
       <c r="C111" t="n">
-        <v>178.623459</v>
+        <v>178.623444</v>
       </c>
     </row>
     <row r="112">
@@ -4641,7 +4641,7 @@
         <v>177.682327</v>
       </c>
       <c r="C112" t="n">
-        <v>177.821732</v>
+        <v>177.821747</v>
       </c>
     </row>
     <row r="113">
@@ -4652,7 +4652,7 @@
         <v>173.929626</v>
       </c>
       <c r="C113" t="n">
-        <v>175.897598</v>
+        <v>175.897614</v>
       </c>
     </row>
     <row r="114">
@@ -4674,7 +4674,7 @@
         <v>170.258499</v>
       </c>
       <c r="C115" t="n">
-        <v>175.41658</v>
+        <v>175.416565</v>
       </c>
     </row>
     <row r="116">
@@ -4682,10 +4682,10 @@
         <v>117</v>
       </c>
       <c r="B116" t="n">
-        <v>167.811081</v>
+        <v>167.811096</v>
       </c>
       <c r="C116" t="n">
-        <v>173.171738</v>
+        <v>173.171753</v>
       </c>
     </row>
     <row r="117">
@@ -4696,7 +4696,7 @@
         <v>168.626892</v>
       </c>
       <c r="C117" t="n">
-        <v>174.294144</v>
+        <v>174.294159</v>
       </c>
     </row>
     <row r="118">
@@ -4707,7 +4707,7 @@
         <v>166.0979</v>
       </c>
       <c r="C118" t="n">
-        <v>174.294144</v>
+        <v>174.294159</v>
       </c>
     </row>
     <row r="119">
@@ -4740,7 +4740,7 @@
         <v>162.018875</v>
       </c>
       <c r="C121" t="n">
-        <v>174.454514</v>
+        <v>174.454529</v>
       </c>
     </row>
     <row r="122">
@@ -4751,7 +4751,7 @@
         <v>162.957047</v>
       </c>
       <c r="C122" t="n">
-        <v>175.897598</v>
+        <v>175.897614</v>
       </c>
     </row>
     <row r="123">
@@ -4762,7 +4762,7 @@
         <v>162.671509</v>
       </c>
       <c r="C123" t="n">
-        <v>175.41658</v>
+        <v>175.416565</v>
       </c>
     </row>
     <row r="124">
@@ -4806,7 +4806,7 @@
         <v>155.533218</v>
       </c>
       <c r="C127" t="n">
-        <v>177.661377</v>
+        <v>177.661407</v>
       </c>
     </row>
     <row r="128">
@@ -4847,7 +4847,7 @@
         <v>132</v>
       </c>
       <c r="B131" t="n">
-        <v>159.122772</v>
+        <v>159.122757</v>
       </c>
       <c r="C131" t="n">
         <v>183.754471</v>
@@ -4883,7 +4883,7 @@
         <v>159.163544</v>
       </c>
       <c r="C134" t="n">
-        <v>180.707901</v>
+        <v>180.707932</v>
       </c>
     </row>
     <row r="135">
@@ -4891,10 +4891,10 @@
         <v>136</v>
       </c>
       <c r="B135" t="n">
-        <v>144.642227</v>
+        <v>144.642212</v>
       </c>
       <c r="C135" t="n">
-        <v>177.661377</v>
+        <v>177.661407</v>
       </c>
     </row>
     <row r="136">
@@ -4902,10 +4902,10 @@
         <v>137</v>
       </c>
       <c r="B136" t="n">
-        <v>148.394913</v>
+        <v>148.394928</v>
       </c>
       <c r="C136" t="n">
-        <v>179.74588</v>
+        <v>179.745865</v>
       </c>
     </row>
     <row r="137">
@@ -4924,7 +4924,7 @@
         <v>139</v>
       </c>
       <c r="B138" t="n">
-        <v>149.985764</v>
+        <v>149.985748</v>
       </c>
       <c r="C138" t="n">
         <v>181.669998</v>
@@ -4949,7 +4949,7 @@
         <v>150.92392</v>
       </c>
       <c r="C140" t="n">
-        <v>185.518234</v>
+        <v>185.51825</v>
       </c>
     </row>
     <row r="141">
@@ -4960,7 +4960,7 @@
         <v>152.800278</v>
       </c>
       <c r="C141" t="n">
-        <v>186.319977</v>
+        <v>186.319962</v>
       </c>
     </row>
     <row r="142">
@@ -4971,7 +4971,7 @@
         <v>153.208176</v>
       </c>
       <c r="C142" t="n">
-        <v>188.564774</v>
+        <v>188.564789</v>
       </c>
     </row>
     <row r="143">
@@ -4990,7 +4990,7 @@
         <v>145</v>
       </c>
       <c r="B144" t="n">
-        <v>151.127869</v>
+        <v>151.127884</v>
       </c>
       <c r="C144" t="n">
         <v>189.526855</v>
@@ -5004,7 +5004,7 @@
         <v>149.12915</v>
       </c>
       <c r="C145" t="n">
-        <v>188.083755</v>
+        <v>188.083771</v>
       </c>
     </row>
     <row r="146">
@@ -5012,10 +5012,10 @@
         <v>147</v>
       </c>
       <c r="B146" t="n">
-        <v>146.029099</v>
+        <v>146.029083</v>
       </c>
       <c r="C146" t="n">
-        <v>184.395828</v>
+        <v>184.395859</v>
       </c>
     </row>
     <row r="147">
@@ -5089,7 +5089,7 @@
         <v>154</v>
       </c>
       <c r="B153" t="n">
-        <v>150.02652</v>
+        <v>150.026535</v>
       </c>
       <c r="C153" t="n">
         <v>178.302765</v>
@@ -5114,7 +5114,7 @@
         <v>145.906723</v>
       </c>
       <c r="C155" t="n">
-        <v>173.171738</v>
+        <v>173.171753</v>
       </c>
     </row>
     <row r="156">
@@ -5133,7 +5133,7 @@
         <v>158</v>
       </c>
       <c r="B157" t="n">
-        <v>149.210739</v>
+        <v>149.210724</v>
       </c>
       <c r="C157" t="n">
         <v>175.095871</v>
@@ -5144,10 +5144,10 @@
         <v>159</v>
       </c>
       <c r="B158" t="n">
-        <v>150.230469</v>
+        <v>150.230484</v>
       </c>
       <c r="C158" t="n">
-        <v>175.737274</v>
+        <v>175.737259</v>
       </c>
     </row>
     <row r="159">
@@ -5155,10 +5155,10 @@
         <v>160</v>
       </c>
       <c r="B159" t="n">
-        <v>150.719971</v>
+        <v>150.719955</v>
       </c>
       <c r="C159" t="n">
-        <v>177.661377</v>
+        <v>177.661407</v>
       </c>
     </row>
     <row r="160">
@@ -5169,7 +5169,7 @@
         <v>153.616074</v>
       </c>
       <c r="C160" t="n">
-        <v>176.057968</v>
+        <v>176.057953</v>
       </c>
     </row>
     <row r="161">
@@ -5180,7 +5180,7 @@
         <v>151.94368</v>
       </c>
       <c r="C161" t="n">
-        <v>175.897598</v>
+        <v>175.897614</v>
       </c>
     </row>
     <row r="162">
@@ -5188,10 +5188,10 @@
         <v>163</v>
       </c>
       <c r="B162" t="n">
-        <v>154.717422</v>
+        <v>154.717407</v>
       </c>
       <c r="C162" t="n">
-        <v>175.256241</v>
+        <v>175.256226</v>
       </c>
     </row>
     <row r="163">
@@ -5199,10 +5199,10 @@
         <v>164</v>
       </c>
       <c r="B163" t="n">
-        <v>157.817474</v>
+        <v>157.817459</v>
       </c>
       <c r="C163" t="n">
-        <v>175.256241</v>
+        <v>175.256226</v>
       </c>
     </row>
     <row r="164">
@@ -5210,10 +5210,10 @@
         <v>165</v>
       </c>
       <c r="B164" t="n">
-        <v>156.716156</v>
+        <v>156.716141</v>
       </c>
       <c r="C164" t="n">
-        <v>155.614059</v>
+        <v>155.614075</v>
       </c>
     </row>
     <row r="165">
@@ -5224,7 +5224,7 @@
         <v>157.001663</v>
       </c>
       <c r="C165" t="n">
-        <v>153.770096</v>
+        <v>153.770111</v>
       </c>
     </row>
     <row r="166">
@@ -5232,7 +5232,7 @@
         <v>167</v>
       </c>
       <c r="B166" t="n">
-        <v>156.634567</v>
+        <v>156.634552</v>
       </c>
       <c r="C166" t="n">
         <v>151.926132</v>
@@ -5243,10 +5243,10 @@
         <v>168</v>
       </c>
       <c r="B167" t="n">
-        <v>154.146332</v>
+        <v>154.146347</v>
       </c>
       <c r="C167" t="n">
-        <v>150.723557</v>
+        <v>150.723572</v>
       </c>
     </row>
     <row r="168">
@@ -5257,7 +5257,7 @@
         <v>154.309509</v>
       </c>
       <c r="C168" t="n">
-        <v>149.120117</v>
+        <v>149.120102</v>
       </c>
     </row>
     <row r="169">
@@ -5268,7 +5268,7 @@
         <v>144.764603</v>
       </c>
       <c r="C169" t="n">
-        <v>148.398575</v>
+        <v>148.39856</v>
       </c>
     </row>
     <row r="170">
@@ -5287,10 +5287,10 @@
         <v>172</v>
       </c>
       <c r="B171" t="n">
-        <v>150.719971</v>
+        <v>150.719955</v>
       </c>
       <c r="C171" t="n">
-        <v>148.158066</v>
+        <v>148.158051</v>
       </c>
     </row>
     <row r="172">
@@ -5298,7 +5298,7 @@
         <v>173</v>
       </c>
       <c r="B172" t="n">
-        <v>144.397491</v>
+        <v>144.397476</v>
       </c>
       <c r="C172" t="n">
         <v>148.799454</v>
@@ -5320,7 +5320,7 @@
         <v>175</v>
       </c>
       <c r="B174" t="n">
-        <v>139.217133</v>
+        <v>139.217117</v>
       </c>
       <c r="C174" t="n">
         <v>147.837357</v>
@@ -5334,7 +5334,7 @@
         <v>137.096039</v>
       </c>
       <c r="C175" t="n">
-        <v>148.398575</v>
+        <v>148.39856</v>
       </c>
     </row>
     <row r="176">
@@ -5345,7 +5345,7 @@
         <v>140.114502</v>
       </c>
       <c r="C176" t="n">
-        <v>148.879608</v>
+        <v>148.879593</v>
       </c>
     </row>
     <row r="177">
@@ -5378,7 +5378,7 @@
         <v>142.643509</v>
       </c>
       <c r="C179" t="n">
-        <v>148.398575</v>
+        <v>148.39856</v>
       </c>
     </row>
     <row r="180">
@@ -5397,10 +5397,10 @@
         <v>182</v>
       </c>
       <c r="B181" t="n">
-        <v>144.397491</v>
+        <v>144.397476</v>
       </c>
       <c r="C181" t="n">
-        <v>151.284744</v>
+        <v>151.28476</v>
       </c>
     </row>
     <row r="182">
@@ -5430,7 +5430,7 @@
         <v>185</v>
       </c>
       <c r="B184" t="n">
-        <v>138.686844</v>
+        <v>138.686859</v>
       </c>
       <c r="C184" t="n">
         <v>152.968384</v>
@@ -5463,7 +5463,7 @@
         <v>188</v>
       </c>
       <c r="B187" t="n">
-        <v>137.626297</v>
+        <v>137.626312</v>
       </c>
       <c r="C187" t="n">
         <v>151.525284</v>
@@ -5477,7 +5477,7 @@
         <v>138.238144</v>
       </c>
       <c r="C188" t="n">
-        <v>152.647705</v>
+        <v>152.647675</v>
       </c>
     </row>
     <row r="189">
@@ -5496,7 +5496,7 @@
         <v>191</v>
       </c>
       <c r="B190" t="n">
-        <v>135.627563</v>
+        <v>135.627579</v>
       </c>
       <c r="C190" t="n">
         <v>149.440796</v>
@@ -5507,10 +5507,10 @@
         <v>192</v>
       </c>
       <c r="B191" t="n">
-        <v>129.386673</v>
+        <v>129.386688</v>
       </c>
       <c r="C191" t="n">
-        <v>148.158066</v>
+        <v>148.158051</v>
       </c>
     </row>
     <row r="192">
@@ -5518,7 +5518,7 @@
         <v>193</v>
       </c>
       <c r="B192" t="n">
-        <v>121.310196</v>
+        <v>121.310188</v>
       </c>
       <c r="C192" t="n">
         <v>150.483032</v>
@@ -5529,7 +5529,7 @@
         <v>194</v>
       </c>
       <c r="B193" t="n">
-        <v>116.945648</v>
+        <v>116.945656</v>
       </c>
       <c r="C193" t="n">
         <v>146.795135</v>
@@ -5543,7 +5543,7 @@
         <v>115.925896</v>
       </c>
       <c r="C194" t="n">
-        <v>141.824463</v>
+        <v>141.824448</v>
       </c>
     </row>
     <row r="195">
@@ -5562,7 +5562,7 @@
         <v>197</v>
       </c>
       <c r="B196" t="n">
-        <v>115.191658</v>
+        <v>115.191666</v>
       </c>
       <c r="C196" t="n">
         <v>140.782227</v>
@@ -5573,10 +5573,10 @@
         <v>198</v>
       </c>
       <c r="B197" t="n">
-        <v>115.273254</v>
+        <v>115.273247</v>
       </c>
       <c r="C197" t="n">
-        <v>141.904617</v>
+        <v>141.904633</v>
       </c>
     </row>
     <row r="198">
@@ -5584,7 +5584,7 @@
         <v>199</v>
       </c>
       <c r="B198" t="n">
-        <v>113.886383</v>
+        <v>113.886375</v>
       </c>
       <c r="C198" t="n">
         <v>142.546005</v>
@@ -5595,7 +5595,7 @@
         <v>200</v>
       </c>
       <c r="B199" t="n">
-        <v>115.436401</v>
+        <v>115.436417</v>
       </c>
       <c r="C199" t="n">
         <v>143.588242</v>
@@ -5606,7 +5606,7 @@
         <v>201</v>
       </c>
       <c r="B200" t="n">
-        <v>112.254768</v>
+        <v>112.254776</v>
       </c>
       <c r="C200" t="n">
         <v>143.748581</v>
@@ -5628,7 +5628,7 @@
         <v>203</v>
       </c>
       <c r="B202" t="n">
-        <v>107.033607</v>
+        <v>107.033615</v>
       </c>
       <c r="C202" t="n">
         <v>142.706345</v>
@@ -5642,7 +5642,7 @@
         <v>106.421753</v>
       </c>
       <c r="C203" t="n">
-        <v>139.820145</v>
+        <v>139.820129</v>
       </c>
     </row>
     <row r="204">
@@ -5650,7 +5650,7 @@
         <v>205</v>
       </c>
       <c r="B204" t="n">
-        <v>103.280907</v>
+        <v>103.280914</v>
       </c>
       <c r="C204" t="n">
         <v>140.782227</v>
@@ -5661,7 +5661,7 @@
         <v>206</v>
       </c>
       <c r="B205" t="n">
-        <v>102.50589</v>
+        <v>102.505898</v>
       </c>
       <c r="C205" t="n">
         <v>141.503769</v>
@@ -5675,7 +5675,7 @@
         <v>103.076958</v>
       </c>
       <c r="C206" t="n">
-        <v>142.064972</v>
+        <v>142.064987</v>
       </c>
     </row>
     <row r="207">
@@ -5686,7 +5686,7 @@
         <v>102.791428</v>
       </c>
       <c r="C207" t="n">
-        <v>140.862381</v>
+        <v>140.862396</v>
       </c>
     </row>
     <row r="208">
@@ -5694,7 +5694,7 @@
         <v>209</v>
       </c>
       <c r="B208" t="n">
-        <v>104.586197</v>
+        <v>104.586189</v>
       </c>
       <c r="C208" t="n">
         <v>144.069275</v>
@@ -5705,10 +5705,10 @@
         <v>210</v>
       </c>
       <c r="B209" t="n">
-        <v>103.280907</v>
+        <v>103.280914</v>
       </c>
       <c r="C209" t="n">
-        <v>139.90033</v>
+        <v>139.900345</v>
       </c>
     </row>
     <row r="210">
@@ -5719,7 +5719,7 @@
         <v>103.076958</v>
       </c>
       <c r="C210" t="n">
-        <v>122.102119</v>
+        <v>122.102127</v>
       </c>
     </row>
     <row r="211">
@@ -5730,7 +5730,7 @@
         <v>108.134956</v>
       </c>
       <c r="C211" t="n">
-        <v>123.625374</v>
+        <v>123.625389</v>
       </c>
     </row>
     <row r="212">
@@ -5738,10 +5738,10 @@
         <v>213</v>
       </c>
       <c r="B212" t="n">
-        <v>111.765282</v>
+        <v>111.765274</v>
       </c>
       <c r="C212" t="n">
-        <v>127.874504</v>
+        <v>127.874519</v>
       </c>
     </row>
     <row r="213">
@@ -5749,7 +5749,7 @@
         <v>214</v>
       </c>
       <c r="B213" t="n">
-        <v>110.337616</v>
+        <v>110.337624</v>
       </c>
       <c r="C213" t="n">
         <v>130.199493</v>
@@ -5763,7 +5763,7 @@
         <v>110.174461</v>
       </c>
       <c r="C214" t="n">
-        <v>130.680527</v>
+        <v>130.680542</v>
       </c>
     </row>
     <row r="215">
@@ -5771,10 +5771,10 @@
         <v>216</v>
       </c>
       <c r="B215" t="n">
-        <v>117.516708</v>
+        <v>117.516716</v>
       </c>
       <c r="C215" t="n">
-        <v>132.524475</v>
+        <v>132.52449</v>
       </c>
     </row>
     <row r="216">
@@ -5782,7 +5782,7 @@
         <v>217</v>
       </c>
       <c r="B216" t="n">
-        <v>117.027222</v>
+        <v>117.027229</v>
       </c>
       <c r="C216" t="n">
         <v>133.326218</v>
@@ -5804,7 +5804,7 @@
         <v>219</v>
       </c>
       <c r="B218" t="n">
-        <v>116.619324</v>
+        <v>116.619316</v>
       </c>
       <c r="C218" t="n">
         <v>130.440018</v>
@@ -5815,7 +5815,7 @@
         <v>220</v>
       </c>
       <c r="B219" t="n">
-        <v>115.028503</v>
+        <v>115.028496</v>
       </c>
       <c r="C219" t="n">
         <v>129.798645</v>
@@ -5840,7 +5840,7 @@
         <v>113.519257</v>
       </c>
       <c r="C221" t="n">
-        <v>127.874504</v>
+        <v>127.874519</v>
       </c>
     </row>
     <row r="222">
@@ -5848,7 +5848,7 @@
         <v>223</v>
       </c>
       <c r="B222" t="n">
-        <v>111.602119</v>
+        <v>111.602127</v>
       </c>
       <c r="C222" t="n">
         <v>127.553825</v>
@@ -5859,10 +5859,10 @@
         <v>224</v>
       </c>
       <c r="B223" t="n">
-        <v>110.500778</v>
+        <v>110.500786</v>
       </c>
       <c r="C223" t="n">
-        <v>128.756424</v>
+        <v>128.756409</v>
       </c>
     </row>
     <row r="224">
@@ -5873,7 +5873,7 @@
         <v>106.544136</v>
       </c>
       <c r="C224" t="n">
-        <v>125.950378</v>
+        <v>125.950386</v>
       </c>
     </row>
     <row r="225">
@@ -5881,10 +5881,10 @@
         <v>226</v>
       </c>
       <c r="B225" t="n">
-        <v>107.441521</v>
+        <v>107.441513</v>
       </c>
       <c r="C225" t="n">
-        <v>127.874504</v>
+        <v>127.874519</v>
       </c>
     </row>
     <row r="226">
@@ -5895,7 +5895,7 @@
         <v>108.461266</v>
       </c>
       <c r="C226" t="n">
-        <v>127.874504</v>
+        <v>127.874519</v>
       </c>
     </row>
     <row r="227">
@@ -5903,10 +5903,10 @@
         <v>228</v>
       </c>
       <c r="B227" t="n">
-        <v>108.869171</v>
+        <v>108.869164</v>
       </c>
       <c r="C227" t="n">
-        <v>128.275375</v>
+        <v>128.27536</v>
       </c>
     </row>
     <row r="228">
@@ -5914,10 +5914,10 @@
         <v>229</v>
       </c>
       <c r="B228" t="n">
-        <v>111.071846</v>
+        <v>111.071838</v>
       </c>
       <c r="C228" t="n">
-        <v>131.081406</v>
+        <v>131.08139</v>
       </c>
     </row>
     <row r="229">
@@ -5925,10 +5925,10 @@
         <v>230</v>
       </c>
       <c r="B229" t="n">
-        <v>110.133675</v>
+        <v>110.133667</v>
       </c>
       <c r="C229" t="n">
-        <v>131.081406</v>
+        <v>131.08139</v>
       </c>
     </row>
     <row r="230">
@@ -5947,7 +5947,7 @@
         <v>232</v>
       </c>
       <c r="B231" t="n">
-        <v>107.441521</v>
+        <v>107.441513</v>
       </c>
       <c r="C231" t="n">
         <v>130.359848</v>
@@ -5958,7 +5958,7 @@
         <v>233</v>
       </c>
       <c r="B232" t="n">
-        <v>107.19677</v>
+        <v>107.196777</v>
       </c>
       <c r="C232" t="n">
         <v>130.359848</v>
@@ -5969,10 +5969,10 @@
         <v>234</v>
       </c>
       <c r="B233" t="n">
-        <v>108.706009</v>
+        <v>108.706017</v>
       </c>
       <c r="C233" t="n">
-        <v>126.671928</v>
+        <v>126.671936</v>
       </c>
     </row>
     <row r="234">
@@ -5980,10 +5980,10 @@
         <v>235</v>
       </c>
       <c r="B234" t="n">
-        <v>108.583649</v>
+        <v>108.583641</v>
       </c>
       <c r="C234" t="n">
-        <v>127.152969</v>
+        <v>127.152977</v>
       </c>
     </row>
     <row r="235">
@@ -5991,7 +5991,7 @@
         <v>236</v>
       </c>
       <c r="B235" t="n">
-        <v>114.620598</v>
+        <v>114.620605</v>
       </c>
       <c r="C235" t="n">
         <v>129.798645</v>
@@ -6002,10 +6002,10 @@
         <v>237</v>
       </c>
       <c r="B236" t="n">
-        <v>111.316582</v>
+        <v>111.316589</v>
       </c>
       <c r="C236" t="n">
-        <v>126.992615</v>
+        <v>126.992592</v>
       </c>
     </row>
     <row r="237">
@@ -6024,10 +6024,10 @@
         <v>239</v>
       </c>
       <c r="B238" t="n">
-        <v>112.050819</v>
+        <v>112.050812</v>
       </c>
       <c r="C238" t="n">
-        <v>127.152969</v>
+        <v>127.152977</v>
       </c>
     </row>
     <row r="239">
@@ -6057,7 +6057,7 @@
         <v>242</v>
       </c>
       <c r="B241" t="n">
-        <v>113.396896</v>
+        <v>113.396889</v>
       </c>
       <c r="C241" t="n">
         <v>128.676224</v>
@@ -6079,7 +6079,7 @@
         <v>244</v>
       </c>
       <c r="B243" t="n">
-        <v>110.459991</v>
+        <v>110.459984</v>
       </c>
       <c r="C243" t="n">
         <v>127.633987</v>
@@ -6090,10 +6090,10 @@
         <v>245</v>
       </c>
       <c r="B244" t="n">
-        <v>112.213974</v>
+        <v>112.213982</v>
       </c>
       <c r="C244" t="n">
-        <v>122.66333</v>
+        <v>122.663322</v>
       </c>
     </row>
     <row r="245">
@@ -6104,7 +6104,7 @@
         <v>109.725769</v>
       </c>
       <c r="C245" t="n">
-        <v>121.781418</v>
+        <v>121.781425</v>
       </c>
     </row>
     <row r="246">
@@ -6112,10 +6112,10 @@
         <v>247</v>
       </c>
       <c r="B246" t="n">
-        <v>105.442787</v>
+        <v>105.442795</v>
       </c>
       <c r="C246" t="n">
-        <v>117.77282</v>
+        <v>117.772827</v>
       </c>
     </row>
     <row r="247">
@@ -6126,7 +6126,7 @@
         <v>104.626984</v>
       </c>
       <c r="C247" t="n">
-        <v>120.258148</v>
+        <v>120.258163</v>
       </c>
     </row>
     <row r="248">
@@ -6137,7 +6137,7 @@
         <v>102.95459</v>
       </c>
       <c r="C248" t="n">
-        <v>120.819366</v>
+        <v>120.819351</v>
       </c>
     </row>
     <row r="249">
@@ -6148,7 +6148,7 @@
         <v>105.157257</v>
       </c>
       <c r="C249" t="n">
-        <v>124.346931</v>
+        <v>124.346947</v>
       </c>
     </row>
     <row r="250">
@@ -6156,10 +6156,10 @@
         <v>251</v>
       </c>
       <c r="B250" t="n">
-        <v>104.994102</v>
+        <v>104.994095</v>
       </c>
       <c r="C250" t="n">
-        <v>126.271072</v>
+        <v>126.271049</v>
       </c>
     </row>
     <row r="251">
@@ -6167,10 +6167,10 @@
         <v>252</v>
       </c>
       <c r="B251" t="n">
-        <v>104.749359</v>
+        <v>104.749352</v>
       </c>
       <c r="C251" t="n">
-        <v>123.865906</v>
+        <v>123.865921</v>
       </c>
     </row>
     <row r="252">
@@ -6178,10 +6178,10 @@
         <v>253</v>
       </c>
       <c r="B252" t="n">
-        <v>109.195496</v>
+        <v>109.195503</v>
       </c>
       <c r="C252" t="n">
-        <v>127.313293</v>
+        <v>127.313301</v>
       </c>
     </row>
     <row r="253">
@@ -6200,10 +6200,10 @@
         <v>255</v>
       </c>
       <c r="B254" t="n">
-        <v>108.379692</v>
+        <v>108.3797</v>
       </c>
       <c r="C254" t="n">
-        <v>126.832275</v>
+        <v>126.832268</v>
       </c>
     </row>
     <row r="255">
@@ -6214,7 +6214,7 @@
         <v>107.074402</v>
       </c>
       <c r="C255" t="n">
-        <v>126.431412</v>
+        <v>126.431419</v>
       </c>
     </row>
     <row r="256">
@@ -6222,7 +6222,7 @@
         <v>257</v>
       </c>
       <c r="B256" t="n">
-        <v>104.219093</v>
+        <v>104.219086</v>
       </c>
       <c r="C256" t="n">
         <v>126.591751</v>
@@ -6244,7 +6244,7 @@
         <v>259</v>
       </c>
       <c r="B258" t="n">
-        <v>106.054642</v>
+        <v>106.054649</v>
       </c>
       <c r="C258" t="n">
         <v>124.266769</v>
@@ -6255,10 +6255,10 @@
         <v>260</v>
       </c>
       <c r="B259" t="n">
-        <v>104.423035</v>
+        <v>104.423042</v>
       </c>
       <c r="C259" t="n">
-        <v>122.583153</v>
+        <v>122.583145</v>
       </c>
     </row>
     <row r="260">
@@ -6266,10 +6266,10 @@
         <v>261</v>
       </c>
       <c r="B260" t="n">
-        <v>105.034897</v>
+        <v>105.034889</v>
       </c>
       <c r="C260" t="n">
-        <v>126.271072</v>
+        <v>126.271049</v>
       </c>
     </row>
     <row r="261">
@@ -6280,7 +6280,7 @@
         <v>103.933556</v>
       </c>
       <c r="C261" t="n">
-        <v>126.030556</v>
+        <v>126.030548</v>
       </c>
     </row>
     <row r="262">
@@ -6288,10 +6288,10 @@
         <v>263</v>
       </c>
       <c r="B262" t="n">
-        <v>103.199326</v>
+        <v>103.199333</v>
       </c>
       <c r="C262" t="n">
-        <v>125.870201</v>
+        <v>125.870209</v>
       </c>
     </row>
     <row r="263">
@@ -6324,7 +6324,7 @@
         <v>101.975624</v>
       </c>
       <c r="C265" t="n">
-        <v>126.190895</v>
+        <v>126.190887</v>
       </c>
     </row>
     <row r="266">
@@ -6332,10 +6332,10 @@
         <v>267</v>
       </c>
       <c r="B266" t="n">
-        <v>99.976906</v>
+        <v>99.976898</v>
       </c>
       <c r="C266" t="n">
-        <v>126.110733</v>
+        <v>126.110725</v>
       </c>
     </row>
     <row r="267">
@@ -6346,7 +6346,7 @@
         <v>102.138779</v>
       </c>
       <c r="C267" t="n">
-        <v>126.832275</v>
+        <v>126.832268</v>
       </c>
     </row>
     <row r="268">
@@ -6354,10 +6354,10 @@
         <v>269</v>
       </c>
       <c r="B268" t="n">
-        <v>99.936111</v>
+        <v>99.936104</v>
       </c>
       <c r="C268" t="n">
-        <v>123.625374</v>
+        <v>123.625389</v>
       </c>
     </row>
     <row r="269">
@@ -6368,7 +6368,7 @@
         <v>99.85453</v>
       </c>
       <c r="C269" t="n">
-        <v>123.46505</v>
+        <v>123.465034</v>
       </c>
     </row>
     <row r="270">
@@ -6379,7 +6379,7 @@
         <v>100.140068</v>
       </c>
       <c r="C270" t="n">
-        <v>123.144371</v>
+        <v>123.144379</v>
       </c>
     </row>
     <row r="271">
@@ -6390,7 +6390,7 @@
         <v>98.304497</v>
       </c>
       <c r="C271" t="n">
-        <v>120.739197</v>
+        <v>120.739204</v>
       </c>
     </row>
     <row r="272">
@@ -6401,7 +6401,7 @@
         <v>103.444077</v>
       </c>
       <c r="C272" t="n">
-        <v>121.781418</v>
+        <v>121.781425</v>
       </c>
     </row>
     <row r="273">
@@ -6409,10 +6409,10 @@
         <v>274</v>
       </c>
       <c r="B273" t="n">
-        <v>101.078232</v>
+        <v>101.078239</v>
       </c>
       <c r="C273" t="n">
-        <v>122.262466</v>
+        <v>122.262451</v>
       </c>
     </row>
     <row r="274">
@@ -6420,10 +6420,10 @@
         <v>275</v>
       </c>
       <c r="B274" t="n">
-        <v>103.199326</v>
+        <v>103.199333</v>
       </c>
       <c r="C274" t="n">
-        <v>122.102119</v>
+        <v>122.102127</v>
       </c>
     </row>
     <row r="275">
@@ -6431,10 +6431,10 @@
         <v>276</v>
       </c>
       <c r="B275" t="n">
-        <v>102.669052</v>
+        <v>102.66906</v>
       </c>
       <c r="C275" t="n">
-        <v>121.781418</v>
+        <v>121.781425</v>
       </c>
     </row>
     <row r="276">
@@ -6445,7 +6445,7 @@
         <v>101.975624</v>
       </c>
       <c r="C276" t="n">
-        <v>120.338333</v>
+        <v>120.338341</v>
       </c>
     </row>
     <row r="277">
@@ -6456,7 +6456,7 @@
         <v>97.896599</v>
       </c>
       <c r="C277" t="n">
-        <v>119.456451</v>
+        <v>119.456436</v>
       </c>
     </row>
     <row r="278">
@@ -6478,7 +6478,7 @@
         <v>101.119026</v>
       </c>
       <c r="C279" t="n">
-        <v>121.220222</v>
+        <v>121.22023</v>
       </c>
     </row>
     <row r="280">
@@ -6489,7 +6489,7 @@
         <v>100.180855</v>
       </c>
       <c r="C280" t="n">
-        <v>122.262466</v>
+        <v>122.262451</v>
       </c>
     </row>
     <row r="281">
@@ -6497,10 +6497,10 @@
         <v>282</v>
       </c>
       <c r="B281" t="n">
-        <v>99.936111</v>
+        <v>99.936104</v>
       </c>
       <c r="C281" t="n">
-        <v>121.220222</v>
+        <v>121.22023</v>
       </c>
     </row>
     <row r="282">
@@ -6508,10 +6508,10 @@
         <v>283</v>
       </c>
       <c r="B282" t="n">
-        <v>101.486145</v>
+        <v>101.486137</v>
       </c>
       <c r="C282" t="n">
-        <v>122.02195</v>
+        <v>122.021935</v>
       </c>
     </row>
     <row r="283">
@@ -6522,7 +6522,7 @@
         <v>103.321701</v>
       </c>
       <c r="C283" t="n">
-        <v>123.545219</v>
+        <v>123.545227</v>
       </c>
     </row>
     <row r="284">
@@ -6533,7 +6533,7 @@
         <v>102.873009</v>
       </c>
       <c r="C284" t="n">
-        <v>121.540916</v>
+        <v>121.540909</v>
       </c>
     </row>
     <row r="285">
@@ -6541,10 +6541,10 @@
         <v>286</v>
       </c>
       <c r="B285" t="n">
-        <v>103.117752</v>
+        <v>103.117744</v>
       </c>
       <c r="C285" t="n">
-        <v>121.781418</v>
+        <v>121.781425</v>
       </c>
     </row>
     <row r="286">
@@ -6555,7 +6555,7 @@
         <v>98.712402</v>
       </c>
       <c r="C286" t="n">
-        <v>120.49868</v>
+        <v>120.498688</v>
       </c>
     </row>
     <row r="287">
@@ -6563,10 +6563,10 @@
         <v>288</v>
       </c>
       <c r="B287" t="n">
-        <v>98.467651</v>
+        <v>98.467667</v>
       </c>
       <c r="C287" t="n">
-        <v>120.57885</v>
+        <v>120.578835</v>
       </c>
     </row>
     <row r="288">
@@ -6577,7 +6577,7 @@
         <v>102.301949</v>
       </c>
       <c r="C288" t="n">
-        <v>121.781418</v>
+        <v>121.781425</v>
       </c>
     </row>
     <row r="289">
@@ -6585,10 +6585,10 @@
         <v>290</v>
       </c>
       <c r="B289" t="n">
-        <v>102.22036</v>
+        <v>102.220367</v>
       </c>
       <c r="C289" t="n">
-        <v>119.777115</v>
+        <v>119.77713</v>
       </c>
     </row>
     <row r="290">
@@ -6596,10 +6596,10 @@
         <v>291</v>
       </c>
       <c r="B290" t="n">
-        <v>106.054642</v>
+        <v>106.054649</v>
       </c>
       <c r="C290" t="n">
-        <v>127.393456</v>
+        <v>127.393478</v>
       </c>
     </row>
     <row r="291">
@@ -6632,7 +6632,7 @@
         <v>105.687538</v>
       </c>
       <c r="C293" t="n">
-        <v>122.422813</v>
+        <v>122.422821</v>
       </c>
     </row>
     <row r="294">
@@ -6640,10 +6640,10 @@
         <v>295</v>
       </c>
       <c r="B294" t="n">
-        <v>104.830948</v>
+        <v>104.83094</v>
       </c>
       <c r="C294" t="n">
-        <v>121.059875</v>
+        <v>121.059883</v>
       </c>
     </row>
     <row r="295">
@@ -6651,10 +6651,10 @@
         <v>296</v>
       </c>
       <c r="B295" t="n">
-        <v>105.442787</v>
+        <v>105.442795</v>
       </c>
       <c r="C295" t="n">
-        <v>119.616783</v>
+        <v>119.616776</v>
       </c>
     </row>
     <row r="296">
@@ -6662,7 +6662,7 @@
         <v>297</v>
       </c>
       <c r="B296" t="n">
-        <v>104.137505</v>
+        <v>104.137512</v>
       </c>
       <c r="C296" t="n">
         <v>117.69265</v>
@@ -6673,10 +6673,10 @@
         <v>298</v>
       </c>
       <c r="B297" t="n">
-        <v>103.036163</v>
+        <v>103.036171</v>
       </c>
       <c r="C297" t="n">
-        <v>116.570229</v>
+        <v>116.570236</v>
       </c>
     </row>
     <row r="298">
@@ -6684,7 +6684,7 @@
         <v>299</v>
       </c>
       <c r="B298" t="n">
-        <v>103.892761</v>
+        <v>103.892769</v>
       </c>
       <c r="C298" t="n">
         <v>115.768517</v>
@@ -6698,7 +6698,7 @@
         <v>104.463829</v>
       </c>
       <c r="C299" t="n">
-        <v>117.933182</v>
+        <v>117.933174</v>
       </c>
     </row>
     <row r="300">
@@ -6706,7 +6706,7 @@
         <v>301</v>
       </c>
       <c r="B300" t="n">
-        <v>105.361214</v>
+        <v>105.361206</v>
       </c>
       <c r="C300" t="n">
         <v>118.013336</v>
@@ -6720,7 +6720,7 @@
         <v>107.971802</v>
       </c>
       <c r="C301" t="n">
-        <v>118.654724</v>
+        <v>118.654716</v>
       </c>
     </row>
     <row r="302">
@@ -6728,10 +6728,10 @@
         <v>303</v>
       </c>
       <c r="B302" t="n">
-        <v>108.706009</v>
+        <v>108.706017</v>
       </c>
       <c r="C302" t="n">
-        <v>120.258148</v>
+        <v>120.258163</v>
       </c>
     </row>
     <row r="303">
@@ -6742,7 +6742,7 @@
         <v>109.481026</v>
       </c>
       <c r="C303" t="n">
-        <v>122.102119</v>
+        <v>122.102127</v>
       </c>
     </row>
     <row r="304">
@@ -6775,7 +6775,7 @@
         <v>108.000374</v>
       </c>
       <c r="C306" t="n">
-        <v>120.899544</v>
+        <v>120.899529</v>
       </c>
     </row>
     <row r="307">
@@ -6786,7 +6786,7 @@
         <v>105.866501</v>
       </c>
       <c r="C307" t="n">
-        <v>120.096039</v>
+        <v>120.096046</v>
       </c>
     </row>
     <row r="308">
@@ -6805,7 +6805,7 @@
         <v>310</v>
       </c>
       <c r="B309" t="n">
-        <v>105.039078</v>
+        <v>105.03907</v>
       </c>
       <c r="C309" t="n">
         <v>114.540001</v>
@@ -6816,7 +6816,7 @@
         <v>311</v>
       </c>
       <c r="B310" t="n">
-        <v>105.474556</v>
+        <v>105.474564</v>
       </c>
       <c r="C310" t="n">
         <v>116.762421</v>
@@ -6827,10 +6827,10 @@
         <v>312</v>
       </c>
       <c r="B311" t="n">
-        <v>101.685844</v>
+        <v>101.685837</v>
       </c>
       <c r="C311" t="n">
-        <v>117.104324</v>
+        <v>117.104317</v>
       </c>
     </row>
     <row r="312">
@@ -6841,7 +6841,7 @@
         <v>101.729393</v>
       </c>
       <c r="C312" t="n">
-        <v>117.959106</v>
+        <v>117.959099</v>
       </c>
     </row>
     <row r="313">
@@ -6852,7 +6852,7 @@
         <v>106.066818</v>
       </c>
       <c r="C313" t="n">
-        <v>121.121765</v>
+        <v>121.12178</v>
       </c>
     </row>
     <row r="314">
@@ -6863,7 +6863,7 @@
         <v>106.737473</v>
       </c>
       <c r="C314" t="n">
-        <v>121.463684</v>
+        <v>121.463692</v>
       </c>
     </row>
     <row r="315">
@@ -6885,7 +6885,7 @@
         <v>109.132637</v>
       </c>
       <c r="C316" t="n">
-        <v>122.745865</v>
+        <v>122.745857</v>
       </c>
     </row>
     <row r="317">
@@ -6907,7 +6907,7 @@
         <v>107.347145</v>
       </c>
       <c r="C318" t="n">
-        <v>122.062027</v>
+        <v>122.062035</v>
       </c>
     </row>
     <row r="319">
@@ -6918,7 +6918,7 @@
         <v>106.389084</v>
       </c>
       <c r="C319" t="n">
-        <v>120.52343</v>
+        <v>120.523438</v>
       </c>
     </row>
     <row r="320">
@@ -6926,7 +6926,7 @@
         <v>321</v>
       </c>
       <c r="B320" t="n">
-        <v>105.953598</v>
+        <v>105.95359</v>
       </c>
       <c r="C320" t="n">
         <v>120.352478</v>
@@ -6937,10 +6937,10 @@
         <v>322</v>
       </c>
       <c r="B321" t="n">
-        <v>108.131027</v>
+        <v>108.13102</v>
       </c>
       <c r="C321" t="n">
-        <v>122.232986</v>
+        <v>122.232979</v>
       </c>
     </row>
     <row r="322">
@@ -6951,7 +6951,7 @@
         <v>110.613289</v>
       </c>
       <c r="C322" t="n">
-        <v>123.515152</v>
+        <v>123.515144</v>
       </c>
     </row>
     <row r="323">
@@ -6984,7 +6984,7 @@
         <v>112.268127</v>
       </c>
       <c r="C325" t="n">
-        <v>124.968254</v>
+        <v>124.968269</v>
       </c>
     </row>
     <row r="326">
@@ -6995,7 +6995,7 @@
         <v>110.87458</v>
       </c>
       <c r="C326" t="n">
-        <v>123.429672</v>
+        <v>123.429657</v>
       </c>
     </row>
     <row r="327">
@@ -7006,7 +7006,7 @@
         <v>110.831032</v>
       </c>
       <c r="C327" t="n">
-        <v>122.062027</v>
+        <v>122.062035</v>
       </c>
     </row>
     <row r="328">
@@ -7017,7 +7017,7 @@
         <v>110.221359</v>
       </c>
       <c r="C328" t="n">
-        <v>119.412231</v>
+        <v>119.412224</v>
       </c>
     </row>
     <row r="329">
@@ -7028,7 +7028,7 @@
         <v>111.919746</v>
       </c>
       <c r="C329" t="n">
-        <v>122.916809</v>
+        <v>122.916817</v>
       </c>
     </row>
     <row r="330">
@@ -7036,7 +7036,7 @@
         <v>331</v>
       </c>
       <c r="B330" t="n">
-        <v>113.705238</v>
+        <v>113.705231</v>
       </c>
       <c r="C330" t="n">
         <v>123.942535</v>
@@ -7047,10 +7047,10 @@
         <v>332</v>
       </c>
       <c r="B331" t="n">
-        <v>102.8181</v>
+        <v>102.818108</v>
       </c>
       <c r="C331" t="n">
-        <v>122.831329</v>
+        <v>122.831322</v>
       </c>
     </row>
     <row r="332">
@@ -7061,7 +7061,7 @@
         <v>103.993912</v>
       </c>
       <c r="C332" t="n">
-        <v>120.779861</v>
+        <v>120.779869</v>
       </c>
     </row>
     <row r="333">
@@ -7069,7 +7069,7 @@
         <v>334</v>
       </c>
       <c r="B333" t="n">
-        <v>102.382622</v>
+        <v>102.382614</v>
       </c>
       <c r="C333" t="n">
         <v>109.325867</v>
@@ -7091,10 +7091,10 @@
         <v>336</v>
       </c>
       <c r="B335" t="n">
-        <v>100.510033</v>
+        <v>100.510025</v>
       </c>
       <c r="C335" t="n">
-        <v>107.78727</v>
+        <v>107.787262</v>
       </c>
     </row>
     <row r="336">
@@ -7138,7 +7138,7 @@
         <v>97.635818</v>
       </c>
       <c r="C339" t="n">
-        <v>108.214661</v>
+        <v>108.214653</v>
       </c>
     </row>
     <row r="340">
@@ -7146,7 +7146,7 @@
         <v>341</v>
       </c>
       <c r="B340" t="n">
-        <v>96.068077</v>
+        <v>96.068085</v>
       </c>
       <c r="C340" t="n">
         <v>106.590576</v>
@@ -7157,10 +7157,10 @@
         <v>342</v>
       </c>
       <c r="B341" t="n">
-        <v>93.890656</v>
+        <v>93.890648</v>
       </c>
       <c r="C341" t="n">
-        <v>106.847008</v>
+        <v>106.847015</v>
       </c>
     </row>
     <row r="342">
@@ -7190,7 +7190,7 @@
         <v>345</v>
       </c>
       <c r="B344" t="n">
-        <v>96.416458</v>
+        <v>96.416466</v>
       </c>
       <c r="C344" t="n">
         <v>106.676064</v>
@@ -7204,7 +7204,7 @@
         <v>96.198715</v>
       </c>
       <c r="C345" t="n">
-        <v>105.992241</v>
+        <v>105.992233</v>
       </c>
     </row>
     <row r="346">
@@ -7212,7 +7212,7 @@
         <v>347</v>
       </c>
       <c r="B346" t="n">
-        <v>96.764847</v>
+        <v>96.764854</v>
       </c>
       <c r="C346" t="n">
         <v>105.906761</v>
@@ -7226,7 +7226,7 @@
         <v>96.28582</v>
       </c>
       <c r="C347" t="n">
-        <v>106.334152</v>
+        <v>106.334145</v>
       </c>
     </row>
     <row r="348">
@@ -7248,7 +7248,7 @@
         <v>98.158401</v>
       </c>
       <c r="C349" t="n">
-        <v>106.077721</v>
+        <v>106.077713</v>
       </c>
     </row>
     <row r="350">
@@ -7256,7 +7256,7 @@
         <v>351</v>
       </c>
       <c r="B350" t="n">
-        <v>97.984207</v>
+        <v>97.984215</v>
       </c>
       <c r="C350" t="n">
         <v>107.359879</v>
@@ -7278,7 +7278,7 @@
         <v>353</v>
       </c>
       <c r="B352" t="n">
-        <v>95.458397</v>
+        <v>95.458389</v>
       </c>
       <c r="C352" t="n">
         <v>107.359879</v>
@@ -7292,7 +7292,7 @@
         <v>97.592278</v>
       </c>
       <c r="C353" t="n">
-        <v>106.847008</v>
+        <v>106.847015</v>
       </c>
     </row>
     <row r="354">
@@ -7300,10 +7300,10 @@
         <v>355</v>
       </c>
       <c r="B354" t="n">
-        <v>94.674515</v>
+        <v>94.674522</v>
       </c>
       <c r="C354" t="n">
-        <v>107.616318</v>
+        <v>107.61631</v>
       </c>
     </row>
     <row r="355">
@@ -7311,7 +7311,7 @@
         <v>356</v>
       </c>
       <c r="B355" t="n">
-        <v>95.589035</v>
+        <v>95.589043</v>
       </c>
       <c r="C355" t="n">
         <v>108.813004</v>
@@ -7322,7 +7322,7 @@
         <v>357</v>
       </c>
       <c r="B356" t="n">
-        <v>96.851952</v>
+        <v>96.851944</v>
       </c>
       <c r="C356" t="n">
         <v>110.266121</v>
@@ -7336,7 +7336,7 @@
         <v>96.939049</v>
       </c>
       <c r="C357" t="n">
-        <v>111.120895</v>
+        <v>111.120888</v>
       </c>
     </row>
     <row r="358">
@@ -7347,7 +7347,7 @@
         <v>97.374535</v>
       </c>
       <c r="C358" t="n">
-        <v>111.975677</v>
+        <v>111.97567</v>
       </c>
     </row>
     <row r="359">
@@ -7355,10 +7355,10 @@
         <v>360</v>
       </c>
       <c r="B359" t="n">
-        <v>95.458397</v>
+        <v>95.458389</v>
       </c>
       <c r="C359" t="n">
-        <v>111.377335</v>
+        <v>111.377327</v>
       </c>
     </row>
     <row r="360">
@@ -7380,7 +7380,7 @@
         <v>90.929352</v>
       </c>
       <c r="C361" t="n">
-        <v>110.864456</v>
+        <v>110.864464</v>
       </c>
     </row>
     <row r="362">
@@ -7388,10 +7388,10 @@
         <v>363</v>
       </c>
       <c r="B362" t="n">
-        <v>91.800323</v>
+        <v>91.800316</v>
       </c>
       <c r="C362" t="n">
-        <v>113.172356</v>
+        <v>113.172348</v>
       </c>
     </row>
     <row r="363">
@@ -7402,7 +7402,7 @@
         <v>90.189026</v>
       </c>
       <c r="C363" t="n">
-        <v>109.667778</v>
+        <v>109.66777</v>
       </c>
     </row>
     <row r="364">
@@ -7413,7 +7413,7 @@
         <v>90.493866</v>
       </c>
       <c r="C364" t="n">
-        <v>108.727516</v>
+        <v>108.727524</v>
       </c>
     </row>
     <row r="365">
@@ -7421,7 +7421,7 @@
         <v>366</v>
       </c>
       <c r="B365" t="n">
-        <v>87.706757</v>
+        <v>87.706749</v>
       </c>
       <c r="C365" t="n">
         <v>107.274406</v>
@@ -7446,7 +7446,7 @@
         <v>87.750305</v>
       </c>
       <c r="C367" t="n">
-        <v>105.222939</v>
+        <v>105.222946</v>
       </c>
     </row>
     <row r="368">
@@ -7454,7 +7454,7 @@
         <v>369</v>
       </c>
       <c r="B368" t="n">
-        <v>89.535805</v>
+        <v>89.535797</v>
       </c>
       <c r="C368" t="n">
         <v>106.676064</v>
@@ -7465,7 +7465,7 @@
         <v>370</v>
       </c>
       <c r="B369" t="n">
-        <v>90.363213</v>
+        <v>90.36322</v>
       </c>
       <c r="C369" t="n">
         <v>106.932487</v>
@@ -7476,7 +7476,7 @@
         <v>371</v>
       </c>
       <c r="B370" t="n">
-        <v>91.234184</v>
+        <v>91.234192</v>
       </c>
       <c r="C370" t="n">
         <v>108.813004</v>
@@ -7509,7 +7509,7 @@
         <v>374</v>
       </c>
       <c r="B373" t="n">
-        <v>91.234184</v>
+        <v>91.234192</v>
       </c>
       <c r="C373" t="n">
         <v>110.180641</v>
@@ -7531,10 +7531,10 @@
         <v>376</v>
       </c>
       <c r="B375" t="n">
-        <v>90.755157</v>
+        <v>90.75515</v>
       </c>
       <c r="C375" t="n">
-        <v>109.411339</v>
+        <v>109.411346</v>
       </c>
     </row>
     <row r="376">
@@ -7564,7 +7564,7 @@
         <v>379</v>
       </c>
       <c r="B378" t="n">
-        <v>89.492241</v>
+        <v>89.492249</v>
       </c>
       <c r="C378" t="n">
         <v>105.393898</v>
@@ -7578,7 +7578,7 @@
         <v>90.232574</v>
       </c>
       <c r="C379" t="n">
-        <v>106.505096</v>
+        <v>106.505104</v>
       </c>
     </row>
     <row r="380">
@@ -7586,7 +7586,7 @@
         <v>381</v>
       </c>
       <c r="B380" t="n">
-        <v>90.668053</v>
+        <v>90.66806</v>
       </c>
       <c r="C380" t="n">
         <v>104.624596</v>
@@ -7600,7 +7600,7 @@
         <v>91.495483</v>
       </c>
       <c r="C381" t="n">
-        <v>105.222939</v>
+        <v>105.222946</v>
       </c>
     </row>
     <row r="382">
@@ -7619,10 +7619,10 @@
         <v>384</v>
       </c>
       <c r="B383" t="n">
-        <v>89.361603</v>
+        <v>89.361595</v>
       </c>
       <c r="C383" t="n">
-        <v>102.145752</v>
+        <v>102.145744</v>
       </c>
     </row>
     <row r="384">
@@ -7633,7 +7633,7 @@
         <v>89.274506</v>
       </c>
       <c r="C384" t="n">
-        <v>101.20549</v>
+        <v>101.205498</v>
       </c>
     </row>
     <row r="385">
@@ -7644,7 +7644,7 @@
         <v>88.53418</v>
       </c>
       <c r="C385" t="n">
-        <v>101.632881</v>
+        <v>101.632889</v>
       </c>
     </row>
     <row r="386">
@@ -7663,7 +7663,7 @@
         <v>388</v>
       </c>
       <c r="B387" t="n">
-        <v>89.709991</v>
+        <v>89.709984</v>
       </c>
       <c r="C387" t="n">
         <v>103.684349</v>
@@ -7674,10 +7674,10 @@
         <v>389</v>
       </c>
       <c r="B388" t="n">
-        <v>90.668053</v>
+        <v>90.66806</v>
       </c>
       <c r="C388" t="n">
-        <v>104.19722</v>
+        <v>104.197212</v>
       </c>
     </row>
     <row r="389">
@@ -7696,7 +7696,7 @@
         <v>391</v>
       </c>
       <c r="B390" t="n">
-        <v>89.143852</v>
+        <v>89.14386</v>
       </c>
       <c r="C390" t="n">
         <v>103.684349</v>
@@ -7707,10 +7707,10 @@
         <v>392</v>
       </c>
       <c r="B391" t="n">
-        <v>87.044815</v>
+        <v>87.044823</v>
       </c>
       <c r="C391" t="n">
-        <v>101.632881</v>
+        <v>101.632889</v>
       </c>
     </row>
     <row r="392">
@@ -7740,10 +7740,10 @@
         <v>395</v>
       </c>
       <c r="B394" t="n">
-        <v>85.564171</v>
+        <v>85.564163</v>
       </c>
       <c r="C394" t="n">
-        <v>99.15403</v>
+        <v>99.154037</v>
       </c>
     </row>
     <row r="395">
@@ -7751,10 +7751,10 @@
         <v>396</v>
       </c>
       <c r="B395" t="n">
-        <v>84.066101</v>
+        <v>84.066093</v>
       </c>
       <c r="C395" t="n">
-        <v>98.042824</v>
+        <v>98.042816</v>
       </c>
     </row>
     <row r="396">
@@ -7762,10 +7762,10 @@
         <v>397</v>
       </c>
       <c r="B396" t="n">
-        <v>83.839653</v>
+        <v>83.839645</v>
       </c>
       <c r="C396" t="n">
-        <v>99.923332</v>
+        <v>99.923325</v>
       </c>
     </row>
     <row r="397">
@@ -7776,7 +7776,7 @@
         <v>83.508675</v>
       </c>
       <c r="C397" t="n">
-        <v>98.726639</v>
+        <v>98.726646</v>
       </c>
     </row>
     <row r="398">
@@ -7784,7 +7784,7 @@
         <v>399</v>
       </c>
       <c r="B398" t="n">
-        <v>83.857063</v>
+        <v>83.857071</v>
       </c>
       <c r="C398" t="n">
         <v>98.641167</v>
@@ -7795,7 +7795,7 @@
         <v>400</v>
       </c>
       <c r="B399" t="n">
-        <v>82.672546</v>
+        <v>82.672539</v>
       </c>
       <c r="C399" t="n">
         <v>98.128304</v>
@@ -7809,7 +7809,7 @@
         <v>81.244148</v>
       </c>
       <c r="C400" t="n">
-        <v>95.991364</v>
+        <v>95.991356</v>
       </c>
     </row>
     <row r="401">
@@ -7828,10 +7828,10 @@
         <v>403</v>
       </c>
       <c r="B402" t="n">
-        <v>77.516396</v>
+        <v>77.516403</v>
       </c>
       <c r="C402" t="n">
-        <v>92.230339</v>
+        <v>92.230347</v>
       </c>
     </row>
     <row r="403">
@@ -7842,7 +7842,7 @@
         <v>76.749947</v>
       </c>
       <c r="C403" t="n">
-        <v>91.461044</v>
+        <v>91.461037</v>
       </c>
     </row>
     <row r="404">
@@ -7850,7 +7850,7 @@
         <v>405</v>
       </c>
       <c r="B404" t="n">
-        <v>79.362862</v>
+        <v>79.362854</v>
       </c>
       <c r="C404" t="n">
         <v>94.709198</v>
@@ -7864,7 +7864,7 @@
         <v>79.955116</v>
       </c>
       <c r="C405" t="n">
-        <v>95.307541</v>
+        <v>95.307533</v>
       </c>
     </row>
     <row r="406">
@@ -7872,7 +7872,7 @@
         <v>407</v>
       </c>
       <c r="B406" t="n">
-        <v>77.882202</v>
+        <v>77.88221</v>
       </c>
       <c r="C406" t="n">
         <v>93.597984</v>
@@ -7883,10 +7883,10 @@
         <v>408</v>
       </c>
       <c r="B407" t="n">
-        <v>77.516396</v>
+        <v>77.516403</v>
       </c>
       <c r="C407" t="n">
-        <v>92.65773</v>
+        <v>92.657738</v>
       </c>
     </row>
     <row r="408">
@@ -7894,10 +7894,10 @@
         <v>409</v>
       </c>
       <c r="B408" t="n">
-        <v>78.561554</v>
+        <v>78.561562</v>
       </c>
       <c r="C408" t="n">
-        <v>94.880142</v>
+        <v>94.88015</v>
       </c>
     </row>
     <row r="409">
@@ -7905,10 +7905,10 @@
         <v>410</v>
       </c>
       <c r="B409" t="n">
-        <v>77.67318</v>
+        <v>77.673172</v>
       </c>
       <c r="C409" t="n">
-        <v>94.880142</v>
+        <v>94.88015</v>
       </c>
     </row>
     <row r="410">
@@ -7916,7 +7916,7 @@
         <v>411</v>
       </c>
       <c r="B410" t="n">
-        <v>76.418968</v>
+        <v>76.418976</v>
       </c>
       <c r="C410" t="n">
         <v>93.256073</v>
@@ -7949,7 +7949,7 @@
         <v>414</v>
       </c>
       <c r="B413" t="n">
-        <v>76.59317</v>
+        <v>76.593178</v>
       </c>
       <c r="C413" t="n">
         <v>80.348953</v>
@@ -7985,7 +7985,7 @@
         <v>75.251877</v>
       </c>
       <c r="C416" t="n">
-        <v>80.562653</v>
+        <v>80.562645</v>
       </c>
     </row>
     <row r="417">
@@ -8007,7 +8007,7 @@
         <v>78.875107</v>
       </c>
       <c r="C418" t="n">
-        <v>82.998756</v>
+        <v>82.998764</v>
       </c>
     </row>
     <row r="419">
@@ -8029,7 +8029,7 @@
         <v>86.644173</v>
       </c>
       <c r="C420" t="n">
-        <v>86.930733</v>
+        <v>86.930725</v>
       </c>
     </row>
     <row r="421">
@@ -8037,7 +8037,7 @@
         <v>422</v>
       </c>
       <c r="B421" t="n">
-        <v>88.055145</v>
+        <v>88.055138</v>
       </c>
       <c r="C421" t="n">
         <v>88.554802</v>
@@ -8051,7 +8051,7 @@
         <v>87.968048</v>
       </c>
       <c r="C422" t="n">
-        <v>88.041939</v>
+        <v>88.041946</v>
       </c>
     </row>
     <row r="423">
@@ -8059,10 +8059,10 @@
         <v>424</v>
       </c>
       <c r="B423" t="n">
-        <v>88.011604</v>
+        <v>88.011597</v>
       </c>
       <c r="C423" t="n">
-        <v>87.870995</v>
+        <v>87.870979</v>
       </c>
     </row>
     <row r="424">
@@ -8084,7 +8084,7 @@
         <v>88.22934</v>
       </c>
       <c r="C425" t="n">
-        <v>88.640274</v>
+        <v>88.640282</v>
       </c>
     </row>
     <row r="426">
@@ -8095,7 +8095,7 @@
         <v>85.02417</v>
       </c>
       <c r="C426" t="n">
-        <v>87.187157</v>
+        <v>87.187164</v>
       </c>
     </row>
     <row r="427">
@@ -8103,10 +8103,10 @@
         <v>428</v>
       </c>
       <c r="B427" t="n">
-        <v>83.247391</v>
+        <v>83.247383</v>
       </c>
       <c r="C427" t="n">
-        <v>87.529083</v>
+        <v>87.529076</v>
       </c>
     </row>
     <row r="428">
@@ -8114,10 +8114,10 @@
         <v>429</v>
       </c>
       <c r="B428" t="n">
-        <v>84.41449</v>
+        <v>84.414482</v>
       </c>
       <c r="C428" t="n">
-        <v>89.495056</v>
+        <v>89.495064</v>
       </c>
     </row>
     <row r="429">
@@ -8125,7 +8125,7 @@
         <v>430</v>
       </c>
       <c r="B429" t="n">
-        <v>85.355141</v>
+        <v>85.355133</v>
       </c>
       <c r="C429" t="n">
         <v>99.495941</v>
@@ -8136,7 +8136,7 @@
         <v>431</v>
       </c>
       <c r="B430" t="n">
-        <v>83.613197</v>
+        <v>83.61319</v>
       </c>
       <c r="C430" t="n">
         <v>101.461922</v>
@@ -8172,7 +8172,7 @@
         <v>82.289322</v>
       </c>
       <c r="C433" t="n">
-        <v>108.385612</v>
+        <v>108.38562</v>
       </c>
     </row>
     <row r="434">
@@ -8180,7 +8180,7 @@
         <v>435</v>
       </c>
       <c r="B434" t="n">
-        <v>83.386734</v>
+        <v>83.386742</v>
       </c>
       <c r="C434" t="n">
         <v>104.881027</v>
@@ -8194,7 +8194,7 @@
         <v>83.073189</v>
       </c>
       <c r="C435" t="n">
-        <v>103.25695</v>
+        <v>103.256958</v>
       </c>
     </row>
     <row r="436">
@@ -8202,7 +8202,7 @@
         <v>437</v>
       </c>
       <c r="B436" t="n">
-        <v>82.742218</v>
+        <v>82.742226</v>
       </c>
       <c r="C436" t="n">
         <v>102.402184</v>
@@ -8216,7 +8216,7 @@
         <v>82.02803</v>
       </c>
       <c r="C437" t="n">
-        <v>99.923332</v>
+        <v>99.923325</v>
       </c>
     </row>
     <row r="438">
@@ -8227,7 +8227,7 @@
         <v>80.216408</v>
       </c>
       <c r="C438" t="n">
-        <v>99.23951</v>
+        <v>99.239502</v>
       </c>
     </row>
     <row r="439">
@@ -8238,7 +8238,7 @@
         <v>79.989952</v>
       </c>
       <c r="C439" t="n">
-        <v>99.15403</v>
+        <v>99.154037</v>
       </c>
     </row>
     <row r="440">
@@ -8260,7 +8260,7 @@
         <v>80.059631</v>
       </c>
       <c r="C441" t="n">
-        <v>102.658607</v>
+        <v>102.658615</v>
       </c>
     </row>
     <row r="442">
@@ -8271,7 +8271,7 @@
         <v>79.972534</v>
       </c>
       <c r="C442" t="n">
-        <v>102.316696</v>
+        <v>102.316704</v>
       </c>
     </row>
     <row r="443">
@@ -8279,7 +8279,7 @@
         <v>444</v>
       </c>
       <c r="B443" t="n">
-        <v>80.164154</v>
+        <v>80.164146</v>
       </c>
       <c r="C443" t="n">
         <v>100.521667</v>
@@ -8290,10 +8290,10 @@
         <v>445</v>
       </c>
       <c r="B444" t="n">
-        <v>82.881584</v>
+        <v>82.881577</v>
       </c>
       <c r="C444" t="n">
-        <v>102.145752</v>
+        <v>102.145744</v>
       </c>
     </row>
     <row r="445">
@@ -8301,7 +8301,7 @@
         <v>446</v>
       </c>
       <c r="B445" t="n">
-        <v>83.595779</v>
+        <v>83.595772</v>
       </c>
       <c r="C445" t="n">
         <v>104.795555</v>
@@ -8326,7 +8326,7 @@
         <v>84.693199</v>
       </c>
       <c r="C447" t="n">
-        <v>109.924217</v>
+        <v>109.92421</v>
       </c>
     </row>
     <row r="448">
@@ -8345,7 +8345,7 @@
         <v>450</v>
       </c>
       <c r="B449" t="n">
-        <v>83.822227</v>
+        <v>83.82222</v>
       </c>
       <c r="C449" t="n">
         <v>110.266121</v>
@@ -8356,10 +8356,10 @@
         <v>451</v>
       </c>
       <c r="B450" t="n">
-        <v>85.877724</v>
+        <v>85.877716</v>
       </c>
       <c r="C450" t="n">
-        <v>112.659492</v>
+        <v>112.6595</v>
       </c>
     </row>
     <row r="451">
@@ -8367,7 +8367,7 @@
         <v>452</v>
       </c>
       <c r="B451" t="n">
-        <v>85.877724</v>
+        <v>85.877716</v>
       </c>
       <c r="C451" t="n">
         <v>113.257835</v>
@@ -8381,7 +8381,7 @@
         <v>85.529327</v>
       </c>
       <c r="C452" t="n">
-        <v>115.394783</v>
+        <v>115.394775</v>
       </c>
     </row>
     <row r="453">
@@ -8392,7 +8392,7 @@
         <v>85.668686</v>
       </c>
       <c r="C453" t="n">
-        <v>114.881905</v>
+        <v>114.881912</v>
       </c>
     </row>
     <row r="454">
@@ -8400,10 +8400,10 @@
         <v>455</v>
       </c>
       <c r="B454" t="n">
-        <v>85.877724</v>
+        <v>85.877716</v>
       </c>
       <c r="C454" t="n">
-        <v>116.07859</v>
+        <v>116.078598</v>
       </c>
     </row>
     <row r="455">
@@ -8425,7 +8425,7 @@
         <v>84.867393</v>
       </c>
       <c r="C456" t="n">
-        <v>115.736671</v>
+        <v>115.736687</v>
       </c>
     </row>
     <row r="457">
@@ -8436,7 +8436,7 @@
         <v>82.829323</v>
       </c>
       <c r="C457" t="n">
-        <v>113.856178</v>
+        <v>113.856171</v>
       </c>
     </row>
     <row r="458">
@@ -8444,7 +8444,7 @@
         <v>459</v>
       </c>
       <c r="B458" t="n">
-        <v>83.247391</v>
+        <v>83.247383</v>
       </c>
       <c r="C458" t="n">
         <v>112.317574</v>
@@ -8488,7 +8488,7 @@
         <v>463</v>
       </c>
       <c r="B462" t="n">
-        <v>81.766731</v>
+        <v>81.766739</v>
       </c>
       <c r="C462" t="n">
         <v>115.651207</v>
@@ -8499,7 +8499,7 @@
         <v>464</v>
       </c>
       <c r="B463" t="n">
-        <v>83.630608</v>
+        <v>83.630615</v>
       </c>
       <c r="C463" t="n">
         <v>116.33503</v>
@@ -8513,7 +8513,7 @@
         <v>83.369324</v>
       </c>
       <c r="C464" t="n">
-        <v>115.993111</v>
+        <v>115.993118</v>
       </c>
     </row>
     <row r="465">
@@ -8532,10 +8532,10 @@
         <v>467</v>
       </c>
       <c r="B466" t="n">
-        <v>82.30674</v>
+        <v>82.306732</v>
       </c>
       <c r="C466" t="n">
-        <v>116.933372</v>
+        <v>116.93338</v>
       </c>
     </row>
     <row r="467">
@@ -8543,7 +8543,7 @@
         <v>468</v>
       </c>
       <c r="B467" t="n">
-        <v>80.442863</v>
+        <v>80.442856</v>
       </c>
       <c r="C467" t="n">
         <v>113.514275</v>
@@ -8557,7 +8557,7 @@
         <v>80.634476</v>
       </c>
       <c r="C468" t="n">
-        <v>111.377335</v>
+        <v>111.377327</v>
       </c>
     </row>
     <row r="469">
@@ -8576,10 +8576,10 @@
         <v>471</v>
       </c>
       <c r="B470" t="n">
-        <v>79.240929</v>
+        <v>79.240921</v>
       </c>
       <c r="C470" t="n">
-        <v>110.949936</v>
+        <v>110.949944</v>
       </c>
     </row>
     <row r="471">
@@ -8587,10 +8587,10 @@
         <v>472</v>
       </c>
       <c r="B471" t="n">
-        <v>79.362862</v>
+        <v>79.362854</v>
       </c>
       <c r="C471" t="n">
-        <v>110.864456</v>
+        <v>110.864464</v>
       </c>
     </row>
     <row r="472">
@@ -8612,7 +8612,7 @@
         <v>78.735756</v>
       </c>
       <c r="C473" t="n">
-        <v>108.727516</v>
+        <v>108.727524</v>
       </c>
     </row>
     <row r="474">
@@ -8645,7 +8645,7 @@
         <v>79.275757</v>
       </c>
       <c r="C476" t="n">
-        <v>108.727516</v>
+        <v>108.727524</v>
       </c>
     </row>
     <row r="477">
@@ -8667,7 +8667,7 @@
         <v>80.129311</v>
       </c>
       <c r="C478" t="n">
-        <v>109.582298</v>
+        <v>109.582291</v>
       </c>
     </row>
     <row r="479">
@@ -8675,10 +8675,10 @@
         <v>480</v>
       </c>
       <c r="B479" t="n">
-        <v>79.746078</v>
+        <v>79.746086</v>
       </c>
       <c r="C479" t="n">
-        <v>109.154907</v>
+        <v>109.154915</v>
       </c>
     </row>
     <row r="480">
@@ -8700,7 +8700,7 @@
         <v>79.223503</v>
       </c>
       <c r="C481" t="n">
-        <v>105.479378</v>
+        <v>105.47937</v>
       </c>
     </row>
     <row r="482">
@@ -8708,7 +8708,7 @@
         <v>483</v>
       </c>
       <c r="B482" t="n">
-        <v>79.780914</v>
+        <v>79.780922</v>
       </c>
       <c r="C482" t="n">
         <v>108.983955</v>
@@ -8719,10 +8719,10 @@
         <v>484</v>
       </c>
       <c r="B483" t="n">
-        <v>82.463509</v>
+        <v>82.463516</v>
       </c>
       <c r="C483" t="n">
-        <v>110.949936</v>
+        <v>110.949944</v>
       </c>
     </row>
     <row r="484">
@@ -8744,7 +8744,7 @@
         <v>84.01384</v>
       </c>
       <c r="C485" t="n">
-        <v>113.172356</v>
+        <v>113.172348</v>
       </c>
     </row>
     <row r="486">
@@ -8766,7 +8766,7 @@
         <v>84.849968</v>
       </c>
       <c r="C487" t="n">
-        <v>113.856178</v>
+        <v>113.856171</v>
       </c>
     </row>
     <row r="488">
@@ -8777,7 +8777,7 @@
         <v>87.271271</v>
       </c>
       <c r="C488" t="n">
-        <v>113.941658</v>
+        <v>113.94165</v>
       </c>
     </row>
     <row r="489">
@@ -8799,7 +8799,7 @@
         <v>92.671295</v>
       </c>
       <c r="C490" t="n">
-        <v>112.488533</v>
+        <v>112.488548</v>
       </c>
     </row>
     <row r="491">
@@ -8807,10 +8807,10 @@
         <v>492</v>
       </c>
       <c r="B491" t="n">
-        <v>94.108398</v>
+        <v>94.108391</v>
       </c>
       <c r="C491" t="n">
-        <v>117.104324</v>
+        <v>117.104317</v>
       </c>
     </row>
     <row r="492">
@@ -8818,7 +8818,7 @@
         <v>493</v>
       </c>
       <c r="B492" t="n">
-        <v>93.193878</v>
+        <v>93.193871</v>
       </c>
       <c r="C492" t="n">
         <v>118.215546</v>
@@ -8832,7 +8832,7 @@
         <v>92.105156</v>
       </c>
       <c r="C493" t="n">
-        <v>116.933372</v>
+        <v>116.93338</v>
       </c>
     </row>
     <row r="494">
@@ -8851,10 +8851,10 @@
         <v>496</v>
       </c>
       <c r="B495" t="n">
-        <v>93.193878</v>
+        <v>93.193871</v>
       </c>
       <c r="C495" t="n">
-        <v>118.899368</v>
+        <v>118.899353</v>
       </c>
     </row>
     <row r="496">
@@ -8865,7 +8865,7 @@
         <v>93.411613</v>
       </c>
       <c r="C496" t="n">
-        <v>119.07032</v>
+        <v>119.070328</v>
       </c>
     </row>
     <row r="497">
@@ -8873,10 +8873,10 @@
         <v>498</v>
       </c>
       <c r="B497" t="n">
-        <v>93.890656</v>
+        <v>93.890648</v>
       </c>
       <c r="C497" t="n">
-        <v>119.497711</v>
+        <v>119.497704</v>
       </c>
     </row>
     <row r="498">
@@ -8884,7 +8884,7 @@
         <v>499</v>
       </c>
       <c r="B498" t="n">
-        <v>96.111618</v>
+        <v>96.111626</v>
       </c>
       <c r="C498" t="n">
         <v>121.976547</v>
@@ -8895,10 +8895,10 @@
         <v>500</v>
       </c>
       <c r="B499" t="n">
-        <v>93.977745</v>
+        <v>93.977753</v>
       </c>
       <c r="C499" t="n">
-        <v>121.463684</v>
+        <v>121.463692</v>
       </c>
     </row>
     <row r="500">
@@ -8909,7 +8909,7 @@
         <v>92.932579</v>
       </c>
       <c r="C500" t="n">
-        <v>120.608917</v>
+        <v>120.60891</v>
       </c>
     </row>
     <row r="501">
@@ -8920,7 +8920,7 @@
         <v>93.847099</v>
       </c>
       <c r="C501" t="n">
-        <v>120.694382</v>
+        <v>120.694389</v>
       </c>
     </row>
     <row r="502">
@@ -8931,7 +8931,7 @@
         <v>94.282585</v>
       </c>
       <c r="C502" t="n">
-        <v>120.52343</v>
+        <v>120.523438</v>
       </c>
     </row>
     <row r="503">
@@ -8939,10 +8939,10 @@
         <v>504</v>
       </c>
       <c r="B503" t="n">
-        <v>96.068077</v>
+        <v>96.068085</v>
       </c>
       <c r="C503" t="n">
-        <v>124.369919</v>
+        <v>124.369926</v>
       </c>
     </row>
     <row r="504">
@@ -8950,7 +8950,7 @@
         <v>505</v>
       </c>
       <c r="B504" t="n">
-        <v>94.979362</v>
+        <v>94.97937</v>
       </c>
       <c r="C504" t="n">
         <v>121.976547</v>
@@ -8972,10 +8972,10 @@
         <v>507</v>
       </c>
       <c r="B506" t="n">
-        <v>94.064842</v>
+        <v>94.06485</v>
       </c>
       <c r="C506" t="n">
-        <v>123.686096</v>
+        <v>123.686104</v>
       </c>
     </row>
     <row r="507">
@@ -8994,10 +8994,10 @@
         <v>509</v>
       </c>
       <c r="B508" t="n">
-        <v>94.674515</v>
+        <v>94.674522</v>
       </c>
       <c r="C508" t="n">
-        <v>123.600624</v>
+        <v>123.600639</v>
       </c>
     </row>
     <row r="509">
@@ -9008,7 +9008,7 @@
         <v>95.806786</v>
       </c>
       <c r="C509" t="n">
-        <v>123.3442</v>
+        <v>123.344208</v>
       </c>
     </row>
     <row r="510">
@@ -9016,7 +9016,7 @@
         <v>511</v>
       </c>
       <c r="B510" t="n">
-        <v>95.632599</v>
+        <v>95.632591</v>
       </c>
       <c r="C510" t="n">
         <v>127.361641</v>
@@ -9030,7 +9030,7 @@
         <v>95.806786</v>
       </c>
       <c r="C511" t="n">
-        <v>125.993996</v>
+        <v>125.993988</v>
       </c>
     </row>
     <row r="512">
@@ -9041,7 +9041,7 @@
         <v>96.721306</v>
       </c>
       <c r="C512" t="n">
-        <v>127.703537</v>
+        <v>127.703552</v>
       </c>
     </row>
     <row r="513">
@@ -9052,7 +9052,7 @@
         <v>94.848717</v>
       </c>
       <c r="C513" t="n">
-        <v>126.934258</v>
+        <v>126.93425</v>
       </c>
     </row>
     <row r="514">
@@ -9060,10 +9060,10 @@
         <v>515</v>
       </c>
       <c r="B514" t="n">
-        <v>95.458397</v>
+        <v>95.458389</v>
       </c>
       <c r="C514" t="n">
-        <v>125.993996</v>
+        <v>125.993988</v>
       </c>
     </row>
     <row r="515">
@@ -9074,7 +9074,7 @@
         <v>92.453545</v>
       </c>
       <c r="C515" t="n">
-        <v>123.087769</v>
+        <v>123.087761</v>
       </c>
     </row>
     <row r="516">
@@ -9085,7 +9085,7 @@
         <v>94.500328</v>
       </c>
       <c r="C516" t="n">
-        <v>125.224693</v>
+        <v>125.224701</v>
       </c>
     </row>
     <row r="517">
@@ -9093,10 +9093,10 @@
         <v>518</v>
       </c>
       <c r="B517" t="n">
-        <v>95.893875</v>
+        <v>95.893883</v>
       </c>
       <c r="C517" t="n">
-        <v>125.993996</v>
+        <v>125.993988</v>
       </c>
     </row>
     <row r="518">
@@ -9104,10 +9104,10 @@
         <v>519</v>
       </c>
       <c r="B518" t="n">
-        <v>94.674515</v>
+        <v>94.674522</v>
       </c>
       <c r="C518" t="n">
-        <v>124.198967</v>
+        <v>124.198982</v>
       </c>
     </row>
     <row r="519">
@@ -9118,7 +9118,7 @@
         <v>98.332603</v>
       </c>
       <c r="C519" t="n">
-        <v>125.481133</v>
+        <v>125.481125</v>
       </c>
     </row>
     <row r="520">
@@ -9126,7 +9126,7 @@
         <v>521</v>
       </c>
       <c r="B520" t="n">
-        <v>97.20034</v>
+        <v>97.200333</v>
       </c>
       <c r="C520" t="n">
         <v>125.652092</v>
@@ -9137,10 +9137,10 @@
         <v>522</v>
       </c>
       <c r="B521" t="n">
-        <v>99.943901</v>
+        <v>99.943893</v>
       </c>
       <c r="C521" t="n">
-        <v>127.276169</v>
+        <v>127.276161</v>
       </c>
     </row>
     <row r="522">
@@ -9148,7 +9148,7 @@
         <v>523</v>
       </c>
       <c r="B522" t="n">
-        <v>100.422928</v>
+        <v>100.422935</v>
       </c>
       <c r="C522" t="n">
         <v>128.472855</v>
@@ -9159,7 +9159,7 @@
         <v>524</v>
       </c>
       <c r="B523" t="n">
-        <v>102.164871</v>
+        <v>102.164879</v>
       </c>
       <c r="C523" t="n">
         <v>131.293625</v>
@@ -9170,7 +9170,7 @@
         <v>525</v>
       </c>
       <c r="B524" t="n">
-        <v>102.513252</v>
+        <v>102.51326</v>
       </c>
       <c r="C524" t="n">
         <v>130.438843</v>
@@ -9192,7 +9192,7 @@
         <v>527</v>
       </c>
       <c r="B526" t="n">
-        <v>105.822945</v>
+        <v>105.822952</v>
       </c>
       <c r="C526" t="n">
         <v>133.516022</v>
@@ -9203,10 +9203,10 @@
         <v>528</v>
       </c>
       <c r="B527" t="n">
-        <v>107.608444</v>
+        <v>107.608437</v>
       </c>
       <c r="C527" t="n">
-        <v>134.285339</v>
+        <v>134.285324</v>
       </c>
     </row>
     <row r="528">
@@ -9214,10 +9214,10 @@
         <v>529</v>
       </c>
       <c r="B528" t="n">
-        <v>106.519722</v>
+        <v>106.51973</v>
       </c>
       <c r="C528" t="n">
-        <v>134.199844</v>
+        <v>134.19986</v>
       </c>
     </row>
     <row r="529">
@@ -9228,7 +9228,7 @@
         <v>105.866501</v>
       </c>
       <c r="C529" t="n">
-        <v>134.883667</v>
+        <v>134.883682</v>
       </c>
     </row>
     <row r="530">
@@ -9239,7 +9239,7 @@
         <v>104.951973</v>
       </c>
       <c r="C530" t="n">
-        <v>135.909393</v>
+        <v>135.909409</v>
       </c>
     </row>
     <row r="531">
@@ -9269,7 +9269,7 @@
         <v>534</v>
       </c>
       <c r="B533" t="n">
-        <v>106.476173</v>
+        <v>106.476181</v>
       </c>
       <c r="C533" t="n">
         <v>138.473724</v>
@@ -9283,7 +9283,7 @@
         <v>104.995529</v>
       </c>
       <c r="C534" t="n">
-        <v>137.020599</v>
+        <v>137.020615</v>
       </c>
     </row>
     <row r="535">
@@ -9294,7 +9294,7 @@
         <v>100.161644</v>
       </c>
       <c r="C535" t="n">
-        <v>134.199844</v>
+        <v>134.19986</v>
       </c>
     </row>
     <row r="536">
@@ -9305,7 +9305,7 @@
         <v>99.116478</v>
       </c>
       <c r="C536" t="n">
-        <v>130.951706</v>
+        <v>130.951691</v>
       </c>
     </row>
     <row r="537">
@@ -9338,7 +9338,7 @@
         <v>91.147095</v>
       </c>
       <c r="C539" t="n">
-        <v>106.847008</v>
+        <v>106.847015</v>
       </c>
     </row>
     <row r="540">
@@ -9346,7 +9346,7 @@
         <v>541</v>
       </c>
       <c r="B540" t="n">
-        <v>91.582573</v>
+        <v>91.582581</v>
       </c>
       <c r="C540" t="n">
         <v>107.872742</v>
@@ -9357,10 +9357,10 @@
         <v>542</v>
       </c>
       <c r="B541" t="n">
-        <v>93.063225</v>
+        <v>93.063232</v>
       </c>
       <c r="C541" t="n">
-        <v>109.83873</v>
+        <v>109.838737</v>
       </c>
     </row>
     <row r="542">
@@ -9371,7 +9371,7 @@
         <v>93.237427</v>
       </c>
       <c r="C542" t="n">
-        <v>106.505096</v>
+        <v>106.505104</v>
       </c>
     </row>
     <row r="543">
@@ -9412,10 +9412,10 @@
         <v>547</v>
       </c>
       <c r="B546" t="n">
-        <v>77.28994</v>
+        <v>77.289948</v>
       </c>
       <c r="C546" t="n">
-        <v>93.854424</v>
+        <v>93.854416</v>
       </c>
     </row>
     <row r="547">
@@ -9426,7 +9426,7 @@
         <v>74.48542</v>
       </c>
       <c r="C547" t="n">
-        <v>92.486771</v>
+        <v>92.486763</v>
       </c>
     </row>
     <row r="548">
@@ -9434,10 +9434,10 @@
         <v>549</v>
       </c>
       <c r="B548" t="n">
-        <v>67.726692</v>
+        <v>67.726685</v>
       </c>
       <c r="C548" t="n">
-        <v>82.272194</v>
+        <v>82.272202</v>
       </c>
     </row>
     <row r="549">
@@ -9448,7 +9448,7 @@
         <v>67.761528</v>
       </c>
       <c r="C549" t="n">
-        <v>83.682587</v>
+        <v>83.682579</v>
       </c>
     </row>
     <row r="550">
@@ -9459,7 +9459,7 @@
         <v>64.486679</v>
       </c>
       <c r="C550" t="n">
-        <v>78.895844</v>
+        <v>78.895836</v>
       </c>
     </row>
     <row r="551">
@@ -9470,7 +9470,7 @@
         <v>64.62603</v>
       </c>
       <c r="C551" t="n">
-        <v>80.220734</v>
+        <v>80.220741</v>
       </c>
     </row>
     <row r="552">
@@ -9492,7 +9492,7 @@
         <v>71.708336</v>
       </c>
       <c r="C553" t="n">
-        <v>78.126534</v>
+        <v>78.126541</v>
       </c>
     </row>
     <row r="554">
@@ -9580,7 +9580,7 @@
         <v>75.642952</v>
       </c>
       <c r="C561" t="n">
-        <v>91.515839</v>
+        <v>91.515846</v>
       </c>
     </row>
     <row r="562">
@@ -9613,7 +9613,7 @@
         <v>71.078796</v>
       </c>
       <c r="C564" t="n">
-        <v>88.706573</v>
+        <v>88.706566</v>
       </c>
     </row>
     <row r="565">
@@ -9624,7 +9624,7 @@
         <v>72.141136</v>
       </c>
       <c r="C565" t="n">
-        <v>88.373268</v>
+        <v>88.37326</v>
       </c>
     </row>
     <row r="566">
@@ -9690,7 +9690,7 @@
         <v>72.318199</v>
       </c>
       <c r="C571" t="n">
-        <v>89.373169</v>
+        <v>89.373177</v>
       </c>
     </row>
     <row r="572">
@@ -9701,7 +9701,7 @@
         <v>71.82637</v>
       </c>
       <c r="C572" t="n">
-        <v>90.992088</v>
+        <v>90.992081</v>
       </c>
     </row>
     <row r="573">
@@ -9734,7 +9734,7 @@
         <v>72.455917</v>
       </c>
       <c r="C575" t="n">
-        <v>91.230164</v>
+        <v>91.230156</v>
       </c>
     </row>
     <row r="576">
@@ -9745,7 +9745,7 @@
         <v>70.134491</v>
       </c>
       <c r="C576" t="n">
-        <v>89.706474</v>
+        <v>89.706482</v>
       </c>
     </row>
     <row r="577">
@@ -9789,7 +9789,7 @@
         <v>79.479202</v>
       </c>
       <c r="C580" t="n">
-        <v>107.89537</v>
+        <v>107.895378</v>
       </c>
     </row>
     <row r="581">
@@ -9833,7 +9833,7 @@
         <v>74.226486</v>
       </c>
       <c r="C584" t="n">
-        <v>95.08696</v>
+        <v>95.086967</v>
       </c>
     </row>
     <row r="585">
@@ -9855,7 +9855,7 @@
         <v>74.619949</v>
       </c>
       <c r="C586" t="n">
-        <v>100.086533</v>
+        <v>100.086525</v>
       </c>
     </row>
     <row r="587">
@@ -9866,7 +9866,7 @@
         <v>74.167473</v>
       </c>
       <c r="C587" t="n">
-        <v>101.134048</v>
+        <v>101.134056</v>
       </c>
     </row>
     <row r="588">
@@ -9899,7 +9899,7 @@
         <v>70.803375</v>
       </c>
       <c r="C590" t="n">
-        <v>99.991302</v>
+        <v>99.991295</v>
       </c>
     </row>
     <row r="591">
@@ -9921,7 +9921,7 @@
         <v>73.400223</v>
       </c>
       <c r="C592" t="n">
-        <v>100.657898</v>
+        <v>100.657906</v>
       </c>
     </row>
     <row r="593">
@@ -9932,7 +9932,7 @@
         <v>75.564255</v>
       </c>
       <c r="C593" t="n">
-        <v>102.467278</v>
+        <v>102.46727</v>
       </c>
     </row>
     <row r="594">
@@ -9976,7 +9976,7 @@
         <v>83.748253</v>
       </c>
       <c r="C597" t="n">
-        <v>111.799789</v>
+        <v>111.799797</v>
       </c>
     </row>
     <row r="598">
@@ -9998,7 +9998,7 @@
         <v>86.128693</v>
       </c>
       <c r="C599" t="n">
-        <v>116.656509</v>
+        <v>116.656517</v>
       </c>
     </row>
     <row r="600">
@@ -10020,7 +10020,7 @@
         <v>89.256706</v>
       </c>
       <c r="C601" t="n">
-        <v>123.893982</v>
+        <v>123.89399</v>
       </c>
     </row>
     <row r="602">
@@ -10075,7 +10075,7 @@
         <v>86.42379</v>
       </c>
       <c r="C606" t="n">
-        <v>117.704041</v>
+        <v>117.704048</v>
       </c>
     </row>
     <row r="607">
@@ -10097,7 +10097,7 @@
         <v>87.663193</v>
       </c>
       <c r="C608" t="n">
-        <v>120.751396</v>
+        <v>120.751404</v>
       </c>
     </row>
     <row r="609">
@@ -10163,7 +10163,7 @@
         <v>87.466461</v>
       </c>
       <c r="C614" t="n">
-        <v>117.704041</v>
+        <v>117.704048</v>
       </c>
     </row>
     <row r="615">
@@ -10207,7 +10207,7 @@
         <v>86.836922</v>
       </c>
       <c r="C618" t="n">
-        <v>117.13266</v>
+        <v>117.132668</v>
       </c>
     </row>
     <row r="619">
@@ -10328,7 +10328,7 @@
         <v>100.185097</v>
       </c>
       <c r="C629" t="n">
-        <v>124.465355</v>
+        <v>124.465363</v>
       </c>
     </row>
     <row r="630">
@@ -10339,7 +10339,7 @@
         <v>100.185097</v>
       </c>
       <c r="C630" t="n">
-        <v>125.512886</v>
+        <v>125.512894</v>
       </c>
     </row>
     <row r="631">
@@ -10361,7 +10361,7 @@
         <v>104.267265</v>
       </c>
       <c r="C632" t="n">
-        <v>125.036736</v>
+        <v>125.036743</v>
       </c>
     </row>
     <row r="633">
@@ -10394,7 +10394,7 @@
         <v>103.72625</v>
       </c>
       <c r="C635" t="n">
-        <v>125.322433</v>
+        <v>125.322441</v>
       </c>
     </row>
     <row r="636">
@@ -10405,7 +10405,7 @@
         <v>104.218079</v>
       </c>
       <c r="C636" t="n">
-        <v>124.941498</v>
+        <v>124.941505</v>
       </c>
     </row>
     <row r="637">
@@ -10416,7 +10416,7 @@
         <v>102.250771</v>
       </c>
       <c r="C637" t="n">
-        <v>122.655998</v>
+        <v>122.655991</v>
       </c>
     </row>
     <row r="638">
@@ -10471,7 +10471,7 @@
         <v>101.168755</v>
       </c>
       <c r="C642" t="n">
-        <v>115.894676</v>
+        <v>115.894669</v>
       </c>
     </row>
     <row r="643">
@@ -10482,7 +10482,7 @@
         <v>100.480202</v>
       </c>
       <c r="C643" t="n">
-        <v>116.75174</v>
+        <v>116.751747</v>
       </c>
     </row>
     <row r="644">
@@ -10493,7 +10493,7 @@
         <v>100.922836</v>
       </c>
       <c r="C644" t="n">
-        <v>115.989914</v>
+        <v>115.989906</v>
       </c>
     </row>
     <row r="645">
@@ -10504,7 +10504,7 @@
         <v>100.332649</v>
       </c>
       <c r="C645" t="n">
-        <v>115.418526</v>
+        <v>115.418518</v>
       </c>
     </row>
     <row r="646">
@@ -10570,7 +10570,7 @@
         <v>102.349144</v>
       </c>
       <c r="C651" t="n">
-        <v>113.609169</v>
+        <v>113.609161</v>
       </c>
     </row>
     <row r="652">
@@ -10614,7 +10614,7 @@
         <v>96.496399</v>
       </c>
       <c r="C655" t="n">
-        <v>110.466576</v>
+        <v>110.466583</v>
       </c>
     </row>
     <row r="656">
@@ -10625,7 +10625,7 @@
         <v>97.047249</v>
       </c>
       <c r="C656" t="n">
-        <v>109.799973</v>
+        <v>109.799965</v>
       </c>
     </row>
     <row r="657">
@@ -10658,7 +10658,7 @@
         <v>97.971878</v>
       </c>
       <c r="C659" t="n">
-        <v>107.228767</v>
+        <v>107.22876</v>
       </c>
     </row>
     <row r="660">
@@ -10669,7 +10669,7 @@
         <v>96.594765</v>
       </c>
       <c r="C660" t="n">
-        <v>106.847847</v>
+        <v>106.847839</v>
       </c>
     </row>
     <row r="661">
@@ -10702,7 +10702,7 @@
         <v>92.463425</v>
       </c>
       <c r="C663" t="n">
-        <v>95.705963</v>
+        <v>95.705956</v>
       </c>
     </row>
     <row r="664">
@@ -10757,7 +10757,7 @@
         <v>87.859924</v>
       </c>
       <c r="C668" t="n">
-        <v>96.467796</v>
+        <v>96.467804</v>
       </c>
     </row>
     <row r="669">
@@ -10768,7 +10768,7 @@
         <v>88.627174</v>
       </c>
       <c r="C669" t="n">
-        <v>98.181938</v>
+        <v>98.181931</v>
       </c>
     </row>
     <row r="670">
@@ -10779,7 +10779,7 @@
         <v>88.587822</v>
       </c>
       <c r="C670" t="n">
-        <v>99.705605</v>
+        <v>99.705612</v>
       </c>
     </row>
     <row r="671">
@@ -10790,7 +10790,7 @@
         <v>86.502487</v>
       </c>
       <c r="C671" t="n">
-        <v>99.610382</v>
+        <v>99.610374</v>
       </c>
     </row>
     <row r="672">
@@ -10812,7 +10812,7 @@
         <v>86.187714</v>
       </c>
       <c r="C673" t="n">
-        <v>99.134232</v>
+        <v>99.134224</v>
       </c>
     </row>
     <row r="674">
@@ -10823,7 +10823,7 @@
         <v>86.384445</v>
       </c>
       <c r="C674" t="n">
-        <v>97.896248</v>
+        <v>97.89624</v>
       </c>
     </row>
     <row r="675">
@@ -10845,7 +10845,7 @@
         <v>83.0597</v>
       </c>
       <c r="C676" t="n">
-        <v>96.372559</v>
+        <v>96.372566</v>
       </c>
     </row>
     <row r="677">
@@ -10856,7 +10856,7 @@
         <v>80.659584</v>
       </c>
       <c r="C677" t="n">
-        <v>94.372734</v>
+        <v>94.372742</v>
       </c>
     </row>
     <row r="678">
@@ -10878,7 +10878,7 @@
         <v>81.938332</v>
       </c>
       <c r="C679" t="n">
-        <v>93.563293</v>
+        <v>93.563286</v>
       </c>
     </row>
     <row r="680">
@@ -10933,7 +10933,7 @@
         <v>84.692558</v>
       </c>
       <c r="C684" t="n">
-        <v>94.848885</v>
+        <v>94.848892</v>
       </c>
     </row>
     <row r="685">
@@ -10955,7 +10955,7 @@
         <v>83.453156</v>
       </c>
       <c r="C686" t="n">
-        <v>103.133881</v>
+        <v>103.133888</v>
       </c>
     </row>
     <row r="687">
@@ -10966,7 +10966,7 @@
         <v>85.57785</v>
       </c>
       <c r="C687" t="n">
-        <v>103.133881</v>
+        <v>103.133888</v>
       </c>
     </row>
     <row r="688">
@@ -10999,7 +10999,7 @@
         <v>89.453445</v>
       </c>
       <c r="C690" t="n">
-        <v>103.990952</v>
+        <v>103.990944</v>
       </c>
     </row>
     <row r="691">
@@ -11076,7 +11076,7 @@
         <v>91.401077</v>
       </c>
       <c r="C697" t="n">
-        <v>103.990952</v>
+        <v>103.990944</v>
       </c>
     </row>
     <row r="698">
@@ -11164,7 +11164,7 @@
         <v>84.161385</v>
       </c>
       <c r="C705" t="n">
-        <v>102.372047</v>
+        <v>102.37204</v>
       </c>
     </row>
     <row r="706">
@@ -11208,7 +11208,7 @@
         <v>86.974632</v>
       </c>
       <c r="C709" t="n">
-        <v>111.799789</v>
+        <v>111.799797</v>
       </c>
     </row>
     <row r="710">
@@ -11230,7 +11230,7 @@
         <v>88.627174</v>
       </c>
       <c r="C711" t="n">
-        <v>109.514275</v>
+        <v>109.514282</v>
       </c>
     </row>
     <row r="712">
@@ -11296,7 +11296,7 @@
         <v>102.447502</v>
       </c>
       <c r="C717" t="n">
-        <v>124.274902</v>
+        <v>124.274895</v>
       </c>
     </row>
     <row r="718">
@@ -11307,7 +11307,7 @@
         <v>102.890144</v>
       </c>
       <c r="C718" t="n">
-        <v>126.274734</v>
+        <v>126.274727</v>
       </c>
     </row>
     <row r="719">
@@ -11362,7 +11362,7 @@
         <v>103.234421</v>
       </c>
       <c r="C723" t="n">
-        <v>124.751053</v>
+        <v>124.751045</v>
       </c>
     </row>
     <row r="724">
@@ -11384,7 +11384,7 @@
         <v>102.98851</v>
       </c>
       <c r="C725" t="n">
-        <v>124.751053</v>
+        <v>124.751045</v>
       </c>
     </row>
     <row r="726">
@@ -11428,7 +11428,7 @@
         <v>102.250771</v>
       </c>
       <c r="C729" t="n">
-        <v>124.751053</v>
+        <v>124.751045</v>
       </c>
     </row>
     <row r="730">
@@ -11450,7 +11450,7 @@
         <v>101.513031</v>
       </c>
       <c r="C731" t="n">
-        <v>124.274902</v>
+        <v>124.274895</v>
       </c>
     </row>
     <row r="732">
@@ -11549,7 +11549,7 @@
         <v>94.529091</v>
       </c>
       <c r="C740" t="n">
-        <v>121.608459</v>
+        <v>121.608467</v>
       </c>
     </row>
     <row r="741">
@@ -11582,7 +11582,7 @@
         <v>96.870193</v>
       </c>
       <c r="C743" t="n">
-        <v>124.941498</v>
+        <v>124.941505</v>
       </c>
     </row>
     <row r="744">
@@ -11593,7 +11593,7 @@
         <v>99.742462</v>
       </c>
       <c r="C744" t="n">
-        <v>125.989037</v>
+        <v>125.989044</v>
       </c>
     </row>
     <row r="745">
@@ -11626,7 +11626,7 @@
         <v>99.004723</v>
       </c>
       <c r="C747" t="n">
-        <v>128.084091</v>
+        <v>128.084106</v>
       </c>
     </row>
     <row r="748">
@@ -11659,7 +11659,7 @@
         <v>103.627884</v>
       </c>
       <c r="C750" t="n">
-        <v>128.941147</v>
+        <v>128.941162</v>
       </c>
     </row>
     <row r="751">
@@ -11670,7 +11670,7 @@
         <v>108.054329</v>
       </c>
       <c r="C751" t="n">
-        <v>132.369446</v>
+        <v>132.369431</v>
       </c>
     </row>
     <row r="752">
@@ -11857,7 +11857,7 @@
         <v>103.480339</v>
       </c>
       <c r="C768" t="n">
-        <v>121.608459</v>
+        <v>121.608467</v>
       </c>
     </row>
     <row r="769">
@@ -11868,7 +11868,7 @@
         <v>104.070534</v>
       </c>
       <c r="C769" t="n">
-        <v>123.893982</v>
+        <v>123.89399</v>
       </c>
     </row>
     <row r="770">
@@ -11945,7 +11945,7 @@
         <v>107.955963</v>
       </c>
       <c r="C776" t="n">
-        <v>126.750885</v>
+        <v>126.750877</v>
       </c>
     </row>
     <row r="777">
@@ -11989,7 +11989,7 @@
         <v>110.857735</v>
       </c>
       <c r="C780" t="n">
-        <v>132.369446</v>
+        <v>132.369431</v>
       </c>
     </row>
     <row r="781">
@@ -12022,7 +12022,7 @@
         <v>111.644661</v>
       </c>
       <c r="C783" t="n">
-        <v>132.940826</v>
+        <v>132.940811</v>
       </c>
     </row>
     <row r="784">
@@ -12033,7 +12033,7 @@
         <v>111.447937</v>
       </c>
       <c r="C784" t="n">
-        <v>134.178787</v>
+        <v>134.178802</v>
       </c>
     </row>
     <row r="785">
@@ -12044,7 +12044,7 @@
         <v>112.333221</v>
       </c>
       <c r="C785" t="n">
-        <v>134.940628</v>
+        <v>134.940643</v>
       </c>
     </row>
     <row r="786">
@@ -12055,7 +12055,7 @@
         <v>115.087448</v>
       </c>
       <c r="C786" t="n">
-        <v>135.226334</v>
+        <v>135.226318</v>
       </c>
     </row>
     <row r="787">
@@ -12077,7 +12077,7 @@
         <v>114.595627</v>
       </c>
       <c r="C788" t="n">
-        <v>136.654785</v>
+        <v>136.65477</v>
       </c>
     </row>
     <row r="789">
@@ -12099,7 +12099,7 @@
         <v>116.366203</v>
       </c>
       <c r="C790" t="n">
-        <v>153.319992</v>
+        <v>153.319977</v>
       </c>
     </row>
     <row r="791">
@@ -12110,7 +12110,7 @@
         <v>116.218651</v>
       </c>
       <c r="C791" t="n">
-        <v>152.367691</v>
+        <v>152.367706</v>
       </c>
     </row>
     <row r="792">
@@ -12121,7 +12121,7 @@
         <v>118.82534</v>
       </c>
       <c r="C792" t="n">
-        <v>151.129715</v>
+        <v>151.1297</v>
       </c>
     </row>
     <row r="793">
@@ -12176,7 +12176,7 @@
         <v>120.54673</v>
       </c>
       <c r="C797" t="n">
-        <v>154.938904</v>
+        <v>154.938889</v>
       </c>
     </row>
     <row r="798">
@@ -12187,7 +12187,7 @@
         <v>120.497543</v>
       </c>
       <c r="C798" t="n">
-        <v>154.272293</v>
+        <v>154.272278</v>
       </c>
     </row>
     <row r="799">
@@ -12198,7 +12198,7 @@
         <v>120.349998</v>
       </c>
       <c r="C799" t="n">
-        <v>155.415054</v>
+        <v>155.415039</v>
       </c>
     </row>
     <row r="800">
@@ -12253,7 +12253,7 @@
         <v>118.25</v>
       </c>
       <c r="C804" t="n">
-        <v>155.224594</v>
+        <v>155.224579</v>
       </c>
     </row>
     <row r="805">
@@ -12264,7 +12264,7 @@
         <v>119.300003</v>
       </c>
       <c r="C805" t="n">
-        <v>159.986084</v>
+        <v>159.986069</v>
       </c>
     </row>
     <row r="806">

</xml_diff>